<commit_message>
Add "hide perfects" option
</commit_message>
<xml_diff>
--- a/AdofaiTweaks.Generator/translations.xlsx
+++ b/AdofaiTweaks.Generator/translations.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="217">
   <si>
     <t>KEY</t>
   </si>
@@ -258,6 +258,12 @@
   </si>
   <si>
     <t>Menos estable</t>
+  </si>
+  <si>
+    <t>HIDE_PERFECTS</t>
+  </si>
+  <si>
+    <t>Hide "Perfect!" judgments</t>
   </si>
   <si>
     <t>Key Limiter</t>
@@ -1205,7 +1211,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1340,6 +1346,14 @@
       </c>
       <c r="D10" t="s">
         <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1374,13 +1388,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1388,69 +1402,69 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B4" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C4" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D4" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C5" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D5" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B6" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C6" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D6" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C7" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D7" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1485,13 +1499,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1499,139 +1513,139 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C3" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D3" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B4" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C4" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D4" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B5" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C5" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D5" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B6" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C6" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D6" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B7" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C7" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D7" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B8" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C8" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D8" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B9" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C9" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D9" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B10" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C10" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D10" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B11" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C11" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D11" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B12" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C12" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D12" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -1666,13 +1680,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C2" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D2" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1680,153 +1694,153 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C3" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D3" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B4" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C4" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D4" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B5" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C5" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D5" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B6" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C6" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D6" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B7" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C7" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D7" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B8" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C8" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D8" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B9" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C9" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D9" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B10" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C10" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D10" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B11" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C11" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="D11" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B12" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C12" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="D12" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B13" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C13" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="D13" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -1861,13 +1875,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C2" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D2" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1875,41 +1889,41 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C3" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="D3" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B4" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C4" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="D4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B5" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D5" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -1944,13 +1958,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C2" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="D2" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1958,41 +1972,41 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C3" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="D3" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B4" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="D4" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B5" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C5" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="D5" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix crash when enabling JudgmentVisuals for the first time
</commit_message>
<xml_diff>
--- a/AdofaiTweaks.Generator/translations.xlsx
+++ b/AdofaiTweaks.Generator/translations.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="222">
   <si>
     <t>KEY</t>
   </si>
@@ -218,6 +218,9 @@
     <t>입력 실수 표시 시간:</t>
   </si>
   <si>
+    <t>Duración de las marcas en pantalla:</t>
+  </si>
+  <si>
     <t>ERROR_METER_TICK_SECONDS</t>
   </si>
   <si>
@@ -227,6 +230,9 @@
     <t>{0} 초</t>
   </si>
   <si>
+    <t>{0} segundo(s)</t>
+  </si>
+  <si>
     <t>ERROR_METER_SENSITIVITY</t>
   </si>
   <si>
@@ -236,6 +242,9 @@
     <t>평균 화살표 감도:</t>
   </si>
   <si>
+    <t>Sensibilidad de la flecha:</t>
+  </si>
+  <si>
     <t>ERROR_METER_MORE_STABLE</t>
   </si>
   <si>
@@ -264,6 +273,12 @@
   </si>
   <si>
     <t>Hide "Perfect!" judgments</t>
+  </si>
+  <si>
+    <t>"정확" 판정 숨기기</t>
+  </si>
+  <si>
+    <t>Esconder juicios de "!Perfecto!"</t>
   </si>
   <si>
     <t>Key Limiter</t>
@@ -1297,63 +1312,78 @@
       <c r="C6" t="s">
         <v>64</v>
       </c>
+      <c r="D6" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C7" t="s">
-        <v>67</v>
+        <v>68</v>
+      </c>
+      <c r="D7" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B8" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C8" t="s">
-        <v>70</v>
+        <v>72</v>
+      </c>
+      <c r="D8" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B9" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C9" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="D9" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B10" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C10" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="D10" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B11" t="s">
-        <v>80</v>
+        <v>83</v>
+      </c>
+      <c r="C11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D11" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1388,13 +1418,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="C2" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D2" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1402,69 +1432,69 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="C3" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D3" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="B4" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="C4" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="D4" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="B5" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="C5" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="D5" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="B6" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="C6" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="D6" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="B7" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="C7" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="D7" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -1499,13 +1529,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="C2" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="D2" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1513,139 +1543,139 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="C3" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="D3" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="B4" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="C4" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="D4" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="B5" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="C5" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="D5" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="B6" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="C6" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="D6" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="B7" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="C7" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="D7" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B8" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="C8" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="D8" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="B9" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="C9" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="D9" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="B10" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="C10" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="D10" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="B11" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="C11" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="D11" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="B12" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="C12" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="D12" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -1680,13 +1710,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="C2" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="D2" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1694,153 +1724,153 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="C3" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="D3" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="B4" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C4" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="D4" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="B5" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="C5" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="D5" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="B6" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="C6" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="D6" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="B7" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="C7" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="D7" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="B8" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="C8" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="D8" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="B9" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="C9" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="D9" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="B10" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="C10" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="D10" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="B11" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="C11" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="D11" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="B12" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="C12" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="D12" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="B13" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="C13" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="D13" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -1875,13 +1905,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="C2" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="D2" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1889,41 +1919,41 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="C3" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="D3" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="B4" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="C4" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="D4" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="B5" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="C5" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="D5" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -1958,13 +1988,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="C2" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="D2" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1972,41 +2002,41 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="C3" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="D3" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="B4" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="C4" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="D4" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="B5" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="C5" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="D5" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add key viewer option for KeyLimiter
</commit_message>
<xml_diff>
--- a/AdofaiTweaks.Generator/translations.xlsx
+++ b/AdofaiTweaks.Generator/translations.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="242">
   <si>
     <t>KEY</t>
   </si>
@@ -170,7 +170,7 @@
     <t>Judgment Visuals</t>
   </si>
   <si>
-    <t>판정 꾸미기</t>
+    <t>판정 비주얼</t>
   </si>
   <si>
     <t>Visualización de los juicios</t>
@@ -179,7 +179,7 @@
     <t>Improves the visuals of judgments.</t>
   </si>
   <si>
-    <t>보이는 판정을 더 낫게 바꿉니다.</t>
+    <t>판정을 더 정확하고 간단하게 보이도록 변경합니다.</t>
   </si>
   <si>
     <t>Mejora los visuales de los juicios.</t>
@@ -345,6 +345,66 @@
   </si>
   <si>
     <t>Cambiar teclas</t>
+  </si>
+  <si>
+    <t>SHOW_KEY_VIEWER</t>
+  </si>
+  <si>
+    <t>Show key viewer for registered keys</t>
+  </si>
+  <si>
+    <t>KEY_VIEWER_SIZE</t>
+  </si>
+  <si>
+    <t>Size:</t>
+  </si>
+  <si>
+    <t>KEY_VIEWER_X_POS</t>
+  </si>
+  <si>
+    <t>X Position:</t>
+  </si>
+  <si>
+    <t>KEY_VIEWER_Y_POS</t>
+  </si>
+  <si>
+    <t>Y Position:</t>
+  </si>
+  <si>
+    <t>PRESSED_OUTLINE_COLOR</t>
+  </si>
+  <si>
+    <t>Pressed outline color:</t>
+  </si>
+  <si>
+    <t>RELEASED_OUTLINE_COLOR</t>
+  </si>
+  <si>
+    <t>Released outline color:</t>
+  </si>
+  <si>
+    <t>PRESSED_BACKGROUND_COLOR</t>
+  </si>
+  <si>
+    <t>Pressed background color:</t>
+  </si>
+  <si>
+    <t>RELEASED_BACKGROUND_COLOR</t>
+  </si>
+  <si>
+    <t>Released background color:</t>
+  </si>
+  <si>
+    <t>PRESSED_TEXT_COLOR</t>
+  </si>
+  <si>
+    <t>Pressed text color:</t>
+  </si>
+  <si>
+    <t>RELEASED_TEXT_COLOR</t>
+  </si>
+  <si>
+    <t>Released text color:</t>
   </si>
   <si>
     <t>Miscellaneous</t>
@@ -1393,7 +1453,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1495,6 +1555,86 @@
       </c>
       <c r="D7" t="s">
         <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>110</v>
+      </c>
+      <c r="B9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>116</v>
+      </c>
+      <c r="B12" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>118</v>
+      </c>
+      <c r="B13" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>120</v>
+      </c>
+      <c r="B14" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>122</v>
+      </c>
+      <c r="B15" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>124</v>
+      </c>
+      <c r="B16" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>126</v>
+      </c>
+      <c r="B17" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1529,13 +1669,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>108</v>
+        <v>128</v>
       </c>
       <c r="C2" t="s">
-        <v>109</v>
+        <v>129</v>
       </c>
       <c r="D2" t="s">
-        <v>110</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1543,139 +1683,139 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>111</v>
+        <v>131</v>
       </c>
       <c r="C3" t="s">
-        <v>112</v>
+        <v>132</v>
       </c>
       <c r="D3" t="s">
-        <v>113</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>114</v>
+        <v>134</v>
       </c>
       <c r="B4" t="s">
-        <v>115</v>
+        <v>135</v>
       </c>
       <c r="C4" t="s">
-        <v>116</v>
+        <v>136</v>
       </c>
       <c r="D4" t="s">
-        <v>117</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>118</v>
+        <v>138</v>
       </c>
       <c r="B5" t="s">
-        <v>119</v>
+        <v>139</v>
       </c>
       <c r="C5" t="s">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="D5" t="s">
-        <v>121</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>122</v>
+        <v>142</v>
       </c>
       <c r="B6" t="s">
-        <v>123</v>
+        <v>143</v>
       </c>
       <c r="C6" t="s">
-        <v>124</v>
+        <v>144</v>
       </c>
       <c r="D6" t="s">
-        <v>125</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>126</v>
+        <v>146</v>
       </c>
       <c r="B7" t="s">
-        <v>127</v>
+        <v>147</v>
       </c>
       <c r="C7" t="s">
-        <v>128</v>
+        <v>148</v>
       </c>
       <c r="D7" t="s">
-        <v>129</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="B8" t="s">
-        <v>131</v>
+        <v>151</v>
       </c>
       <c r="C8" t="s">
-        <v>132</v>
+        <v>152</v>
       </c>
       <c r="D8" t="s">
-        <v>133</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>134</v>
+        <v>154</v>
       </c>
       <c r="B9" t="s">
-        <v>135</v>
+        <v>155</v>
       </c>
       <c r="C9" t="s">
-        <v>136</v>
+        <v>156</v>
       </c>
       <c r="D9" t="s">
-        <v>137</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>138</v>
+        <v>158</v>
       </c>
       <c r="B10" t="s">
-        <v>139</v>
+        <v>159</v>
       </c>
       <c r="C10" t="s">
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="D10" t="s">
-        <v>141</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>142</v>
+        <v>162</v>
       </c>
       <c r="B11" t="s">
-        <v>143</v>
+        <v>163</v>
       </c>
       <c r="C11" t="s">
-        <v>144</v>
+        <v>164</v>
       </c>
       <c r="D11" t="s">
-        <v>145</v>
+        <v>165</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>146</v>
+        <v>166</v>
       </c>
       <c r="B12" t="s">
-        <v>147</v>
+        <v>167</v>
       </c>
       <c r="C12" t="s">
-        <v>148</v>
+        <v>168</v>
       </c>
       <c r="D12" t="s">
-        <v>149</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -1710,13 +1850,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>150</v>
+        <v>170</v>
       </c>
       <c r="C2" t="s">
-        <v>151</v>
+        <v>171</v>
       </c>
       <c r="D2" t="s">
-        <v>152</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1724,153 +1864,153 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>153</v>
+        <v>173</v>
       </c>
       <c r="C3" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="D3" t="s">
-        <v>155</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>156</v>
+        <v>176</v>
       </c>
       <c r="B4" t="s">
-        <v>157</v>
+        <v>177</v>
       </c>
       <c r="C4" t="s">
-        <v>158</v>
+        <v>178</v>
       </c>
       <c r="D4" t="s">
-        <v>159</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
       <c r="B5" t="s">
-        <v>161</v>
+        <v>181</v>
       </c>
       <c r="C5" t="s">
-        <v>162</v>
+        <v>182</v>
       </c>
       <c r="D5" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>164</v>
+        <v>184</v>
       </c>
       <c r="B6" t="s">
-        <v>165</v>
+        <v>185</v>
       </c>
       <c r="C6" t="s">
-        <v>166</v>
+        <v>186</v>
       </c>
       <c r="D6" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>168</v>
+        <v>188</v>
       </c>
       <c r="B7" t="s">
-        <v>169</v>
+        <v>189</v>
       </c>
       <c r="C7" t="s">
-        <v>170</v>
+        <v>190</v>
       </c>
       <c r="D7" t="s">
-        <v>171</v>
+        <v>191</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>172</v>
+        <v>192</v>
       </c>
       <c r="B8" t="s">
-        <v>173</v>
+        <v>193</v>
       </c>
       <c r="C8" t="s">
-        <v>174</v>
+        <v>194</v>
       </c>
       <c r="D8" t="s">
-        <v>175</v>
+        <v>195</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>176</v>
+        <v>196</v>
       </c>
       <c r="B9" t="s">
-        <v>177</v>
+        <v>197</v>
       </c>
       <c r="C9" t="s">
-        <v>178</v>
+        <v>198</v>
       </c>
       <c r="D9" t="s">
-        <v>179</v>
+        <v>199</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="B10" t="s">
-        <v>181</v>
+        <v>201</v>
       </c>
       <c r="C10" t="s">
-        <v>182</v>
+        <v>202</v>
       </c>
       <c r="D10" t="s">
-        <v>183</v>
+        <v>203</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>184</v>
+        <v>204</v>
       </c>
       <c r="B11" t="s">
-        <v>185</v>
+        <v>205</v>
       </c>
       <c r="C11" t="s">
-        <v>186</v>
+        <v>206</v>
       </c>
       <c r="D11" t="s">
-        <v>187</v>
+        <v>207</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>188</v>
+        <v>208</v>
       </c>
       <c r="B12" t="s">
-        <v>189</v>
+        <v>209</v>
       </c>
       <c r="C12" t="s">
-        <v>190</v>
+        <v>210</v>
       </c>
       <c r="D12" t="s">
-        <v>191</v>
+        <v>211</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>192</v>
+        <v>212</v>
       </c>
       <c r="B13" t="s">
-        <v>193</v>
+        <v>213</v>
       </c>
       <c r="C13" t="s">
-        <v>194</v>
+        <v>214</v>
       </c>
       <c r="D13" t="s">
-        <v>195</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -1905,13 +2045,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>196</v>
+        <v>216</v>
       </c>
       <c r="C2" t="s">
-        <v>197</v>
+        <v>217</v>
       </c>
       <c r="D2" t="s">
-        <v>198</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1919,41 +2059,41 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>199</v>
+        <v>219</v>
       </c>
       <c r="C3" t="s">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="D3" t="s">
-        <v>201</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>156</v>
+        <v>176</v>
       </c>
       <c r="B4" t="s">
-        <v>202</v>
+        <v>222</v>
       </c>
       <c r="C4" t="s">
-        <v>203</v>
+        <v>223</v>
       </c>
       <c r="D4" t="s">
-        <v>204</v>
+        <v>224</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
       <c r="B5" t="s">
-        <v>205</v>
+        <v>225</v>
       </c>
       <c r="C5" t="s">
-        <v>206</v>
+        <v>226</v>
       </c>
       <c r="D5" t="s">
-        <v>207</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -1988,13 +2128,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>208</v>
+        <v>228</v>
       </c>
       <c r="C2" t="s">
-        <v>209</v>
+        <v>229</v>
       </c>
       <c r="D2" t="s">
-        <v>210</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2002,41 +2142,41 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>211</v>
+        <v>231</v>
       </c>
       <c r="C3" t="s">
-        <v>212</v>
+        <v>232</v>
       </c>
       <c r="D3" t="s">
-        <v>213</v>
+        <v>233</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>214</v>
+        <v>234</v>
       </c>
       <c r="B4" t="s">
-        <v>215</v>
+        <v>235</v>
       </c>
       <c r="C4" t="s">
-        <v>216</v>
+        <v>236</v>
       </c>
       <c r="D4" t="s">
-        <v>217</v>
+        <v>237</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>218</v>
+        <v>238</v>
       </c>
       <c r="B5" t="s">
-        <v>219</v>
+        <v>239</v>
       </c>
       <c r="C5" t="s">
-        <v>220</v>
+        <v>240</v>
       </c>
       <c r="D5" t="s">
-        <v>221</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Move repeated GUILayout logic to separate file
</commit_message>
<xml_diff>
--- a/AdofaiTweaks.Generator/translations.xlsx
+++ b/AdofaiTweaks.Generator/translations.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="227">
   <si>
     <t>KEY</t>
   </si>
@@ -353,6 +353,9 @@
     <t>Show key viewer for registered keys</t>
   </si>
   <si>
+    <t>등록된 키들의 키뷰어 보이기</t>
+  </si>
+  <si>
     <t>KEY_VIEWER_SIZE</t>
   </si>
   <si>
@@ -365,48 +368,72 @@
     <t>X Position:</t>
   </si>
   <si>
+    <t>가로 위치:</t>
+  </si>
+  <si>
     <t>KEY_VIEWER_Y_POS</t>
   </si>
   <si>
     <t>Y Position:</t>
   </si>
   <si>
+    <t>세로 위치:</t>
+  </si>
+  <si>
     <t>PRESSED_OUTLINE_COLOR</t>
   </si>
   <si>
     <t>Pressed outline color:</t>
   </si>
   <si>
+    <t>누른 키의 테두리 색상:</t>
+  </si>
+  <si>
     <t>RELEASED_OUTLINE_COLOR</t>
   </si>
   <si>
     <t>Released outline color:</t>
   </si>
   <si>
+    <t>누르지 않은 키의 테두리 색상:</t>
+  </si>
+  <si>
     <t>PRESSED_BACKGROUND_COLOR</t>
   </si>
   <si>
     <t>Pressed background color:</t>
   </si>
   <si>
+    <t>누른 키의 배경 색상:</t>
+  </si>
+  <si>
     <t>RELEASED_BACKGROUND_COLOR</t>
   </si>
   <si>
     <t>Released background color:</t>
   </si>
   <si>
+    <t>누르지 않은 키의 배경 색상:</t>
+  </si>
+  <si>
     <t>PRESSED_TEXT_COLOR</t>
   </si>
   <si>
     <t>Pressed text color:</t>
   </si>
   <si>
+    <t>누른 키의 텍스트 색상:</t>
+  </si>
+  <si>
     <t>RELEASED_TEXT_COLOR</t>
   </si>
   <si>
     <t>Released text color:</t>
   </si>
   <si>
+    <t>누르지 않은 키의 텍스트 색상:</t>
+  </si>
+  <si>
     <t>Miscellaneous</t>
   </si>
   <si>
@@ -575,100 +602,28 @@
     <t>Planeta 2:</t>
   </si>
   <si>
-    <t>BODY_R</t>
-  </si>
-  <si>
-    <t>Body R:</t>
-  </si>
-  <si>
-    <t>행성 R:</t>
-  </si>
-  <si>
-    <t>Cuerpo R:</t>
-  </si>
-  <si>
-    <t>BODY_G</t>
-  </si>
-  <si>
-    <t>Body G:</t>
-  </si>
-  <si>
-    <t>행성 G:</t>
-  </si>
-  <si>
-    <t>Cuerpo G:</t>
-  </si>
-  <si>
-    <t>BODY_B</t>
-  </si>
-  <si>
-    <t>Body B:</t>
-  </si>
-  <si>
-    <t>행성 B:</t>
-  </si>
-  <si>
-    <t>Cuerpo B:</t>
-  </si>
-  <si>
-    <t>TAIL_R</t>
-  </si>
-  <si>
-    <t>Tail R:</t>
-  </si>
-  <si>
-    <t>꼬리 파티클 R:</t>
-  </si>
-  <si>
-    <t>Cola R:</t>
-  </si>
-  <si>
-    <t>TAIL_G</t>
-  </si>
-  <si>
-    <t>Tail G:</t>
-  </si>
-  <si>
-    <t>꼬리 파티클 G:</t>
-  </si>
-  <si>
-    <t>Cola G:</t>
-  </si>
-  <si>
-    <t>TAIL_B</t>
-  </si>
-  <si>
-    <t>Tail B:</t>
-  </si>
-  <si>
-    <t>꼬리 파티클 B:</t>
-  </si>
-  <si>
-    <t>Cola B:</t>
-  </si>
-  <si>
-    <t>BODY_HEX</t>
-  </si>
-  <si>
-    <t>Body Hex:</t>
-  </si>
-  <si>
-    <t>행성 Hex:</t>
-  </si>
-  <si>
-    <t>Cuerpo Hex:</t>
-  </si>
-  <si>
-    <t>TAIL_HEX</t>
-  </si>
-  <si>
-    <t>Tail Hex:</t>
-  </si>
-  <si>
-    <t>꼬리 파티클 Hex:</t>
-  </si>
-  <si>
-    <t>Cola Hex:</t>
+    <t>BODY</t>
+  </si>
+  <si>
+    <t>Body:</t>
+  </si>
+  <si>
+    <t>행성:</t>
+  </si>
+  <si>
+    <t>Cuerpo:</t>
+  </si>
+  <si>
+    <t>TAIL</t>
+  </si>
+  <si>
+    <t>Tail:</t>
+  </si>
+  <si>
+    <t>꼬리 파티클:</t>
+  </si>
+  <si>
+    <t>Cola:</t>
   </si>
   <si>
     <t>Planet Opacity</t>
@@ -1564,77 +1519,107 @@
       <c r="B8" t="s">
         <v>109</v>
       </c>
+      <c r="C8" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B9" t="s">
-        <v>111</v>
+        <v>112</v>
+      </c>
+      <c r="C9" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B10" t="s">
-        <v>113</v>
+        <v>114</v>
+      </c>
+      <c r="C10" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B11" t="s">
-        <v>115</v>
+        <v>117</v>
+      </c>
+      <c r="C11" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B12" t="s">
-        <v>117</v>
+        <v>120</v>
+      </c>
+      <c r="C12" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="B13" t="s">
-        <v>119</v>
+        <v>123</v>
+      </c>
+      <c r="C13" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B14" t="s">
-        <v>121</v>
+        <v>126</v>
+      </c>
+      <c r="C14" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="B15" t="s">
-        <v>123</v>
+        <v>129</v>
+      </c>
+      <c r="C15" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="B16" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
+        <v>132</v>
+      </c>
+      <c r="C16" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="B17" t="s">
-        <v>127</v>
+        <v>135</v>
+      </c>
+      <c r="C17" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -1669,13 +1654,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="C2" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="D2" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1683,139 +1668,139 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="C3" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="D3" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="B4" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="C4" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="D4" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="B5" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
       <c r="C5" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
       <c r="D5" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="B6" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
       <c r="C6" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="D6" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="B7" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="C7" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="D7" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="B8" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
       <c r="C8" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
       <c r="D8" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="B9" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="C9" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="D9" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="B10" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="C10" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
       <c r="D10" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>162</v>
+        <v>171</v>
       </c>
       <c r="B11" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
       <c r="C11" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="D11" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>166</v>
+        <v>175</v>
       </c>
       <c r="B12" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="C12" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="D12" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -1825,7 +1810,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1850,13 +1835,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="C2" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="D2" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1864,153 +1849,69 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="C3" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="D3" t="s">
-        <v>175</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="B4" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="C4" t="s">
-        <v>178</v>
+        <v>187</v>
       </c>
       <c r="D4" t="s">
-        <v>179</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>180</v>
+        <v>189</v>
       </c>
       <c r="B5" t="s">
-        <v>181</v>
+        <v>190</v>
       </c>
       <c r="C5" t="s">
-        <v>182</v>
+        <v>191</v>
       </c>
       <c r="D5" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>184</v>
+        <v>193</v>
       </c>
       <c r="B6" t="s">
-        <v>185</v>
+        <v>194</v>
       </c>
       <c r="C6" t="s">
-        <v>186</v>
+        <v>195</v>
       </c>
       <c r="D6" t="s">
-        <v>187</v>
+        <v>196</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>188</v>
+        <v>197</v>
       </c>
       <c r="B7" t="s">
-        <v>189</v>
+        <v>198</v>
       </c>
       <c r="C7" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D7" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>192</v>
-      </c>
-      <c r="B8" t="s">
-        <v>193</v>
-      </c>
-      <c r="C8" t="s">
-        <v>194</v>
-      </c>
-      <c r="D8" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
-        <v>196</v>
-      </c>
-      <c r="B9" t="s">
-        <v>197</v>
-      </c>
-      <c r="C9" t="s">
-        <v>198</v>
-      </c>
-      <c r="D9" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
         <v>200</v>
-      </c>
-      <c r="B10" t="s">
-        <v>201</v>
-      </c>
-      <c r="C10" t="s">
-        <v>202</v>
-      </c>
-      <c r="D10" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
-        <v>204</v>
-      </c>
-      <c r="B11" t="s">
-        <v>205</v>
-      </c>
-      <c r="C11" t="s">
-        <v>206</v>
-      </c>
-      <c r="D11" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
-        <v>208</v>
-      </c>
-      <c r="B12" t="s">
-        <v>209</v>
-      </c>
-      <c r="C12" t="s">
-        <v>210</v>
-      </c>
-      <c r="D12" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
-        <v>212</v>
-      </c>
-      <c r="B13" t="s">
-        <v>213</v>
-      </c>
-      <c r="C13" t="s">
-        <v>214</v>
-      </c>
-      <c r="D13" t="s">
-        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -2045,13 +1946,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
       <c r="C2" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
       <c r="D2" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2059,41 +1960,41 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
       <c r="C3" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="D3" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="B4" t="s">
-        <v>222</v>
+        <v>207</v>
       </c>
       <c r="C4" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="D4" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>180</v>
+        <v>189</v>
       </c>
       <c r="B5" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="C5" t="s">
-        <v>226</v>
+        <v>211</v>
       </c>
       <c r="D5" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -2128,13 +2029,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>228</v>
+        <v>213</v>
       </c>
       <c r="C2" t="s">
-        <v>229</v>
+        <v>214</v>
       </c>
       <c r="D2" t="s">
-        <v>230</v>
+        <v>215</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2142,41 +2043,41 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>231</v>
+        <v>216</v>
       </c>
       <c r="C3" t="s">
-        <v>232</v>
+        <v>217</v>
       </c>
       <c r="D3" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="B4" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="C4" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
       <c r="D4" t="s">
-        <v>237</v>
+        <v>222</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>238</v>
+        <v>223</v>
       </c>
       <c r="B5" t="s">
-        <v>239</v>
+        <v>224</v>
       </c>
       <c r="C5" t="s">
-        <v>240</v>
+        <v>225</v>
       </c>
       <c r="D5" t="s">
-        <v>241</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add key press animations
</commit_message>
<xml_diff>
--- a/AdofaiTweaks.Generator/translations.xlsx
+++ b/AdofaiTweaks.Generator/translations.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="230">
   <si>
     <t>KEY</t>
   </si>
@@ -356,6 +356,15 @@
     <t>등록된 키들의 키뷰어 보이기</t>
   </si>
   <si>
+    <t>ANIMATE_KEYS</t>
+  </si>
+  <si>
+    <t>Animate key presses</t>
+  </si>
+  <si>
+    <t>키를 눌렀을 때 효과 보이기</t>
+  </si>
+  <si>
     <t>KEY_VIEWER_SIZE</t>
   </si>
   <si>
@@ -395,7 +404,7 @@
     <t>Released outline color:</t>
   </si>
   <si>
-    <t>누르지 않은 키의 테두리 색상:</t>
+    <t>뗀 키의 테두리 색상:</t>
   </si>
   <si>
     <t>PRESSED_BACKGROUND_COLOR</t>
@@ -413,7 +422,7 @@
     <t>Released background color:</t>
   </si>
   <si>
-    <t>누르지 않은 키의 배경 색상:</t>
+    <t>뗀 키의 배경 색상:</t>
   </si>
   <si>
     <t>PRESSED_TEXT_COLOR</t>
@@ -431,7 +440,7 @@
     <t>Released text color:</t>
   </si>
   <si>
-    <t>누르지 않은 키의 텍스트 색상:</t>
+    <t>뗀 키의 텍스트 색상:</t>
   </si>
   <si>
     <t>Miscellaneous</t>
@@ -1408,7 +1417,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1531,18 +1540,18 @@
         <v>112</v>
       </c>
       <c r="C9" t="s">
-        <v>60</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B10" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C10" t="s">
-        <v>115</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1620,6 +1629,17 @@
       </c>
       <c r="C17" t="s">
         <v>136</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>137</v>
+      </c>
+      <c r="B18" t="s">
+        <v>138</v>
+      </c>
+      <c r="C18" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -1654,13 +1674,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D2" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1668,139 +1688,139 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="C3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="D3" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B4" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C4" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="D4" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B5" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C5" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D5" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B6" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="C6" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="D6" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B7" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="C7" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="D7" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="B8" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C8" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="D8" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B9" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="C9" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="D9" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="B10" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="C10" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="D10" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="B11" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C11" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="D11" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="B12" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C12" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="D12" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -1835,13 +1855,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="C2" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="D2" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1849,69 +1869,69 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C3" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="D3" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="B4" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="C4" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="D4" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="B5" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="C5" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="D5" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="B6" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="C6" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="D6" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="B7" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="C7" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="D7" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -1946,13 +1966,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="C2" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="D2" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1960,41 +1980,41 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C3" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="D3" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="B4" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="C4" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="D4" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="B5" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="C5" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="D5" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -2029,13 +2049,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="C2" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="D2" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2043,41 +2063,41 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="C3" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="D3" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="B4" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="C4" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="D4" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="B5" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="C5" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="D5" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Viewer show only during gameplay option + small fixes
</commit_message>
<xml_diff>
--- a/AdofaiTweaks.Generator/translations.xlsx
+++ b/AdofaiTweaks.Generator/translations.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="245">
   <si>
     <t>KEY</t>
   </si>
@@ -356,6 +356,21 @@
     <t>등록된 키들의 키뷰어 보이기</t>
   </si>
   <si>
+    <t>Mostrar teclas en pantalla</t>
+  </si>
+  <si>
+    <t>VIEWER_ONLY_GAMEPLAY</t>
+  </si>
+  <si>
+    <t>Only show during gameplay</t>
+  </si>
+  <si>
+    <t>레벨 플레이중에만 보이기</t>
+  </si>
+  <si>
+    <t>Sólo mostrar mientras juegas</t>
+  </si>
+  <si>
     <t>ANIMATE_KEYS</t>
   </si>
   <si>
@@ -365,12 +380,18 @@
     <t>키를 눌렀을 때 효과 보이기</t>
   </si>
   <si>
+    <t>Animar pulsaciones de teclas</t>
+  </si>
+  <si>
     <t>KEY_VIEWER_SIZE</t>
   </si>
   <si>
     <t>Size:</t>
   </si>
   <si>
+    <t>Tamaño:</t>
+  </si>
+  <si>
     <t>KEY_VIEWER_X_POS</t>
   </si>
   <si>
@@ -380,6 +401,9 @@
     <t>가로 위치:</t>
   </si>
   <si>
+    <t>Posición X:</t>
+  </si>
+  <si>
     <t>KEY_VIEWER_Y_POS</t>
   </si>
   <si>
@@ -389,6 +413,9 @@
     <t>세로 위치:</t>
   </si>
   <si>
+    <t>Posición Y:</t>
+  </si>
+  <si>
     <t>PRESSED_OUTLINE_COLOR</t>
   </si>
   <si>
@@ -398,6 +425,9 @@
     <t>누른 키의 테두리 색상:</t>
   </si>
   <si>
+    <t>Color del contorno de las teclas pulsadas:</t>
+  </si>
+  <si>
     <t>RELEASED_OUTLINE_COLOR</t>
   </si>
   <si>
@@ -407,6 +437,9 @@
     <t>뗀 키의 테두리 색상:</t>
   </si>
   <si>
+    <t>Color del contorno de las teclas sin pulsar:</t>
+  </si>
+  <si>
     <t>PRESSED_BACKGROUND_COLOR</t>
   </si>
   <si>
@@ -416,6 +449,9 @@
     <t>누른 키의 배경 색상:</t>
   </si>
   <si>
+    <t>Color del fondo de las teclas pulsadas:</t>
+  </si>
+  <si>
     <t>RELEASED_BACKGROUND_COLOR</t>
   </si>
   <si>
@@ -425,6 +461,9 @@
     <t>뗀 키의 배경 색상:</t>
   </si>
   <si>
+    <t>Color del fondo de las teclas sin pulsar:</t>
+  </si>
+  <si>
     <t>PRESSED_TEXT_COLOR</t>
   </si>
   <si>
@@ -434,6 +473,9 @@
     <t>누른 키의 텍스트 색상:</t>
   </si>
   <si>
+    <t>Color del texto de las teclas pulsadas:</t>
+  </si>
+  <si>
     <t>RELEASED_TEXT_COLOR</t>
   </si>
   <si>
@@ -441,6 +483,9 @@
   </si>
   <si>
     <t>뗀 키의 텍스트 색상:</t>
+  </si>
+  <si>
+    <t>Color del texto de las teclas sin pulsar:</t>
   </si>
   <si>
     <t>Miscellaneous</t>
@@ -1417,7 +1462,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1531,115 +1576,162 @@
       <c r="C8" t="s">
         <v>110</v>
       </c>
+      <c r="D8" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B9" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C9" t="s">
-        <v>113</v>
+        <v>114</v>
+      </c>
+      <c r="D9" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B10" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C10" t="s">
-        <v>60</v>
+        <v>118</v>
+      </c>
+      <c r="D10" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="B11" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C11" t="s">
-        <v>118</v>
+        <v>60</v>
+      </c>
+      <c r="D11" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="B12" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="C12" t="s">
-        <v>121</v>
+        <v>125</v>
+      </c>
+      <c r="D12" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B13" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="C13" t="s">
-        <v>124</v>
+        <v>129</v>
+      </c>
+      <c r="D13" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="B14" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="C14" t="s">
-        <v>127</v>
+        <v>133</v>
+      </c>
+      <c r="D14" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="B15" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="C15" t="s">
-        <v>130</v>
+        <v>137</v>
+      </c>
+      <c r="D15" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B16" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="C16" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>141</v>
+      </c>
+      <c r="D16" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="B17" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="C17" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>145</v>
+      </c>
+      <c r="D17" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="B18" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="C18" t="s">
-        <v>139</v>
+        <v>149</v>
+      </c>
+      <c r="D18" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>151</v>
+      </c>
+      <c r="B19" t="s">
+        <v>152</v>
+      </c>
+      <c r="C19" t="s">
+        <v>153</v>
+      </c>
+      <c r="D19" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -1674,13 +1766,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>140</v>
+        <v>155</v>
       </c>
       <c r="C2" t="s">
-        <v>141</v>
+        <v>156</v>
       </c>
       <c r="D2" t="s">
-        <v>142</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1688,139 +1780,139 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>143</v>
+        <v>158</v>
       </c>
       <c r="C3" t="s">
-        <v>144</v>
+        <v>159</v>
       </c>
       <c r="D3" t="s">
-        <v>145</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>146</v>
+        <v>161</v>
       </c>
       <c r="B4" t="s">
-        <v>147</v>
+        <v>162</v>
       </c>
       <c r="C4" t="s">
-        <v>148</v>
+        <v>163</v>
       </c>
       <c r="D4" t="s">
-        <v>149</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="B5" t="s">
-        <v>151</v>
+        <v>166</v>
       </c>
       <c r="C5" t="s">
-        <v>152</v>
+        <v>167</v>
       </c>
       <c r="D5" t="s">
-        <v>153</v>
+        <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>154</v>
+        <v>169</v>
       </c>
       <c r="B6" t="s">
-        <v>155</v>
+        <v>170</v>
       </c>
       <c r="C6" t="s">
-        <v>156</v>
+        <v>171</v>
       </c>
       <c r="D6" t="s">
-        <v>157</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>158</v>
+        <v>173</v>
       </c>
       <c r="B7" t="s">
-        <v>159</v>
+        <v>174</v>
       </c>
       <c r="C7" t="s">
-        <v>160</v>
+        <v>175</v>
       </c>
       <c r="D7" t="s">
-        <v>161</v>
+        <v>176</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>162</v>
+        <v>177</v>
       </c>
       <c r="B8" t="s">
-        <v>163</v>
+        <v>178</v>
       </c>
       <c r="C8" t="s">
-        <v>164</v>
+        <v>179</v>
       </c>
       <c r="D8" t="s">
-        <v>165</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>166</v>
+        <v>181</v>
       </c>
       <c r="B9" t="s">
-        <v>167</v>
+        <v>182</v>
       </c>
       <c r="C9" t="s">
-        <v>168</v>
+        <v>183</v>
       </c>
       <c r="D9" t="s">
-        <v>169</v>
+        <v>184</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>170</v>
+        <v>185</v>
       </c>
       <c r="B10" t="s">
-        <v>171</v>
+        <v>186</v>
       </c>
       <c r="C10" t="s">
-        <v>172</v>
+        <v>187</v>
       </c>
       <c r="D10" t="s">
-        <v>173</v>
+        <v>188</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>174</v>
+        <v>189</v>
       </c>
       <c r="B11" t="s">
-        <v>175</v>
+        <v>190</v>
       </c>
       <c r="C11" t="s">
-        <v>176</v>
+        <v>191</v>
       </c>
       <c r="D11" t="s">
-        <v>177</v>
+        <v>192</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>178</v>
+        <v>193</v>
       </c>
       <c r="B12" t="s">
-        <v>179</v>
+        <v>194</v>
       </c>
       <c r="C12" t="s">
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="D12" t="s">
-        <v>181</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -1855,13 +1947,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>182</v>
+        <v>197</v>
       </c>
       <c r="C2" t="s">
-        <v>183</v>
+        <v>198</v>
       </c>
       <c r="D2" t="s">
-        <v>184</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1869,69 +1961,69 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>185</v>
+        <v>200</v>
       </c>
       <c r="C3" t="s">
-        <v>186</v>
+        <v>201</v>
       </c>
       <c r="D3" t="s">
-        <v>187</v>
+        <v>202</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>188</v>
+        <v>203</v>
       </c>
       <c r="B4" t="s">
-        <v>189</v>
+        <v>204</v>
       </c>
       <c r="C4" t="s">
-        <v>190</v>
+        <v>205</v>
       </c>
       <c r="D4" t="s">
-        <v>191</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>192</v>
+        <v>207</v>
       </c>
       <c r="B5" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
       <c r="C5" t="s">
-        <v>194</v>
+        <v>209</v>
       </c>
       <c r="D5" t="s">
-        <v>195</v>
+        <v>210</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>196</v>
+        <v>211</v>
       </c>
       <c r="B6" t="s">
-        <v>197</v>
+        <v>212</v>
       </c>
       <c r="C6" t="s">
-        <v>198</v>
+        <v>213</v>
       </c>
       <c r="D6" t="s">
-        <v>199</v>
+        <v>214</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>200</v>
+        <v>215</v>
       </c>
       <c r="B7" t="s">
-        <v>201</v>
+        <v>216</v>
       </c>
       <c r="C7" t="s">
-        <v>202</v>
+        <v>217</v>
       </c>
       <c r="D7" t="s">
-        <v>203</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -1966,13 +2058,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>204</v>
+        <v>219</v>
       </c>
       <c r="C2" t="s">
-        <v>205</v>
+        <v>220</v>
       </c>
       <c r="D2" t="s">
-        <v>206</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1980,41 +2072,41 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>207</v>
+        <v>222</v>
       </c>
       <c r="C3" t="s">
-        <v>208</v>
+        <v>223</v>
       </c>
       <c r="D3" t="s">
-        <v>209</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>188</v>
+        <v>203</v>
       </c>
       <c r="B4" t="s">
-        <v>210</v>
+        <v>225</v>
       </c>
       <c r="C4" t="s">
-        <v>211</v>
+        <v>226</v>
       </c>
       <c r="D4" t="s">
-        <v>212</v>
+        <v>227</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>192</v>
+        <v>207</v>
       </c>
       <c r="B5" t="s">
-        <v>213</v>
+        <v>228</v>
       </c>
       <c r="C5" t="s">
-        <v>214</v>
+        <v>229</v>
       </c>
       <c r="D5" t="s">
-        <v>215</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -2049,13 +2141,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>216</v>
+        <v>231</v>
       </c>
       <c r="C2" t="s">
-        <v>217</v>
+        <v>232</v>
       </c>
       <c r="D2" t="s">
-        <v>218</v>
+        <v>233</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2063,41 +2155,41 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>219</v>
+        <v>234</v>
       </c>
       <c r="C3" t="s">
-        <v>220</v>
+        <v>235</v>
       </c>
       <c r="D3" t="s">
-        <v>221</v>
+        <v>236</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>222</v>
+        <v>237</v>
       </c>
       <c r="B4" t="s">
-        <v>223</v>
+        <v>238</v>
       </c>
       <c r="C4" t="s">
-        <v>224</v>
+        <v>239</v>
       </c>
       <c r="D4" t="s">
-        <v>225</v>
+        <v>240</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>226</v>
+        <v>241</v>
       </c>
       <c r="B5" t="s">
-        <v>227</v>
+        <v>242</v>
       </c>
       <c r="C5" t="s">
-        <v>228</v>
+        <v>243</v>
       </c>
       <c r="D5" t="s">
-        <v>229</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Separate key viewer and limiter
</commit_message>
<xml_diff>
--- a/AdofaiTweaks.Generator/translations.xlsx
+++ b/AdofaiTweaks.Generator/translations.xlsx
@@ -11,17 +11,18 @@
     <sheet name="HideUiElements" sheetId="2" r:id="rId2"/>
     <sheet name="JudgmentVisuals" sheetId="3" r:id="rId3"/>
     <sheet name="KeyLimiter" sheetId="4" r:id="rId4"/>
-    <sheet name="Miscellaneous" sheetId="5" r:id="rId5"/>
-    <sheet name="PlanetColor" sheetId="6" r:id="rId6"/>
-    <sheet name="PlanetOpacity" sheetId="7" r:id="rId7"/>
-    <sheet name="RestrictJudgments" sheetId="8" r:id="rId8"/>
+    <sheet name="KeyViewer" sheetId="5" r:id="rId5"/>
+    <sheet name="Miscellaneous" sheetId="6" r:id="rId6"/>
+    <sheet name="PlanetColor" sheetId="7" r:id="rId7"/>
+    <sheet name="PlanetOpacity" sheetId="8" r:id="rId8"/>
+    <sheet name="RestrictJudgments" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="247">
   <si>
     <t>KEY</t>
   </si>
@@ -347,16 +348,22 @@
     <t>Cambiar teclas</t>
   </si>
   <si>
-    <t>SHOW_KEY_VIEWER</t>
-  </si>
-  <si>
-    <t>Show key viewer for registered keys</t>
+    <t>Key Viewer</t>
+  </si>
+  <si>
+    <t>키뷰어</t>
+  </si>
+  <si>
+    <t>Teclas en pantella</t>
+  </si>
+  <si>
+    <t>Shows a key viewer for registered keys</t>
   </si>
   <si>
     <t>등록된 키들의 키뷰어 보이기</t>
   </si>
   <si>
-    <t>Mostrar teclas en pantalla</t>
+    <t>Muestra teclas en pantalla</t>
   </si>
   <si>
     <t>VIEWER_ONLY_GAMEPLAY</t>
@@ -1462,7 +1469,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1566,180 +1573,277 @@
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>108</v>
-      </c>
-      <c r="B8" t="s">
-        <v>109</v>
-      </c>
-      <c r="C8" t="s">
-        <v>110</v>
-      </c>
-      <c r="D8" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
-        <v>112</v>
-      </c>
-      <c r="B9" t="s">
-        <v>113</v>
-      </c>
-      <c r="C9" t="s">
-        <v>114</v>
-      </c>
-      <c r="D9" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>116</v>
-      </c>
-      <c r="B10" t="s">
-        <v>117</v>
-      </c>
-      <c r="C10" t="s">
-        <v>118</v>
-      </c>
-      <c r="D10" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
-        <v>120</v>
-      </c>
-      <c r="B11" t="s">
-        <v>121</v>
-      </c>
-      <c r="C11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D11" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
-        <v>123</v>
-      </c>
-      <c r="B12" t="s">
-        <v>124</v>
-      </c>
-      <c r="C12" t="s">
-        <v>125</v>
-      </c>
-      <c r="D12" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
-        <v>127</v>
-      </c>
-      <c r="B13" t="s">
-        <v>128</v>
-      </c>
-      <c r="C13" t="s">
-        <v>129</v>
-      </c>
-      <c r="D13" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
-        <v>131</v>
-      </c>
-      <c r="B14" t="s">
-        <v>132</v>
-      </c>
-      <c r="C14" t="s">
-        <v>133</v>
-      </c>
-      <c r="D14" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
-        <v>135</v>
-      </c>
-      <c r="B15" t="s">
-        <v>136</v>
-      </c>
-      <c r="C15" t="s">
-        <v>137</v>
-      </c>
-      <c r="D15" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" t="s">
-        <v>139</v>
-      </c>
-      <c r="B16" t="s">
-        <v>140</v>
-      </c>
-      <c r="C16" t="s">
-        <v>141</v>
-      </c>
-      <c r="D16" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" t="s">
-        <v>143</v>
-      </c>
-      <c r="B17" t="s">
-        <v>144</v>
-      </c>
-      <c r="C17" t="s">
-        <v>145</v>
-      </c>
-      <c r="D17" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" t="s">
-        <v>147</v>
-      </c>
-      <c r="B18" t="s">
-        <v>148</v>
-      </c>
-      <c r="C18" t="s">
-        <v>149</v>
-      </c>
-      <c r="D18" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" t="s">
-        <v>151</v>
-      </c>
-      <c r="B19" t="s">
-        <v>152</v>
-      </c>
-      <c r="C19" t="s">
-        <v>153</v>
-      </c>
-      <c r="D19" t="s">
-        <v>154</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C8" t="s">
+        <v>116</v>
+      </c>
+      <c r="D8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>122</v>
+      </c>
+      <c r="B10" t="s">
+        <v>123</v>
+      </c>
+      <c r="C10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>125</v>
+      </c>
+      <c r="B11" t="s">
+        <v>126</v>
+      </c>
+      <c r="C11" t="s">
+        <v>127</v>
+      </c>
+      <c r="D11" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>129</v>
+      </c>
+      <c r="B12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C12" t="s">
+        <v>131</v>
+      </c>
+      <c r="D12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>133</v>
+      </c>
+      <c r="B13" t="s">
+        <v>134</v>
+      </c>
+      <c r="C13" t="s">
+        <v>135</v>
+      </c>
+      <c r="D13" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>137</v>
+      </c>
+      <c r="B14" t="s">
+        <v>138</v>
+      </c>
+      <c r="C14" t="s">
+        <v>139</v>
+      </c>
+      <c r="D14" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>141</v>
+      </c>
+      <c r="B15" t="s">
+        <v>142</v>
+      </c>
+      <c r="C15" t="s">
+        <v>143</v>
+      </c>
+      <c r="D15" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>145</v>
+      </c>
+      <c r="B16" t="s">
+        <v>146</v>
+      </c>
+      <c r="C16" t="s">
+        <v>147</v>
+      </c>
+      <c r="D16" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>149</v>
+      </c>
+      <c r="B17" t="s">
+        <v>150</v>
+      </c>
+      <c r="C17" t="s">
+        <v>151</v>
+      </c>
+      <c r="D17" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>153</v>
+      </c>
+      <c r="B18" t="s">
+        <v>154</v>
+      </c>
+      <c r="C18" t="s">
+        <v>155</v>
+      </c>
+      <c r="D18" t="s">
+        <v>156</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D12"/>
   <sheetViews>
@@ -1766,13 +1870,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C2" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D2" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1780,139 +1884,139 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C3" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D3" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B4" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C4" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D4" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B5" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C5" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D5" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B6" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C6" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D6" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B7" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C7" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D7" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B8" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C8" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="D8" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B9" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C9" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="D9" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B10" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C10" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="D10" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B11" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C11" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="D11" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B12" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C12" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="D12" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -1920,7 +2024,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -1947,13 +2051,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C2" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="D2" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1961,152 +2065,69 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="C3" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="D3" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B4" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C4" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="D4" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B5" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C5" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="D5" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B6" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C6" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="D6" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B7" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C7" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="D7" t="s">
-        <v>218</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" t="s">
-        <v>219</v>
-      </c>
-      <c r="C2" t="s">
         <v>220</v>
-      </c>
-      <c r="D2" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" t="s">
-        <v>222</v>
-      </c>
-      <c r="C3" t="s">
-        <v>223</v>
-      </c>
-      <c r="D3" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>203</v>
-      </c>
-      <c r="B4" t="s">
-        <v>225</v>
-      </c>
-      <c r="C4" t="s">
-        <v>226</v>
-      </c>
-      <c r="D4" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>207</v>
-      </c>
-      <c r="B5" t="s">
-        <v>228</v>
-      </c>
-      <c r="C5" t="s">
-        <v>229</v>
-      </c>
-      <c r="D5" t="s">
-        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -2141,13 +2162,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="C2" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="D2" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2155,41 +2176,124 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="C3" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="D3" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>237</v>
+        <v>205</v>
       </c>
       <c r="B4" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="C4" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="D4" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
+        <v>209</v>
+      </c>
+      <c r="B5" t="s">
+        <v>230</v>
+      </c>
+      <c r="C5" t="s">
+        <v>231</v>
+      </c>
+      <c r="D5" t="s">
+        <v>232</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>233</v>
+      </c>
+      <c r="C2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>236</v>
+      </c>
+      <c r="C3" t="s">
+        <v>237</v>
+      </c>
+      <c r="D3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>239</v>
+      </c>
+      <c r="B4" t="s">
+        <v>240</v>
+      </c>
+      <c r="C4" t="s">
         <v>241</v>
       </c>
+      <c r="D4" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>243</v>
+      </c>
       <c r="B5" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C5" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="D5" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Allow for different key viewer profiles
</commit_message>
<xml_diff>
--- a/AdofaiTweaks.Generator/translations.xlsx
+++ b/AdofaiTweaks.Generator/translations.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="267">
   <si>
     <t>KEY</t>
   </si>
@@ -297,7 +297,7 @@
     <t>켜져 있을 때, 사용자가 등록한 키들로만 입력처리 되도록 제한합니다.</t>
   </si>
   <si>
-    <t>Cuando está activo, restringe qué teclas cuentan como válidas</t>
+    <t>Cuando está activo, restringe qué teclas cuentan como válidas.</t>
   </si>
   <si>
     <t>REGISTERED_KEYS</t>
@@ -357,13 +357,13 @@
     <t>Teclas en pantella</t>
   </si>
   <si>
-    <t>Shows a key viewer for registered keys</t>
-  </si>
-  <si>
-    <t>등록된 키들의 키뷰어 보이기</t>
-  </si>
-  <si>
-    <t>Muestra teclas en pantalla</t>
+    <t>Shows a key viewer for registered keys.</t>
+  </si>
+  <si>
+    <t>등록된 키들의 키뷰어 보이기.</t>
+  </si>
+  <si>
+    <t>Muestra teclas en pantalla.</t>
   </si>
   <si>
     <t>VIEWER_ONLY_GAMEPLAY</t>
@@ -493,6 +493,66 @@
   </si>
   <si>
     <t>Color del texto de las teclas sin pulsar:</t>
+  </si>
+  <si>
+    <t>PROFILES</t>
+  </si>
+  <si>
+    <t>Profiles:</t>
+  </si>
+  <si>
+    <t>프로파일들:</t>
+  </si>
+  <si>
+    <t>Perfiles:</t>
+  </si>
+  <si>
+    <t>PROFILE_NAME</t>
+  </si>
+  <si>
+    <t>Profile name:</t>
+  </si>
+  <si>
+    <t>프로파일 이름:</t>
+  </si>
+  <si>
+    <t>Nombre del perfil:</t>
+  </si>
+  <si>
+    <t>NEW</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>생성</t>
+  </si>
+  <si>
+    <t>Nuevo</t>
+  </si>
+  <si>
+    <t>DUPLICATE</t>
+  </si>
+  <si>
+    <t>Duplicate</t>
+  </si>
+  <si>
+    <t>복제</t>
+  </si>
+  <si>
+    <t>Duplicar</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <t>Delete</t>
+  </si>
+  <si>
+    <t>삭제</t>
+  </si>
+  <si>
+    <t>Eliminar</t>
   </si>
   <si>
     <t>Miscellaneous</t>
@@ -1580,7 +1640,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1836,6 +1896,76 @@
       </c>
       <c r="D18" t="s">
         <v>156</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>157</v>
+      </c>
+      <c r="B19" t="s">
+        <v>158</v>
+      </c>
+      <c r="C19" t="s">
+        <v>159</v>
+      </c>
+      <c r="D19" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>161</v>
+      </c>
+      <c r="B20" t="s">
+        <v>162</v>
+      </c>
+      <c r="C20" t="s">
+        <v>163</v>
+      </c>
+      <c r="D20" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>165</v>
+      </c>
+      <c r="B21" t="s">
+        <v>166</v>
+      </c>
+      <c r="C21" t="s">
+        <v>167</v>
+      </c>
+      <c r="D21" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>169</v>
+      </c>
+      <c r="B22" t="s">
+        <v>170</v>
+      </c>
+      <c r="C22" t="s">
+        <v>171</v>
+      </c>
+      <c r="D22" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>173</v>
+      </c>
+      <c r="B23" t="s">
+        <v>174</v>
+      </c>
+      <c r="C23" t="s">
+        <v>175</v>
+      </c>
+      <c r="D23" t="s">
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -1870,13 +2000,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>157</v>
+        <v>177</v>
       </c>
       <c r="C2" t="s">
-        <v>158</v>
+        <v>178</v>
       </c>
       <c r="D2" t="s">
-        <v>159</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1884,139 +2014,139 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
       <c r="C3" t="s">
-        <v>161</v>
+        <v>181</v>
       </c>
       <c r="D3" t="s">
-        <v>162</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
       <c r="B4" t="s">
-        <v>164</v>
+        <v>184</v>
       </c>
       <c r="C4" t="s">
-        <v>165</v>
+        <v>185</v>
       </c>
       <c r="D4" t="s">
-        <v>166</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
       <c r="B5" t="s">
-        <v>168</v>
+        <v>188</v>
       </c>
       <c r="C5" t="s">
-        <v>169</v>
+        <v>189</v>
       </c>
       <c r="D5" t="s">
-        <v>170</v>
+        <v>190</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>171</v>
+        <v>191</v>
       </c>
       <c r="B6" t="s">
-        <v>172</v>
+        <v>192</v>
       </c>
       <c r="C6" t="s">
-        <v>173</v>
+        <v>193</v>
       </c>
       <c r="D6" t="s">
-        <v>174</v>
+        <v>194</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>175</v>
+        <v>195</v>
       </c>
       <c r="B7" t="s">
-        <v>176</v>
+        <v>196</v>
       </c>
       <c r="C7" t="s">
-        <v>177</v>
+        <v>197</v>
       </c>
       <c r="D7" t="s">
-        <v>178</v>
+        <v>198</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>179</v>
+        <v>199</v>
       </c>
       <c r="B8" t="s">
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="C8" t="s">
-        <v>181</v>
+        <v>201</v>
       </c>
       <c r="D8" t="s">
-        <v>182</v>
+        <v>202</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>183</v>
+        <v>203</v>
       </c>
       <c r="B9" t="s">
-        <v>184</v>
+        <v>204</v>
       </c>
       <c r="C9" t="s">
-        <v>185</v>
+        <v>205</v>
       </c>
       <c r="D9" t="s">
-        <v>186</v>
+        <v>206</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>187</v>
+        <v>207</v>
       </c>
       <c r="B10" t="s">
-        <v>188</v>
+        <v>208</v>
       </c>
       <c r="C10" t="s">
-        <v>189</v>
+        <v>209</v>
       </c>
       <c r="D10" t="s">
-        <v>190</v>
+        <v>210</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>191</v>
+        <v>211</v>
       </c>
       <c r="B11" t="s">
-        <v>192</v>
+        <v>212</v>
       </c>
       <c r="C11" t="s">
-        <v>193</v>
+        <v>213</v>
       </c>
       <c r="D11" t="s">
-        <v>194</v>
+        <v>214</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>195</v>
+        <v>215</v>
       </c>
       <c r="B12" t="s">
-        <v>196</v>
+        <v>216</v>
       </c>
       <c r="C12" t="s">
-        <v>197</v>
+        <v>217</v>
       </c>
       <c r="D12" t="s">
-        <v>198</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -2051,13 +2181,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>199</v>
+        <v>219</v>
       </c>
       <c r="C2" t="s">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="D2" t="s">
-        <v>201</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2065,69 +2195,69 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>202</v>
+        <v>222</v>
       </c>
       <c r="C3" t="s">
-        <v>203</v>
+        <v>223</v>
       </c>
       <c r="D3" t="s">
-        <v>204</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>205</v>
+        <v>225</v>
       </c>
       <c r="B4" t="s">
-        <v>206</v>
+        <v>226</v>
       </c>
       <c r="C4" t="s">
-        <v>207</v>
+        <v>227</v>
       </c>
       <c r="D4" t="s">
-        <v>208</v>
+        <v>228</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>209</v>
+        <v>229</v>
       </c>
       <c r="B5" t="s">
-        <v>210</v>
+        <v>230</v>
       </c>
       <c r="C5" t="s">
-        <v>211</v>
+        <v>231</v>
       </c>
       <c r="D5" t="s">
-        <v>212</v>
+        <v>232</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>213</v>
+        <v>233</v>
       </c>
       <c r="B6" t="s">
-        <v>214</v>
+        <v>234</v>
       </c>
       <c r="C6" t="s">
-        <v>215</v>
+        <v>235</v>
       </c>
       <c r="D6" t="s">
-        <v>216</v>
+        <v>236</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>217</v>
+        <v>237</v>
       </c>
       <c r="B7" t="s">
-        <v>218</v>
+        <v>238</v>
       </c>
       <c r="C7" t="s">
-        <v>219</v>
+        <v>239</v>
       </c>
       <c r="D7" t="s">
-        <v>220</v>
+        <v>240</v>
       </c>
     </row>
   </sheetData>
@@ -2162,13 +2292,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>221</v>
+        <v>241</v>
       </c>
       <c r="C2" t="s">
-        <v>222</v>
+        <v>242</v>
       </c>
       <c r="D2" t="s">
-        <v>223</v>
+        <v>243</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2176,41 +2306,41 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>224</v>
+        <v>244</v>
       </c>
       <c r="C3" t="s">
-        <v>225</v>
+        <v>245</v>
       </c>
       <c r="D3" t="s">
-        <v>226</v>
+        <v>246</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>205</v>
+        <v>225</v>
       </c>
       <c r="B4" t="s">
-        <v>227</v>
+        <v>247</v>
       </c>
       <c r="C4" t="s">
-        <v>228</v>
+        <v>248</v>
       </c>
       <c r="D4" t="s">
-        <v>229</v>
+        <v>249</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>209</v>
+        <v>229</v>
       </c>
       <c r="B5" t="s">
-        <v>230</v>
+        <v>250</v>
       </c>
       <c r="C5" t="s">
-        <v>231</v>
+        <v>251</v>
       </c>
       <c r="D5" t="s">
-        <v>232</v>
+        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -2245,13 +2375,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>233</v>
+        <v>253</v>
       </c>
       <c r="C2" t="s">
-        <v>234</v>
+        <v>254</v>
       </c>
       <c r="D2" t="s">
-        <v>235</v>
+        <v>255</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2259,41 +2389,41 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>236</v>
+        <v>256</v>
       </c>
       <c r="C3" t="s">
-        <v>237</v>
+        <v>257</v>
       </c>
       <c r="D3" t="s">
-        <v>238</v>
+        <v>258</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>239</v>
+        <v>259</v>
       </c>
       <c r="B4" t="s">
-        <v>240</v>
+        <v>260</v>
       </c>
       <c r="C4" t="s">
-        <v>241</v>
+        <v>261</v>
       </c>
       <c r="D4" t="s">
-        <v>242</v>
+        <v>262</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>243</v>
+        <v>263</v>
       </c>
       <c r="B5" t="s">
-        <v>244</v>
+        <v>264</v>
       </c>
       <c r="C5" t="s">
-        <v>245</v>
+        <v>265</v>
       </c>
       <c r="D5" t="s">
-        <v>246</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add option to show key press total
</commit_message>
<xml_diff>
--- a/AdofaiTweaks.Generator/translations.xlsx
+++ b/AdofaiTweaks.Generator/translations.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="271">
   <si>
     <t>KEY</t>
   </si>
@@ -553,6 +553,18 @@
   </si>
   <si>
     <t>Eliminar</t>
+  </si>
+  <si>
+    <t>SHOW_KEY_PRESS_TOTAL</t>
+  </si>
+  <si>
+    <t>Show key press total</t>
+  </si>
+  <si>
+    <t>총 키를 누른 횟수 표시하기</t>
+  </si>
+  <si>
+    <t>Mostrar número total de pulsaciones</t>
   </si>
   <si>
     <t>Miscellaneous</t>
@@ -1640,7 +1652,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1966,6 +1978,20 @@
       </c>
       <c r="D23" t="s">
         <v>176</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>177</v>
+      </c>
+      <c r="B24" t="s">
+        <v>178</v>
+      </c>
+      <c r="C24" t="s">
+        <v>179</v>
+      </c>
+      <c r="D24" t="s">
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -2000,13 +2026,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="C2" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="D2" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2014,139 +2040,139 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="C3" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="D3" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="B4" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="C4" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="D4" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="B5" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="C5" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="D5" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="B6" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="C6" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="D6" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="B7" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="C7" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="D7" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="B8" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="C8" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="D8" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="B9" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="C9" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="D9" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="B10" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="C10" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="D10" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="B11" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="C11" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="D11" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="B12" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="C12" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="D12" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -2181,13 +2207,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="C2" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="D2" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2195,69 +2221,69 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="C3" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="D3" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="B4" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="C4" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="D4" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="B5" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="C5" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="D5" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="B6" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="C6" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="D6" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="B7" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="C7" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="D7" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -2292,13 +2318,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="C2" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="D2" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2306,41 +2332,41 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="C3" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="D3" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="B4" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="C4" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="D4" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="B5" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="C5" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="D5" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
     </row>
   </sheetData>
@@ -2375,13 +2401,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="C2" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="D2" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2389,41 +2415,41 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="C3" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="D3" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="B4" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="C4" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="D4" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="B5" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="C5" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="D5" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add toggle to control key limiter in CLS and main menu
</commit_message>
<xml_diff>
--- a/AdofaiTweaks.Generator/translations.xlsx
+++ b/AdofaiTweaks.Generator/translations.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="275">
   <si>
     <t>KEY</t>
   </si>
@@ -348,6 +348,18 @@
     <t>Cambiar teclas</t>
   </si>
   <si>
+    <t>LIMIT_CLS</t>
+  </si>
+  <si>
+    <t>Limit keys in CLS (Custom Level Select)</t>
+  </si>
+  <si>
+    <t>LIMIT_MAIN_MENU</t>
+  </si>
+  <si>
+    <t>Limit keys in main menu</t>
+  </si>
+  <si>
     <t>Key Viewer</t>
   </si>
   <si>
@@ -360,7 +372,7 @@
     <t>Shows a key viewer for registered keys.</t>
   </si>
   <si>
-    <t>등록된 키들의 키뷰어 보이기.</t>
+    <t>등록된 키들의 키뷰어를 보여줍니다.</t>
   </si>
   <si>
     <t>Muestra teclas en pantalla.</t>
@@ -1541,7 +1553,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1643,6 +1655,22 @@
       </c>
       <c r="D7" t="s">
         <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>110</v>
+      </c>
+      <c r="B9" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -1677,13 +1705,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C2" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D2" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1691,13 +1719,13 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="C3" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D3" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1758,240 +1786,240 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="B8" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="C8" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D8" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="B9" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="C9" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D9" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="B10" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="C10" t="s">
         <v>60</v>
       </c>
       <c r="D10" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B11" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="C11" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="D11" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B12" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C12" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="D12" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B13" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="C13" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="D13" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="B14" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="C14" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="D14" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="B15" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="C15" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="D15" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B16" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="C16" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="D16" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="B17" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="C17" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="D17" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="B18" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="C18" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="D18" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="B19" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="C19" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="D19" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="B20" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="C20" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="D20" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="B21" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C21" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="D21" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="B22" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="C22" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D22" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="B23" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="C23" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="D23" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="B24" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="C24" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="D24" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -2026,13 +2054,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="C2" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="D2" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2040,139 +2068,139 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="C3" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="D3" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="B4" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="C4" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="D4" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="B5" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="C5" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="D5" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="B6" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="C6" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="D6" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="B7" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="C7" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="D7" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="B8" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="C8" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="D8" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="B9" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="C9" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="D9" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="B10" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="C10" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="D10" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="B11" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="C11" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="D11" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="B12" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="C12" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="D12" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -2207,13 +2235,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="C2" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="D2" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2221,69 +2249,69 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="C3" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="D3" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="B4" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="C4" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="D4" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="B5" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="C5" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="D5" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="B6" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="C6" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="D6" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="B7" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="C7" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="D7" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
     </row>
   </sheetData>
@@ -2318,13 +2346,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="C2" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="D2" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2332,41 +2360,41 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="C3" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="D3" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="B4" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="C4" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="D4" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="B5" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="C5" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="D5" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
     </row>
   </sheetData>
@@ -2401,13 +2429,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="C2" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="D2" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2415,41 +2443,41 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="C3" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="D3" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="B4" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="C4" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="D4" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="B5" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="C5" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="D5" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Disable Effects tweak
</commit_message>
<xml_diff>
--- a/AdofaiTweaks.Generator/translations.xlsx
+++ b/AdofaiTweaks.Generator/translations.xlsx
@@ -8,21 +8,22 @@
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" r:id="rId1"/>
-    <sheet name="HideUiElements" sheetId="2" r:id="rId2"/>
-    <sheet name="JudgmentVisuals" sheetId="3" r:id="rId3"/>
-    <sheet name="KeyLimiter" sheetId="4" r:id="rId4"/>
-    <sheet name="KeyViewer" sheetId="5" r:id="rId5"/>
-    <sheet name="Miscellaneous" sheetId="6" r:id="rId6"/>
-    <sheet name="PlanetColor" sheetId="7" r:id="rId7"/>
-    <sheet name="PlanetOpacity" sheetId="8" r:id="rId8"/>
-    <sheet name="RestrictJudgments" sheetId="9" r:id="rId9"/>
+    <sheet name="DisableEffects" sheetId="2" r:id="rId2"/>
+    <sheet name="HideUiElements" sheetId="3" r:id="rId3"/>
+    <sheet name="JudgmentVisuals" sheetId="4" r:id="rId4"/>
+    <sheet name="KeyLimiter" sheetId="5" r:id="rId5"/>
+    <sheet name="KeyViewer" sheetId="6" r:id="rId6"/>
+    <sheet name="Miscellaneous" sheetId="7" r:id="rId7"/>
+    <sheet name="PlanetColor" sheetId="8" r:id="rId8"/>
+    <sheet name="PlanetOpacity" sheetId="9" r:id="rId9"/>
+    <sheet name="RestrictJudgments" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="289">
   <si>
     <t>KEY</t>
   </si>
@@ -75,6 +76,45 @@
     <t>NAME</t>
   </si>
   <si>
+    <t>Disable Effects</t>
+  </si>
+  <si>
+    <t>DESCRIPTION</t>
+  </si>
+  <si>
+    <t>Disables certain effects to improve performance.</t>
+  </si>
+  <si>
+    <t>FILTER</t>
+  </si>
+  <si>
+    <t>Disable VFX filters (Grayscale, Arcade, etc.)</t>
+  </si>
+  <si>
+    <t>BLOOM</t>
+  </si>
+  <si>
+    <t>Disable bloom</t>
+  </si>
+  <si>
+    <t>FLASH</t>
+  </si>
+  <si>
+    <t>Disable screen flashes</t>
+  </si>
+  <si>
+    <t>HALL_OF_MIRRORS</t>
+  </si>
+  <si>
+    <t>Disable "Hall of Mirrors" effect</t>
+  </si>
+  <si>
+    <t>SCREEN_SHAKE</t>
+  </si>
+  <si>
+    <t>Disable screen shake</t>
+  </si>
+  <si>
     <t>Hide UI Elements</t>
   </si>
   <si>
@@ -84,9 +124,6 @@
     <t>Ocultar elementos de la IU</t>
   </si>
   <si>
-    <t>DESCRIPTION</t>
-  </si>
-  <si>
     <t>Hides certain UI elements from gameplay.</t>
   </si>
   <si>
@@ -354,10 +391,16 @@
     <t>Limit keys in CLS (Custom Level Select)</t>
   </si>
   <si>
+    <t>CLS (커스텀 레벨 선택) 에서 키 제한하기</t>
+  </si>
+  <si>
     <t>LIMIT_MAIN_MENU</t>
   </si>
   <si>
     <t>Limit keys in main menu</t>
+  </si>
+  <si>
+    <t>메인 메뉴에서 키 제한하기</t>
   </si>
   <si>
     <t>Key Viewer</t>
@@ -1245,7 +1288,173 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C2" t="s">
+        <v>276</v>
+      </c>
+      <c r="D2" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>278</v>
+      </c>
+      <c r="C3" t="s">
+        <v>279</v>
+      </c>
+      <c r="D3" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>281</v>
+      </c>
+      <c r="B4" t="s">
+        <v>282</v>
+      </c>
+      <c r="C4" t="s">
+        <v>283</v>
+      </c>
+      <c r="D4" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B5" t="s">
+        <v>286</v>
+      </c>
+      <c r="C5" t="s">
+        <v>287</v>
+      </c>
+      <c r="D5" t="s">
+        <v>288</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D9"/>
   <sheetViews>
@@ -1272,111 +1481,111 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="D7" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="C8" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="D8" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="D9" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1384,7 +1593,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D11"/>
   <sheetViews>
@@ -1411,139 +1620,139 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="D2" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="C3" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="D3" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="C4" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="D4" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="C5" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="D5" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="C6" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="D6" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="B7" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C7" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="D7" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="B8" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="C8" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="D8" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="B9" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="C9" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="D9" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="B10" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="C10" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="D10" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="B11" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="C11" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="D11" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1551,7 +1760,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D9"/>
   <sheetViews>
@@ -1578,99 +1787,105 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="C2" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="D2" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C3" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="D3" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="B4" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="C4" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="D4" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="B5" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="C5" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="D5" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="B6" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="C6" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="D6" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="B7" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="C7" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="D7" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="B8" t="s">
-        <v>109</v>
+        <v>121</v>
+      </c>
+      <c r="C8" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="B9" t="s">
-        <v>111</v>
+        <v>124</v>
+      </c>
+      <c r="C9" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -1678,7 +1893,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D24"/>
   <sheetViews>
@@ -1705,321 +1920,321 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>112</v>
+        <v>126</v>
       </c>
       <c r="C2" t="s">
-        <v>113</v>
+        <v>127</v>
       </c>
       <c r="D2" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="C3" t="s">
-        <v>116</v>
+        <v>130</v>
       </c>
       <c r="D3" t="s">
-        <v>117</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="B4" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="C4" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="D4" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="B5" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="C5" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="D5" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="B6" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="C6" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="D6" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="B7" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="C7" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="D7" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
       <c r="B8" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="C8" t="s">
-        <v>120</v>
+        <v>134</v>
       </c>
       <c r="D8" t="s">
-        <v>121</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
       <c r="B9" t="s">
-        <v>123</v>
+        <v>137</v>
       </c>
       <c r="C9" t="s">
-        <v>124</v>
+        <v>138</v>
       </c>
       <c r="D9" t="s">
-        <v>125</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>126</v>
+        <v>140</v>
       </c>
       <c r="B10" t="s">
-        <v>127</v>
+        <v>141</v>
       </c>
       <c r="C10" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="D10" t="s">
-        <v>128</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
       <c r="B11" t="s">
-        <v>130</v>
+        <v>144</v>
       </c>
       <c r="C11" t="s">
-        <v>131</v>
+        <v>145</v>
       </c>
       <c r="D11" t="s">
-        <v>132</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>133</v>
+        <v>147</v>
       </c>
       <c r="B12" t="s">
-        <v>134</v>
+        <v>148</v>
       </c>
       <c r="C12" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="D12" t="s">
-        <v>136</v>
+        <v>150</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>137</v>
+        <v>151</v>
       </c>
       <c r="B13" t="s">
-        <v>138</v>
+        <v>152</v>
       </c>
       <c r="C13" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="D13" t="s">
-        <v>140</v>
+        <v>154</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>141</v>
+        <v>155</v>
       </c>
       <c r="B14" t="s">
-        <v>142</v>
+        <v>156</v>
       </c>
       <c r="C14" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
       <c r="D14" t="s">
-        <v>144</v>
+        <v>158</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>145</v>
+        <v>159</v>
       </c>
       <c r="B15" t="s">
-        <v>146</v>
+        <v>160</v>
       </c>
       <c r="C15" t="s">
-        <v>147</v>
+        <v>161</v>
       </c>
       <c r="D15" t="s">
-        <v>148</v>
+        <v>162</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>149</v>
+        <v>163</v>
       </c>
       <c r="B16" t="s">
-        <v>150</v>
+        <v>164</v>
       </c>
       <c r="C16" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="D16" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>153</v>
+        <v>167</v>
       </c>
       <c r="B17" t="s">
-        <v>154</v>
+        <v>168</v>
       </c>
       <c r="C17" t="s">
-        <v>155</v>
+        <v>169</v>
       </c>
       <c r="D17" t="s">
-        <v>156</v>
+        <v>170</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>157</v>
+        <v>171</v>
       </c>
       <c r="B18" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="C18" t="s">
-        <v>159</v>
+        <v>173</v>
       </c>
       <c r="D18" t="s">
-        <v>160</v>
+        <v>174</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>161</v>
+        <v>175</v>
       </c>
       <c r="B19" t="s">
-        <v>162</v>
+        <v>176</v>
       </c>
       <c r="C19" t="s">
-        <v>163</v>
+        <v>177</v>
       </c>
       <c r="D19" t="s">
-        <v>164</v>
+        <v>178</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>165</v>
+        <v>179</v>
       </c>
       <c r="B20" t="s">
-        <v>166</v>
+        <v>180</v>
       </c>
       <c r="C20" t="s">
-        <v>167</v>
+        <v>181</v>
       </c>
       <c r="D20" t="s">
-        <v>168</v>
+        <v>182</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="B21" t="s">
-        <v>170</v>
+        <v>184</v>
       </c>
       <c r="C21" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="D21" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>173</v>
+        <v>187</v>
       </c>
       <c r="B22" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="C22" t="s">
-        <v>175</v>
+        <v>189</v>
       </c>
       <c r="D22" t="s">
-        <v>176</v>
+        <v>190</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>177</v>
+        <v>191</v>
       </c>
       <c r="B23" t="s">
-        <v>178</v>
+        <v>192</v>
       </c>
       <c r="C23" t="s">
-        <v>179</v>
+        <v>193</v>
       </c>
       <c r="D23" t="s">
-        <v>180</v>
+        <v>194</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>181</v>
+        <v>195</v>
       </c>
       <c r="B24" t="s">
-        <v>182</v>
+        <v>196</v>
       </c>
       <c r="C24" t="s">
-        <v>183</v>
+        <v>197</v>
       </c>
       <c r="D24" t="s">
-        <v>184</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -2027,7 +2242,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D12"/>
   <sheetViews>
@@ -2054,153 +2269,153 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>185</v>
+        <v>199</v>
       </c>
       <c r="C2" t="s">
-        <v>186</v>
+        <v>200</v>
       </c>
       <c r="D2" t="s">
-        <v>187</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>188</v>
+        <v>202</v>
       </c>
       <c r="C3" t="s">
-        <v>189</v>
+        <v>203</v>
       </c>
       <c r="D3" t="s">
-        <v>190</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>191</v>
+        <v>205</v>
       </c>
       <c r="B4" t="s">
-        <v>192</v>
+        <v>206</v>
       </c>
       <c r="C4" t="s">
-        <v>193</v>
+        <v>207</v>
       </c>
       <c r="D4" t="s">
-        <v>194</v>
+        <v>208</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>195</v>
+        <v>209</v>
       </c>
       <c r="B5" t="s">
-        <v>196</v>
+        <v>210</v>
       </c>
       <c r="C5" t="s">
-        <v>197</v>
+        <v>211</v>
       </c>
       <c r="D5" t="s">
-        <v>198</v>
+        <v>212</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>199</v>
+        <v>213</v>
       </c>
       <c r="B6" t="s">
-        <v>200</v>
+        <v>214</v>
       </c>
       <c r="C6" t="s">
-        <v>201</v>
+        <v>215</v>
       </c>
       <c r="D6" t="s">
-        <v>202</v>
+        <v>216</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>203</v>
+        <v>217</v>
       </c>
       <c r="B7" t="s">
-        <v>204</v>
+        <v>218</v>
       </c>
       <c r="C7" t="s">
-        <v>205</v>
+        <v>219</v>
       </c>
       <c r="D7" t="s">
-        <v>206</v>
+        <v>220</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>207</v>
+        <v>221</v>
       </c>
       <c r="B8" t="s">
-        <v>208</v>
+        <v>222</v>
       </c>
       <c r="C8" t="s">
-        <v>209</v>
+        <v>223</v>
       </c>
       <c r="D8" t="s">
-        <v>210</v>
+        <v>224</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>211</v>
+        <v>225</v>
       </c>
       <c r="B9" t="s">
-        <v>212</v>
+        <v>226</v>
       </c>
       <c r="C9" t="s">
-        <v>213</v>
+        <v>227</v>
       </c>
       <c r="D9" t="s">
-        <v>214</v>
+        <v>228</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>215</v>
+        <v>229</v>
       </c>
       <c r="B10" t="s">
-        <v>216</v>
+        <v>230</v>
       </c>
       <c r="C10" t="s">
-        <v>217</v>
+        <v>231</v>
       </c>
       <c r="D10" t="s">
-        <v>218</v>
+        <v>232</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>219</v>
+        <v>233</v>
       </c>
       <c r="B11" t="s">
-        <v>220</v>
+        <v>234</v>
       </c>
       <c r="C11" t="s">
-        <v>221</v>
+        <v>235</v>
       </c>
       <c r="D11" t="s">
-        <v>222</v>
+        <v>236</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>223</v>
+        <v>237</v>
       </c>
       <c r="B12" t="s">
-        <v>224</v>
+        <v>238</v>
       </c>
       <c r="C12" t="s">
-        <v>225</v>
+        <v>239</v>
       </c>
       <c r="D12" t="s">
-        <v>226</v>
+        <v>240</v>
       </c>
     </row>
   </sheetData>
@@ -2208,7 +2423,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -2235,166 +2450,83 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>227</v>
+        <v>241</v>
       </c>
       <c r="C2" t="s">
-        <v>228</v>
+        <v>242</v>
       </c>
       <c r="D2" t="s">
-        <v>229</v>
+        <v>243</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>230</v>
+        <v>244</v>
       </c>
       <c r="C3" t="s">
-        <v>231</v>
+        <v>245</v>
       </c>
       <c r="D3" t="s">
-        <v>232</v>
+        <v>246</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>233</v>
+        <v>247</v>
       </c>
       <c r="B4" t="s">
-        <v>234</v>
+        <v>248</v>
       </c>
       <c r="C4" t="s">
-        <v>235</v>
+        <v>249</v>
       </c>
       <c r="D4" t="s">
-        <v>236</v>
+        <v>250</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>237</v>
+        <v>251</v>
       </c>
       <c r="B5" t="s">
-        <v>238</v>
+        <v>252</v>
       </c>
       <c r="C5" t="s">
-        <v>239</v>
+        <v>253</v>
       </c>
       <c r="D5" t="s">
-        <v>240</v>
+        <v>254</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>241</v>
+        <v>255</v>
       </c>
       <c r="B6" t="s">
-        <v>242</v>
+        <v>256</v>
       </c>
       <c r="C6" t="s">
-        <v>243</v>
+        <v>257</v>
       </c>
       <c r="D6" t="s">
-        <v>244</v>
+        <v>258</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
       <c r="B7" t="s">
-        <v>246</v>
+        <v>260</v>
       </c>
       <c r="C7" t="s">
-        <v>247</v>
+        <v>261</v>
       </c>
       <c r="D7" t="s">
-        <v>248</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" t="s">
-        <v>249</v>
-      </c>
-      <c r="C2" t="s">
-        <v>250</v>
-      </c>
-      <c r="D2" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" t="s">
-        <v>252</v>
-      </c>
-      <c r="C3" t="s">
-        <v>253</v>
-      </c>
-      <c r="D3" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>233</v>
-      </c>
-      <c r="B4" t="s">
-        <v>255</v>
-      </c>
-      <c r="C4" t="s">
-        <v>256</v>
-      </c>
-      <c r="D4" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>237</v>
-      </c>
-      <c r="B5" t="s">
-        <v>258</v>
-      </c>
-      <c r="C5" t="s">
-        <v>259</v>
-      </c>
-      <c r="D5" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -2429,46 +2561,46 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="C2" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="D2" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="C3" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="D3" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>267</v>
+        <v>247</v>
       </c>
       <c r="B4" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C4" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D4" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>271</v>
+        <v>251</v>
       </c>
       <c r="B5" t="s">
         <v>272</v>

</xml_diff>

<commit_message>
Add tile movement limit to Disable Effects
</commit_message>
<xml_diff>
--- a/AdofaiTweaks.Generator/translations.xlsx
+++ b/AdofaiTweaks.Generator/translations.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="293">
   <si>
     <t>KEY</t>
   </si>
@@ -113,6 +113,18 @@
   </si>
   <si>
     <t>Disable screen shake</t>
+  </si>
+  <si>
+    <t>TILE_MOVEMENT_MAX</t>
+  </si>
+  <si>
+    <t>Max number of moving tiles at once:</t>
+  </si>
+  <si>
+    <t>TILE_MOVEMENT_UNLIMITED</t>
+  </si>
+  <si>
+    <t>Unlimited</t>
   </si>
   <si>
     <t>Hide UI Elements</t>
@@ -1315,13 +1327,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="C2" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="D2" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1329,41 +1341,41 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="C3" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="D3" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="B4" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="C4" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="D4" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="B5" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="C5" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="D5" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -1373,7 +1385,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1447,6 +1459,22 @@
       </c>
       <c r="B8" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1481,13 +1509,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1495,97 +1523,97 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D4" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D6" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C7" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D7" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C8" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B9" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C9" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="D9" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1620,13 +1648,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1634,125 +1662,125 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D3" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B4" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C4" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D4" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C5" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D5" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B6" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C6" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="D6" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B7" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="D7" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B8" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C8" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D8" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="B9" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="C9" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="D9" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B10" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="C10" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="D10" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="B11" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C11" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="D11" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1787,13 +1815,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C2" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="D2" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1801,91 +1829,91 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="C3" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D3" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="B4" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C4" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="D4" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B5" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="C5" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="D5" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="B6" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="C6" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="D6" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="B7" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C7" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="D7" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="B8" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="C8" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="B9" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C9" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1920,13 +1948,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="C2" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="D2" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1934,307 +1962,307 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="C3" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="D3" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="B4" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C4" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="D4" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B5" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="C5" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="D5" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="B6" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="C6" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="D6" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="B7" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C7" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="D7" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="B8" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="C8" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="D8" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="B9" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="C9" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="D9" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="B10" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="C10" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D10" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B11" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="C11" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="D11" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="B12" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="C12" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="D12" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="B13" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="C13" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="D13" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="B14" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="C14" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="D14" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="B15" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="C15" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="D15" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="B16" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="C16" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="D16" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="B17" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="C17" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="D17" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="B18" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="C18" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D18" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="B19" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="C19" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="D19" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="B20" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="C20" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="D20" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="B21" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="C21" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="D21" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="B22" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="C22" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="D22" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="B23" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="C23" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="D23" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="B24" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="C24" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="D24" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -2269,13 +2297,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="C2" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="D2" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2283,139 +2311,139 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="C3" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="D3" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="B4" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="C4" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="D4" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="B5" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="C5" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="D5" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="B6" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="C6" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="D6" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="B7" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="C7" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="D7" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="B8" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="C8" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="D8" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="B9" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="C9" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="D9" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="B10" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="C10" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="D10" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="B11" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="C11" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="D11" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="B12" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="C12" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="D12" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -2450,13 +2478,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="C2" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="D2" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2464,69 +2492,69 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="C3" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="D3" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="B4" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="C4" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="D4" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="B5" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="C5" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="D5" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="B6" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="C6" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="D6" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="B7" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="C7" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="D7" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -2561,13 +2589,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="C2" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="D2" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2575,41 +2603,41 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="C3" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="D3" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="B4" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="C4" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="D4" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="B5" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="C5" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="D5" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Use RDString for some settings messages
</commit_message>
<xml_diff>
--- a/AdofaiTweaks.Generator/translations.xlsx
+++ b/AdofaiTweaks.Generator/translations.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="319">
   <si>
     <t>KEY</t>
   </si>
@@ -100,13 +100,13 @@
     <t>FILTER</t>
   </si>
   <si>
-    <t>Disable VFX filters (Grayscale, Arcade, etc.)</t>
-  </si>
-  <si>
-    <t>VFX 필터 (흑백, 아케이드, 등..) 끄기</t>
-  </si>
-  <si>
-    <t>Desactivar efectos de filtro (Grayscale, Arcade, etc.)</t>
+    <t>Disable VFX filters ({0}, {1}, etc.)</t>
+  </si>
+  <si>
+    <t>VFX 필터 ({0}, {1}, 등..) 끄기</t>
+  </si>
+  <si>
+    <t>Desactivar efectos de filtro ({0}, {1}, etc.)</t>
   </si>
   <si>
     <t>BLOOM</t>
@@ -136,13 +136,13 @@
     <t>HALL_OF_MIRRORS</t>
   </si>
   <si>
-    <t>Disable "Hall of Mirrors" effect</t>
-  </si>
-  <si>
-    <t>"거울의 방" 이펙트 끄기</t>
-  </si>
-  <si>
-    <t>Desactivar Cuarto de Espejos (Hall of Mirrors)</t>
+    <t>Disable "{0}" effect</t>
+  </si>
+  <si>
+    <t>"{0}" 이펙트 끄기</t>
+  </si>
+  <si>
+    <t>Desactivar "{0}"</t>
   </si>
   <si>
     <t>SCREEN_SHAKE</t>
@@ -214,13 +214,13 @@
     <t>JUDGE_TEXT</t>
   </si>
   <si>
-    <t>Hide judgment text (Perfect, EPerfect, etc.)</t>
-  </si>
-  <si>
-    <t>판정 텍스트 숨기기 (정확, 빠름, 등..)</t>
-  </si>
-  <si>
-    <t>Ocultar texto de juicios (Perfecto, PerfectoP, etc.)</t>
+    <t>Hide judgment text ({0}, {1}, etc.)</t>
+  </si>
+  <si>
+    <t>판정 텍스트 숨기기 ({0}, {1}, 등..)</t>
+  </si>
+  <si>
+    <t>Ocultar texto de juicios ({0}, {1}, etc.)</t>
   </si>
   <si>
     <t>MISSES</t>
@@ -376,13 +376,13 @@
     <t>HIDE_PERFECTS</t>
   </si>
   <si>
-    <t>Hide "Perfect!" judgments</t>
-  </si>
-  <si>
-    <t>"정확" 판정 숨기기</t>
-  </si>
-  <si>
-    <t>Esconder juicios de "!Perfecto!"</t>
+    <t>Hide "{0}" judgments</t>
+  </si>
+  <si>
+    <t>"{0}" 판정 숨기기</t>
+  </si>
+  <si>
+    <t>Esconder juicios de "{0}"</t>
   </si>
   <si>
     <t>Key Limiter</t>
@@ -818,6 +818,24 @@
   </si>
   <si>
     <t>Desactivar el zoom del editor cuando estás jugando</t>
+  </si>
+  <si>
+    <t>SET_HITSOUND_VOLUME</t>
+  </si>
+  <si>
+    <t>Set the overall hitsound volume</t>
+  </si>
+  <si>
+    <t>전체적인 힛사운드 음량 조정하기</t>
+  </si>
+  <si>
+    <t>CURRENT_HITSOUND_VOLUME</t>
+  </si>
+  <si>
+    <t>Volume:</t>
+  </si>
+  <si>
+    <t>음량:</t>
   </si>
   <si>
     <t>Planet Color</t>
@@ -1387,13 +1405,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>299</v>
+        <v>305</v>
       </c>
       <c r="C2" t="s">
-        <v>300</v>
+        <v>306</v>
       </c>
       <c r="D2" t="s">
-        <v>301</v>
+        <v>307</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1401,41 +1419,41 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>302</v>
+        <v>308</v>
       </c>
       <c r="C3" t="s">
-        <v>303</v>
+        <v>309</v>
       </c>
       <c r="D3" t="s">
-        <v>304</v>
+        <v>310</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>305</v>
+        <v>311</v>
       </c>
       <c r="B4" t="s">
-        <v>306</v>
+        <v>312</v>
       </c>
       <c r="C4" t="s">
-        <v>307</v>
+        <v>313</v>
       </c>
       <c r="D4" t="s">
-        <v>308</v>
+        <v>314</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>309</v>
+        <v>315</v>
       </c>
       <c r="B5" t="s">
-        <v>310</v>
+        <v>316</v>
       </c>
       <c r="C5" t="s">
-        <v>311</v>
+        <v>317</v>
       </c>
       <c r="D5" t="s">
-        <v>312</v>
+        <v>318</v>
       </c>
     </row>
   </sheetData>
@@ -2392,7 +2410,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2564,6 +2582,28 @@
       </c>
       <c r="D12" t="s">
         <v>264</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>265</v>
+      </c>
+      <c r="B13" t="s">
+        <v>266</v>
+      </c>
+      <c r="C13" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>268</v>
+      </c>
+      <c r="B14" t="s">
+        <v>269</v>
+      </c>
+      <c r="C14" t="s">
+        <v>270</v>
       </c>
     </row>
   </sheetData>
@@ -2598,13 +2638,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="C2" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
       <c r="D2" t="s">
-        <v>267</v>
+        <v>273</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2612,69 +2652,69 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="C3" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="D3" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="B4" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="C4" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
       <c r="D4" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="B5" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="C5" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="D5" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="B6" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="C6" t="s">
-        <v>281</v>
+        <v>287</v>
       </c>
       <c r="D6" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>283</v>
+        <v>289</v>
       </c>
       <c r="B7" t="s">
-        <v>284</v>
+        <v>290</v>
       </c>
       <c r="C7" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="D7" t="s">
-        <v>286</v>
+        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -2709,13 +2749,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
       <c r="C2" t="s">
-        <v>288</v>
+        <v>294</v>
       </c>
       <c r="D2" t="s">
-        <v>289</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2723,41 +2763,41 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="C3" t="s">
-        <v>291</v>
+        <v>297</v>
       </c>
       <c r="D3" t="s">
-        <v>292</v>
+        <v>298</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="B4" t="s">
-        <v>293</v>
+        <v>299</v>
       </c>
       <c r="C4" t="s">
-        <v>294</v>
+        <v>300</v>
       </c>
       <c r="D4" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="B5" t="s">
-        <v>296</v>
+        <v>302</v>
       </c>
       <c r="C5" t="s">
-        <v>297</v>
+        <v>303</v>
       </c>
       <c r="D5" t="s">
-        <v>298</v>
+        <v>304</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add ability to move hit error meter
</commit_message>
<xml_diff>
--- a/AdofaiTweaks.Generator/translations.xlsx
+++ b/AdofaiTweaks.Generator/translations.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="488">
   <si>
     <t>KEY</t>
   </si>
@@ -64,6 +64,9 @@
     <t>C'est un string de test.</t>
   </si>
   <si>
+    <t>Đây là dòng chữ thử nghiệm</t>
+  </si>
+  <si>
     <t>GLOBAL_LANGUAGE</t>
   </si>
   <si>
@@ -82,6 +85,9 @@
     <t>Langue:</t>
   </si>
   <si>
+    <t>Ngôn ngữ:</t>
+  </si>
+  <si>
     <t>LANGUAGE_NAME</t>
   </si>
   <si>
@@ -121,6 +127,9 @@
     <t>Désactiver les Effets</t>
   </si>
   <si>
+    <t>Tắt hiệu ứng</t>
+  </si>
+  <si>
     <t>DESCRIPTION</t>
   </si>
   <si>
@@ -139,6 +148,9 @@
     <t>Désactive certains effets pour améliorer la performance.</t>
   </si>
   <si>
+    <t>Tắt đi một số hiệu ứng nhất định nhằm cải thiện chất lượng</t>
+  </si>
+  <si>
     <t>FILTER</t>
   </si>
   <si>
@@ -157,6 +169,9 @@
     <t>Désactive le filtre "VFX" ({0}, {1}, etc.)</t>
   </si>
   <si>
+    <t>Tắt hiệu ứng thay đổi tầm nhìn ({0}, {1}, v.v)</t>
+  </si>
+  <si>
     <t>BLOOM</t>
   </si>
   <si>
@@ -175,6 +190,9 @@
     <t>Désactive le bloom</t>
   </si>
   <si>
+    <t>Tắt hiệu ứng "nở"</t>
+  </si>
+  <si>
     <t>FLASH</t>
   </si>
   <si>
@@ -193,6 +211,9 @@
     <t>Désactive les flashs</t>
   </si>
   <si>
+    <t>Tắt hiệu ứng nháy màn hình</t>
+  </si>
+  <si>
     <t>HALL_OF_MIRRORS</t>
   </si>
   <si>
@@ -211,6 +232,9 @@
     <t>Désactive l'effets "{0}"</t>
   </si>
   <si>
+    <t>Tắt hiệu ứng "{0}"</t>
+  </si>
+  <si>
     <t>SCREEN_SHAKE</t>
   </si>
   <si>
@@ -229,6 +253,9 @@
     <t>Désactive les tremblements de l'écran</t>
   </si>
   <si>
+    <t>Tắt màn hình rung lắc</t>
+  </si>
+  <si>
     <t>TILE_MOVEMENT_MAX</t>
   </si>
   <si>
@@ -247,6 +274,9 @@
     <t>Nombre max de tile qui bougent en même temps:</t>
   </si>
   <si>
+    <t>Thay đổi số lượng ô có thể di chuyển một lúc:</t>
+  </si>
+  <si>
     <t>TILE_MOVEMENT_UNLIMITED</t>
   </si>
   <si>
@@ -265,6 +295,27 @@
     <t>Infini</t>
   </si>
   <si>
+    <t>Không giới hạn</t>
+  </si>
+  <si>
+    <t>EXCLUDE_FILTER_LIST</t>
+  </si>
+  <si>
+    <t>Excluded Filters ({0})</t>
+  </si>
+  <si>
+    <t>비활성화 제외 필터들 ({0})</t>
+  </si>
+  <si>
+    <t>EXCLUDE_FILTER_START_LIST</t>
+  </si>
+  <si>
+    <t>Filters to exclude:</t>
+  </si>
+  <si>
+    <t>제외할 필터들:</t>
+  </si>
+  <si>
     <t>Hide UI Elements</t>
   </si>
   <si>
@@ -280,6 +331,9 @@
     <t>Masque des éléments d'UI</t>
   </si>
   <si>
+    <t>Ẩn giao diện (UI)</t>
+  </si>
+  <si>
     <t>Hides certain UI elements from gameplay.</t>
   </si>
   <si>
@@ -295,6 +349,9 @@
     <t>Masque certains éléments d'UI du gameplay.</t>
   </si>
   <si>
+    <t>Làm ẩn một số giao diện (UI) khi chơi</t>
+  </si>
+  <si>
     <t>EVERYTHING</t>
   </si>
   <si>
@@ -313,6 +370,9 @@
     <t>Masque tout les éléments (Note: ça inclu peut-être des textes sécifique dans le menu)</t>
   </si>
   <si>
+    <t>Làm ẩn tất cả các giao diện (UI) (lựa chọn này sẽ làm ẩn một số dòng chữ trong màn hình chính)</t>
+  </si>
+  <si>
     <t>JUDGE_TEXT</t>
   </si>
   <si>
@@ -331,6 +391,9 @@
     <t>Masque les textes de jugements ({0}, {1}, etc.)</t>
   </si>
   <si>
+    <t>Ẩn dòng chữ hiển thị độ chính xác ({0}, {1}, v.v)</t>
+  </si>
+  <si>
     <t>MISSES</t>
   </si>
   <si>
@@ -349,6 +412,9 @@
     <t>Masque les indicateur de raté (croix rouge)</t>
   </si>
   <si>
+    <t>Ẩn chỉ thị nhấn trượt (ô trắng có chữ X)</t>
+  </si>
+  <si>
     <t>SONG_TITLE</t>
   </si>
   <si>
@@ -367,6 +433,9 @@
     <t>Masque le nom de l'artiste et de la musique</t>
   </si>
   <si>
+    <t>Ẩn tên nhạc, tác giả</t>
+  </si>
+  <si>
     <t>AUTO</t>
   </si>
   <si>
@@ -385,6 +454,9 @@
     <t>Masque otto, le texte d'autoplay et la timing target</t>
   </si>
   <si>
+    <t>Ẩn Otto, dòng chữ "tự động chơi" và biểu tượng biểu thị độ chính xác cần thiết</t>
+  </si>
+  <si>
     <t>BETA_BUILD</t>
   </si>
   <si>
@@ -403,6 +475,9 @@
     <t>Masque le texte "Beta Build"</t>
   </si>
   <si>
+    <t>Ẩn dòng chữ "Beta Build"</t>
+  </si>
+  <si>
     <t>Judgment Visuals</t>
   </si>
   <si>
@@ -418,6 +493,9 @@
     <t>Visuels de Jugements</t>
   </si>
   <si>
+    <t>Thay đổi biểu thị độ chính xác</t>
+  </si>
+  <si>
     <t>Improves the visuals of judgments.</t>
   </si>
   <si>
@@ -433,6 +511,9 @@
     <t>Améliore le visuel de jugements.</t>
   </si>
   <si>
+    <t>Cải thiện cách biểu thị độ chính xác.</t>
+  </si>
+  <si>
     <t>SHOW_HIT_ERROR_METER</t>
   </si>
   <si>
@@ -448,6 +529,9 @@
     <t>Affiche le visualiseur de hit</t>
   </si>
   <si>
+    <t>Hiển thị bảng đo cho biết độ chính xác</t>
+  </si>
+  <si>
     <t>ERROR_METER_SCALE</t>
   </si>
   <si>
@@ -466,6 +550,9 @@
     <t>Taille:</t>
   </si>
   <si>
+    <t>Kích cỡ:</t>
+  </si>
+  <si>
     <t>ERROR_METER_TICK_LIFE</t>
   </si>
   <si>
@@ -481,6 +568,9 @@
     <t>Tick d'affiche des hit</t>
   </si>
   <si>
+    <t>Thời gian hiển thị các vạch:</t>
+  </si>
+  <si>
     <t>ERROR_METER_TICK_SECONDS</t>
   </si>
   <si>
@@ -499,6 +589,9 @@
     <t>{0} seconde(s)</t>
   </si>
   <si>
+    <t>{0} giây</t>
+  </si>
+  <si>
     <t>ERROR_METER_SENSITIVITY</t>
   </si>
   <si>
@@ -517,6 +610,9 @@
     <t>Sensibilité de la flèche au desus</t>
   </si>
   <si>
+    <t>Độ nhạy của mũi tên:</t>
+  </si>
+  <si>
     <t>ERROR_METER_MORE_STABLE</t>
   </si>
   <si>
@@ -535,6 +631,9 @@
     <t>Plus stable</t>
   </si>
   <si>
+    <t>Ổn định hơn</t>
+  </si>
+  <si>
     <t>ERROR_METER_LESS_STABLE</t>
   </si>
   <si>
@@ -553,6 +652,9 @@
     <t>Moins stable</t>
   </si>
   <si>
+    <t>Kém ổn định hơn</t>
+  </si>
+  <si>
     <t>HIDE_PERFECTS</t>
   </si>
   <si>
@@ -571,6 +673,45 @@
     <t>Masque les "{0}" jugements</t>
   </si>
   <si>
+    <t>Ẩn dòng chữ "{0}"</t>
+  </si>
+  <si>
+    <t>ERROR_METER_X_POS</t>
+  </si>
+  <si>
+    <t>X Position:</t>
+  </si>
+  <si>
+    <t>가로 위치:</t>
+  </si>
+  <si>
+    <t>Posición X:</t>
+  </si>
+  <si>
+    <t>Position X:</t>
+  </si>
+  <si>
+    <t>Vị trí theo trục ngang (X):</t>
+  </si>
+  <si>
+    <t>ERROR_METER_Y_POS</t>
+  </si>
+  <si>
+    <t>Y Position:</t>
+  </si>
+  <si>
+    <t>세로 위치:</t>
+  </si>
+  <si>
+    <t>Posición Y:</t>
+  </si>
+  <si>
+    <t>Position Y:</t>
+  </si>
+  <si>
+    <t>Vị trí theo trục dọc (Y):</t>
+  </si>
+  <si>
     <t>Key Viewer</t>
   </si>
   <si>
@@ -583,6 +724,9 @@
     <t>Viewer de Touche</t>
   </si>
   <si>
+    <t>Hiển thị phím</t>
+  </si>
+  <si>
     <t>Shows a key viewer for registered keys.</t>
   </si>
   <si>
@@ -595,6 +739,9 @@
     <t>Affiche les touches appuyer.</t>
   </si>
   <si>
+    <t>Hiển thị những phím được nhấn khi đang chơi.</t>
+  </si>
+  <si>
     <t>REGISTERED_KEYS</t>
   </si>
   <si>
@@ -610,6 +757,9 @@
     <t>Touches registrer</t>
   </si>
   <si>
+    <t>Những phím được thêm vào:</t>
+  </si>
+  <si>
     <t>DONE</t>
   </si>
   <si>
@@ -625,6 +775,9 @@
     <t>Valider</t>
   </si>
   <si>
+    <t>Hoàn tất</t>
+  </si>
+  <si>
     <t>PRESS_KEY_REGISTER</t>
   </si>
   <si>
@@ -640,6 +793,9 @@
     <t>Appuy sur une touche pour l'enregister/la d'esenregistrer</t>
   </si>
   <si>
+    <t>Nhấn phím để thêm / loại bỏ chúng</t>
+  </si>
+  <si>
     <t>CHANGE_KEYS</t>
   </si>
   <si>
@@ -655,6 +811,9 @@
     <t>Changer les touche</t>
   </si>
   <si>
+    <t>Đổi phím</t>
+  </si>
+  <si>
     <t>VIEWER_ONLY_GAMEPLAY</t>
   </si>
   <si>
@@ -670,6 +829,9 @@
     <t>Seulement visible durant le gameplay</t>
   </si>
   <si>
+    <t>Chỉ hiện lên khi đang chơi</t>
+  </si>
+  <si>
     <t>ANIMATE_KEYS</t>
   </si>
   <si>
@@ -685,6 +847,9 @@
     <t>Anime l'appuy de touche</t>
   </si>
   <si>
+    <t>Thêm hiệu ứng khi nhấn</t>
+  </si>
+  <si>
     <t>KEY_VIEWER_SIZE</t>
   </si>
   <si>
@@ -694,36 +859,15 @@
     <t>Tamaño:</t>
   </si>
   <si>
+    <t>Kích cỡ</t>
+  </si>
+  <si>
     <t>KEY_VIEWER_X_POS</t>
   </si>
   <si>
-    <t>X Position:</t>
-  </si>
-  <si>
-    <t>가로 위치:</t>
-  </si>
-  <si>
-    <t>Posición X:</t>
-  </si>
-  <si>
-    <t>Position X:</t>
-  </si>
-  <si>
     <t>KEY_VIEWER_Y_POS</t>
   </si>
   <si>
-    <t>Y Position:</t>
-  </si>
-  <si>
-    <t>세로 위치:</t>
-  </si>
-  <si>
-    <t>Posición Y:</t>
-  </si>
-  <si>
-    <t>Position Y:</t>
-  </si>
-  <si>
     <t>PRESSED_OUTLINE_COLOR</t>
   </si>
   <si>
@@ -739,6 +883,9 @@
     <t>Couleur du contour lorsque la touche est appuyer:</t>
   </si>
   <si>
+    <t>Màu cạnh ngoài cùng khi nhấn phím:</t>
+  </si>
+  <si>
     <t>RELEASED_OUTLINE_COLOR</t>
   </si>
   <si>
@@ -754,6 +901,9 @@
     <t>Couleur du contour lorsque la touche est relaché</t>
   </si>
   <si>
+    <t>Màu cạnh ngoài cùng khi thả phím:</t>
+  </si>
+  <si>
     <t>PRESSED_BACKGROUND_COLOR</t>
   </si>
   <si>
@@ -769,6 +919,9 @@
     <t>Couleur de l'arrière plan lorsque la touche est présser</t>
   </si>
   <si>
+    <t>Màu nền khi nhấn phím:</t>
+  </si>
+  <si>
     <t>RELEASED_BACKGROUND_COLOR</t>
   </si>
   <si>
@@ -784,6 +937,9 @@
     <t>Couleur de l'arrière plan lorsque la touche est relaché</t>
   </si>
   <si>
+    <t>Màu nền khi thả phím:</t>
+  </si>
+  <si>
     <t>PRESSED_TEXT_COLOR</t>
   </si>
   <si>
@@ -799,6 +955,9 @@
     <t>Couleur du texte lorsque la touche est présser</t>
   </si>
   <si>
+    <t>Màu chữ khi nhấn phím:</t>
+  </si>
+  <si>
     <t>RELEASED_TEXT_COLOR</t>
   </si>
   <si>
@@ -814,6 +973,9 @@
     <t>Couleur du texte lorsque la touche est relacher</t>
   </si>
   <si>
+    <t>Màu chữ khi thả phím:</t>
+  </si>
+  <si>
     <t>PROFILES</t>
   </si>
   <si>
@@ -829,6 +991,9 @@
     <t>Profiles</t>
   </si>
   <si>
+    <t>Những cài đặt đã lưu:</t>
+  </si>
+  <si>
     <t>PROFILE_NAME</t>
   </si>
   <si>
@@ -844,6 +1009,9 @@
     <t>Nom du profile</t>
   </si>
   <si>
+    <t>Tên cài đặt:</t>
+  </si>
+  <si>
     <t>NEW</t>
   </si>
   <si>
@@ -859,6 +1027,9 @@
     <t>Nouveau</t>
   </si>
   <si>
+    <t>Tạo mới</t>
+  </si>
+  <si>
     <t>DUPLICATE</t>
   </si>
   <si>
@@ -874,6 +1045,9 @@
     <t>Dupliquer</t>
   </si>
   <si>
+    <t>Sao chép</t>
+  </si>
+  <si>
     <t>DELETE</t>
   </si>
   <si>
@@ -889,6 +1063,9 @@
     <t>Suprimmer</t>
   </si>
   <si>
+    <t>Xoá</t>
+  </si>
+  <si>
     <t>SHOW_KEY_PRESS_TOTAL</t>
   </si>
   <si>
@@ -904,6 +1081,9 @@
     <t>Affichger le total des touche appuyer</t>
   </si>
   <si>
+    <t>Biểu thị tổng số lần đã nhấn phím</t>
+  </si>
+  <si>
     <t>Key Limiter</t>
   </si>
   <si>
@@ -916,6 +1096,9 @@
     <t>Limiteur de Trouches</t>
   </si>
   <si>
+    <t>Giới hạn phím nhấn</t>
+  </si>
+  <si>
     <t>When active, restricts which keys count as input.</t>
   </si>
   <si>
@@ -928,6 +1111,9 @@
     <t>Quand activée, restreint les touche qui compte comme une input.</t>
   </si>
   <si>
+    <t>Giới hạn những phím nhất định được nhấn khi được kích hoạt.</t>
+  </si>
+  <si>
     <t>Zarejestrowane przyciski:</t>
   </si>
   <si>
@@ -943,9 +1129,15 @@
     <t>Appuy sur une touche pour l'enregistrer/la d'ésenregistrer</t>
   </si>
   <si>
+    <t>Nhấn phím để thêm / loại bỏ...</t>
+  </si>
+  <si>
     <t>Changer les touches</t>
   </si>
   <si>
+    <t>Thay đổi phím</t>
+  </si>
+  <si>
     <t>LIMIT_CLS</t>
   </si>
   <si>
@@ -961,6 +1153,9 @@
     <t>Limit les touche dans le selcteur de custom song</t>
   </si>
   <si>
+    <t>Giới hạn phím nhấn khi lựa chọn vòng chơi</t>
+  </si>
+  <si>
     <t>LIMIT_MAIN_MENU</t>
   </si>
   <si>
@@ -976,6 +1171,9 @@
     <t>Limite les touche  dans le menu principale</t>
   </si>
   <si>
+    <t>Giới hạn phím nhấn khi ở màn hình chính</t>
+  </si>
+  <si>
     <t>Miscellaneous</t>
   </si>
   <si>
@@ -988,6 +1186,9 @@
     <t>Divers</t>
   </si>
   <si>
+    <t>Cài đặt khác</t>
+  </si>
+  <si>
     <t>Tweaks that do not belong in any particular section.</t>
   </si>
   <si>
@@ -1000,6 +1201,9 @@
     <t>Des tweaks qui ne se range pas dans les autre catégorie.</t>
   </si>
   <si>
+    <t>Các cài đặt không thuộc vào bất kì phần cụ thể nào.</t>
+  </si>
+  <si>
     <t>GLITCH_FLIP</t>
   </si>
   <si>
@@ -1015,109 +1219,7 @@
     <t>Désactive le retournement d'écran pour le filte "{0}"</t>
   </si>
   <si>
-    <t>NO_FAIL</t>
-  </si>
-  <si>
-    <t>No fail mode</t>
-  </si>
-  <si>
-    <t>무적 모드</t>
-  </si>
-  <si>
-    <t>Modo sin fallos</t>
-  </si>
-  <si>
-    <t>Mode invincible</t>
-  </si>
-  <si>
-    <t>NO_FAIL_ENABLED</t>
-  </si>
-  <si>
-    <t>No fail enabled!</t>
-  </si>
-  <si>
-    <t>무적 모드 켜짐!</t>
-  </si>
-  <si>
-    <t>¡Modo sin fallos activado!</t>
-  </si>
-  <si>
-    <t>Mode invincible activée</t>
-  </si>
-  <si>
-    <t>MISS_COUNT</t>
-  </si>
-  <si>
-    <t>Misses: {0}</t>
-  </si>
-  <si>
-    <t>미스 수: {0}</t>
-  </si>
-  <si>
-    <t>Fallos: {0}</t>
-  </si>
-  <si>
-    <t>Ratés: {0}</t>
-  </si>
-  <si>
-    <t>OVERLOAD_COUNT</t>
-  </si>
-  <si>
-    <t>Overloads: {0}</t>
-  </si>
-  <si>
-    <t>과부하 수: {0}</t>
-  </si>
-  <si>
-    <t>Sobrecargas: {0}</t>
-  </si>
-  <si>
-    <t>Morts: {0}</t>
-  </si>
-  <si>
-    <t>PREVENT_OTTO_FAIL</t>
-  </si>
-  <si>
-    <t>Prevent Otto from failing</t>
-  </si>
-  <si>
-    <t>오토가 죽는 것을 방지하기</t>
-  </si>
-  <si>
-    <t>Prevenir que Otto falle</t>
-  </si>
-  <si>
-    <t>Empêche otto de mourir</t>
-  </si>
-  <si>
-    <t>EDITOR_DIFFICULTY</t>
-  </si>
-  <si>
-    <t>Set judgment difficulty in the editor</t>
-  </si>
-  <si>
-    <t>에디터 이내에서 난이도 설정하기</t>
-  </si>
-  <si>
-    <t>Cambiar la ventana de tiempo en el editor</t>
-  </si>
-  <si>
-    <t>Choisir la difficulté de jugements dans l'éditeur</t>
-  </si>
-  <si>
-    <t>EDITOR_DIFFICULTY_CURRENT</t>
-  </si>
-  <si>
-    <t>(Current: {0})</t>
-  </si>
-  <si>
-    <t>(현재 난이도: {0})</t>
-  </si>
-  <si>
-    <t>(Ventana actual: {0})</t>
-  </si>
-  <si>
-    <t>(En cour: {0})</t>
+    <t>Vô hiệu hoá xoay màn hình cho hiệu ứng "{0}"</t>
   </si>
   <si>
     <t>EDITOR_ZOOM</t>
@@ -1135,6 +1237,9 @@
     <t>Désactive le zoom en avant/en arrière de l'éditeur pendant la partie</t>
   </si>
   <si>
+    <t>Vô hiệu hoá phóng to / thu nhỏ khi chơi</t>
+  </si>
+  <si>
     <t>SET_HITSOUND_VOLUME</t>
   </si>
   <si>
@@ -1147,6 +1252,9 @@
     <t>Choisir le volume du hitsound</t>
   </si>
   <si>
+    <t>Chỉnh âm lượng "hitsound"</t>
+  </si>
+  <si>
     <t>CURRENT_HITSOUND_VOLUME</t>
   </si>
   <si>
@@ -1156,6 +1264,9 @@
     <t>음량:</t>
   </si>
   <si>
+    <t>Âm lượng:</t>
+  </si>
+  <si>
     <t>Planet Opacity</t>
   </si>
   <si>
@@ -1168,6 +1279,9 @@
     <t>Opactié des Planètes</t>
   </si>
   <si>
+    <t>Độ trong suốt của hành tinh</t>
+  </si>
+  <si>
     <t>Sets the opacity of the planets.</t>
   </si>
   <si>
@@ -1180,6 +1294,9 @@
     <t>Change l'opactié des planètes.</t>
   </si>
   <si>
+    <t>Chỉnh độ trong suốt của các hành tinh.</t>
+  </si>
+  <si>
     <t>PLANET_ONE</t>
   </si>
   <si>
@@ -1195,6 +1312,9 @@
     <t>Planète 1:</t>
   </si>
   <si>
+    <t>Độ trong suốt của hành tinh thứ nhất:</t>
+  </si>
+  <si>
     <t>PLANET_TWO</t>
   </si>
   <si>
@@ -1210,6 +1330,9 @@
     <t>Planète 2:</t>
   </si>
   <si>
+    <t>Độ trong suốt của hành tinh thứ hai:</t>
+  </si>
+  <si>
     <t>Planet Color</t>
   </si>
   <si>
@@ -1222,6 +1345,9 @@
     <t>Couleur de Planètes</t>
   </si>
   <si>
+    <t>Màu của các hành tinh</t>
+  </si>
+  <si>
     <t>Sets the color of the planets.</t>
   </si>
   <si>
@@ -1234,6 +1360,9 @@
     <t>Choisir la couleur des planètes.</t>
   </si>
   <si>
+    <t>Thay đổi màu dành cho từng hành tinh.</t>
+  </si>
+  <si>
     <t>Planet 1:</t>
   </si>
   <si>
@@ -1243,6 +1372,9 @@
     <t>Planeta 1:</t>
   </si>
   <si>
+    <t>Hành tinh thứ nhất:</t>
+  </si>
+  <si>
     <t>Planet 2:</t>
   </si>
   <si>
@@ -1252,6 +1384,9 @@
     <t>Planeta 2:</t>
   </si>
   <si>
+    <t>Hành tinh thứ hai:</t>
+  </si>
+  <si>
     <t>BODY</t>
   </si>
   <si>
@@ -1267,6 +1402,9 @@
     <t>Corp:</t>
   </si>
   <si>
+    <t>Thân:</t>
+  </si>
+  <si>
     <t>TAIL</t>
   </si>
   <si>
@@ -1282,6 +1420,9 @@
     <t>Trainé:</t>
   </si>
   <si>
+    <t>Đuôi:</t>
+  </si>
+  <si>
     <t>Restrict Judgments</t>
   </si>
   <si>
@@ -1294,6 +1435,9 @@
     <t>Jugements Restreint</t>
   </si>
   <si>
+    <t>Giới hạn lỗi cho phép</t>
+  </si>
+  <si>
     <t>Kills the player on certain judgments.</t>
   </si>
   <si>
@@ -1306,6 +1450,9 @@
     <t>Tue le joueur dans certain jugements.</t>
   </si>
   <si>
+    <t>Làm bạn thua khi phạm lỗi sai nhất định.</t>
+  </si>
+  <si>
     <t>RESTRICT</t>
   </si>
   <si>
@@ -1321,6 +1468,9 @@
     <t>Jugements restreint: "{0}"</t>
   </si>
   <si>
+    <t>Giới hạn lỗi: "{0}"</t>
+  </si>
+  <si>
     <t>CUSTOM_DEATH</t>
   </si>
   <si>
@@ -1333,7 +1483,10 @@
     <t xml:space="preserve">Mensaje de muerte personalizado con restricción de juicio (Nota: "{judgment}" será reemplazado por el nombre de la ventana de tiempo) </t>
   </si>
   <si>
-    <t>Message de mort personnalisé sur la restriction de jugements (note : "{judgement}" ouccurence vas être remplacer par le nom du jugements)</t>
+    <t>Message de mort personnalisé sur la restriction de jugements (note: "{judgement}" ouccurence vas être remplacer par le nom du jugements)</t>
+  </si>
+  <si>
+    <t>Dòng chữ thông báo thua khác khi phạm lỗi sai nhất định</t>
   </si>
 </sst>
 </file>
@@ -1713,48 +1866,54 @@
       <c r="F2" t="s">
         <v>12</v>
       </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1795,82 +1954,94 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>419</v>
+        <v>466</v>
       </c>
       <c r="C2" t="s">
-        <v>420</v>
+        <v>467</v>
       </c>
       <c r="D2" t="s">
-        <v>421</v>
+        <v>468</v>
       </c>
       <c r="E2" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="F2" t="s">
-        <v>422</v>
+        <v>469</v>
+      </c>
+      <c r="G2" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>423</v>
+        <v>471</v>
       </c>
       <c r="C3" t="s">
-        <v>424</v>
+        <v>472</v>
       </c>
       <c r="D3" t="s">
-        <v>425</v>
+        <v>473</v>
       </c>
       <c r="E3" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="F3" t="s">
-        <v>426</v>
+        <v>474</v>
+      </c>
+      <c r="G3" t="s">
+        <v>475</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>427</v>
+        <v>476</v>
       </c>
       <c r="B4" t="s">
-        <v>428</v>
+        <v>477</v>
       </c>
       <c r="C4" t="s">
-        <v>429</v>
+        <v>478</v>
       </c>
       <c r="D4" t="s">
-        <v>430</v>
+        <v>479</v>
       </c>
       <c r="E4" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="F4" t="s">
-        <v>431</v>
+        <v>480</v>
+      </c>
+      <c r="G4" t="s">
+        <v>481</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>432</v>
+        <v>482</v>
       </c>
       <c r="B5" t="s">
-        <v>433</v>
+        <v>483</v>
       </c>
       <c r="C5" t="s">
-        <v>434</v>
+        <v>484</v>
       </c>
       <c r="D5" t="s">
-        <v>435</v>
+        <v>485</v>
       </c>
       <c r="E5" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="F5" t="s">
-        <v>436</v>
+        <v>486</v>
+      </c>
+      <c r="G5" t="s">
+        <v>487</v>
       </c>
     </row>
   </sheetData>
@@ -1880,7 +2051,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1911,182 +2082,231 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F2" t="s">
-        <v>31</v>
+        <v>33</v>
+      </c>
+      <c r="G2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F3" t="s">
-        <v>37</v>
+        <v>40</v>
+      </c>
+      <c r="G3" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E4" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F4" t="s">
-        <v>43</v>
+        <v>47</v>
+      </c>
+      <c r="G4" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="D5" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="E5" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="F5" t="s">
-        <v>49</v>
+        <v>54</v>
+      </c>
+      <c r="G5" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="D6" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="E6" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="F6" t="s">
-        <v>55</v>
+        <v>61</v>
+      </c>
+      <c r="G6" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="C7" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="D7" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="E7" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="F7" t="s">
-        <v>61</v>
+        <v>68</v>
+      </c>
+      <c r="G7" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="B8" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="C8" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="D8" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="E8" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="F8" t="s">
-        <v>67</v>
+        <v>75</v>
+      </c>
+      <c r="G8" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="B9" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="C9" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="D9" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="E9" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="F9" t="s">
-        <v>73</v>
+        <v>82</v>
+      </c>
+      <c r="G9" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="B10" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="C10" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="D10" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="E10" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="F10" t="s">
-        <v>79</v>
+        <v>89</v>
+      </c>
+      <c r="G10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" t="s">
+        <v>92</v>
+      </c>
+      <c r="C11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>94</v>
+      </c>
+      <c r="B12" t="s">
+        <v>95</v>
+      </c>
+      <c r="C12" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -2127,162 +2347,186 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>97</v>
       </c>
       <c r="C2" t="s">
-        <v>81</v>
+        <v>98</v>
       </c>
       <c r="D2" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="E2" t="s">
-        <v>83</v>
+        <v>100</v>
       </c>
       <c r="F2" t="s">
-        <v>84</v>
+        <v>101</v>
+      </c>
+      <c r="G2" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
+        <v>103</v>
       </c>
       <c r="C3" t="s">
-        <v>86</v>
+        <v>104</v>
       </c>
       <c r="D3" t="s">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="E3" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
       <c r="F3" t="s">
-        <v>89</v>
+        <v>107</v>
+      </c>
+      <c r="G3" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>90</v>
+        <v>109</v>
       </c>
       <c r="B4" t="s">
-        <v>91</v>
+        <v>110</v>
       </c>
       <c r="C4" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="D4" t="s">
-        <v>93</v>
+        <v>112</v>
       </c>
       <c r="E4" t="s">
-        <v>94</v>
+        <v>113</v>
       </c>
       <c r="F4" t="s">
-        <v>95</v>
+        <v>114</v>
+      </c>
+      <c r="G4" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>96</v>
+        <v>116</v>
       </c>
       <c r="B5" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="C5" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
       <c r="D5" t="s">
-        <v>99</v>
+        <v>119</v>
       </c>
       <c r="E5" t="s">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="F5" t="s">
-        <v>101</v>
+        <v>121</v>
+      </c>
+      <c r="G5" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>102</v>
+        <v>123</v>
       </c>
       <c r="B6" t="s">
-        <v>103</v>
+        <v>124</v>
       </c>
       <c r="C6" t="s">
-        <v>104</v>
+        <v>125</v>
       </c>
       <c r="D6" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="E6" t="s">
-        <v>106</v>
+        <v>127</v>
       </c>
       <c r="F6" t="s">
-        <v>107</v>
+        <v>128</v>
+      </c>
+      <c r="G6" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>108</v>
+        <v>130</v>
       </c>
       <c r="B7" t="s">
-        <v>109</v>
+        <v>131</v>
       </c>
       <c r="C7" t="s">
-        <v>110</v>
+        <v>132</v>
       </c>
       <c r="D7" t="s">
-        <v>111</v>
+        <v>133</v>
       </c>
       <c r="E7" t="s">
-        <v>112</v>
+        <v>134</v>
       </c>
       <c r="F7" t="s">
-        <v>113</v>
+        <v>135</v>
+      </c>
+      <c r="G7" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>114</v>
+        <v>137</v>
       </c>
       <c r="B8" t="s">
-        <v>115</v>
+        <v>138</v>
       </c>
       <c r="C8" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="D8" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="E8" t="s">
-        <v>118</v>
+        <v>141</v>
       </c>
       <c r="F8" t="s">
-        <v>119</v>
+        <v>142</v>
+      </c>
+      <c r="G8" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>120</v>
+        <v>144</v>
       </c>
       <c r="B9" t="s">
-        <v>121</v>
+        <v>145</v>
       </c>
       <c r="C9" t="s">
-        <v>122</v>
+        <v>146</v>
       </c>
       <c r="D9" t="s">
-        <v>123</v>
+        <v>147</v>
       </c>
       <c r="E9" t="s">
-        <v>124</v>
+        <v>148</v>
       </c>
       <c r="F9" t="s">
-        <v>125</v>
+        <v>149</v>
+      </c>
+      <c r="G9" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -2292,7 +2536,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2323,202 +2567,278 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>126</v>
+        <v>151</v>
       </c>
       <c r="C2" t="s">
-        <v>127</v>
+        <v>152</v>
       </c>
       <c r="D2" t="s">
-        <v>128</v>
+        <v>153</v>
       </c>
       <c r="E2" t="s">
-        <v>129</v>
+        <v>154</v>
       </c>
       <c r="F2" t="s">
-        <v>130</v>
+        <v>155</v>
+      </c>
+      <c r="G2" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>131</v>
+        <v>157</v>
       </c>
       <c r="C3" t="s">
-        <v>132</v>
+        <v>158</v>
       </c>
       <c r="D3" t="s">
-        <v>133</v>
+        <v>159</v>
       </c>
       <c r="E3" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="F3" t="s">
-        <v>135</v>
+        <v>161</v>
+      </c>
+      <c r="G3" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>136</v>
+        <v>163</v>
       </c>
       <c r="B4" t="s">
-        <v>137</v>
+        <v>164</v>
       </c>
       <c r="C4" t="s">
-        <v>138</v>
+        <v>165</v>
       </c>
       <c r="D4" t="s">
-        <v>139</v>
+        <v>166</v>
       </c>
       <c r="E4" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="F4" t="s">
-        <v>140</v>
+        <v>167</v>
+      </c>
+      <c r="G4" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>141</v>
+        <v>169</v>
       </c>
       <c r="B5" t="s">
-        <v>142</v>
+        <v>170</v>
       </c>
       <c r="C5" t="s">
-        <v>143</v>
+        <v>171</v>
       </c>
       <c r="D5" t="s">
-        <v>144</v>
+        <v>172</v>
       </c>
       <c r="E5" t="s">
-        <v>145</v>
+        <v>173</v>
       </c>
       <c r="F5" t="s">
-        <v>146</v>
+        <v>174</v>
+      </c>
+      <c r="G5" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>147</v>
+        <v>176</v>
       </c>
       <c r="B6" t="s">
-        <v>148</v>
+        <v>177</v>
       </c>
       <c r="C6" t="s">
-        <v>149</v>
+        <v>178</v>
       </c>
       <c r="D6" t="s">
-        <v>150</v>
+        <v>179</v>
       </c>
       <c r="E6" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="F6" t="s">
-        <v>151</v>
+        <v>180</v>
+      </c>
+      <c r="G6" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>152</v>
+        <v>182</v>
       </c>
       <c r="B7" t="s">
-        <v>153</v>
+        <v>183</v>
       </c>
       <c r="C7" t="s">
-        <v>154</v>
+        <v>184</v>
       </c>
       <c r="D7" t="s">
-        <v>155</v>
+        <v>185</v>
       </c>
       <c r="E7" t="s">
-        <v>156</v>
+        <v>186</v>
       </c>
       <c r="F7" t="s">
-        <v>157</v>
+        <v>187</v>
+      </c>
+      <c r="G7" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>158</v>
+        <v>189</v>
       </c>
       <c r="B8" t="s">
-        <v>159</v>
+        <v>190</v>
       </c>
       <c r="C8" t="s">
-        <v>160</v>
+        <v>191</v>
       </c>
       <c r="D8" t="s">
-        <v>161</v>
+        <v>192</v>
       </c>
       <c r="E8" t="s">
-        <v>162</v>
+        <v>193</v>
       </c>
       <c r="F8" t="s">
-        <v>163</v>
+        <v>194</v>
+      </c>
+      <c r="G8" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>164</v>
+        <v>196</v>
       </c>
       <c r="B9" t="s">
-        <v>165</v>
+        <v>197</v>
       </c>
       <c r="C9" t="s">
-        <v>166</v>
+        <v>198</v>
       </c>
       <c r="D9" t="s">
-        <v>167</v>
+        <v>199</v>
       </c>
       <c r="E9" t="s">
-        <v>168</v>
+        <v>200</v>
       </c>
       <c r="F9" t="s">
-        <v>169</v>
+        <v>201</v>
+      </c>
+      <c r="G9" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>170</v>
+        <v>203</v>
       </c>
       <c r="B10" t="s">
-        <v>171</v>
+        <v>204</v>
       </c>
       <c r="C10" t="s">
-        <v>172</v>
+        <v>205</v>
       </c>
       <c r="D10" t="s">
-        <v>173</v>
+        <v>206</v>
       </c>
       <c r="E10" t="s">
-        <v>174</v>
+        <v>207</v>
       </c>
       <c r="F10" t="s">
-        <v>175</v>
+        <v>208</v>
+      </c>
+      <c r="G10" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>176</v>
+        <v>210</v>
       </c>
       <c r="B11" t="s">
-        <v>177</v>
+        <v>211</v>
       </c>
       <c r="C11" t="s">
-        <v>178</v>
+        <v>212</v>
       </c>
       <c r="D11" t="s">
-        <v>179</v>
+        <v>213</v>
       </c>
       <c r="E11" t="s">
-        <v>180</v>
+        <v>214</v>
       </c>
       <c r="F11" t="s">
-        <v>181</v>
+        <v>215</v>
+      </c>
+      <c r="G11" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>217</v>
+      </c>
+      <c r="B12" t="s">
+        <v>218</v>
+      </c>
+      <c r="C12" t="s">
+        <v>219</v>
+      </c>
+      <c r="D12" t="s">
+        <v>220</v>
+      </c>
+      <c r="E12" t="s">
+        <v>160</v>
+      </c>
+      <c r="F12" t="s">
+        <v>221</v>
+      </c>
+      <c r="G12" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>223</v>
+      </c>
+      <c r="B13" t="s">
+        <v>224</v>
+      </c>
+      <c r="C13" t="s">
+        <v>225</v>
+      </c>
+      <c r="D13" t="s">
+        <v>226</v>
+      </c>
+      <c r="E13" t="s">
+        <v>160</v>
+      </c>
+      <c r="F13" t="s">
+        <v>227</v>
+      </c>
+      <c r="G13" t="s">
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -2559,462 +2879,531 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>182</v>
+        <v>229</v>
       </c>
       <c r="C2" t="s">
-        <v>183</v>
+        <v>230</v>
       </c>
       <c r="D2" t="s">
-        <v>184</v>
+        <v>231</v>
       </c>
       <c r="E2" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="F2" t="s">
-        <v>185</v>
+        <v>232</v>
+      </c>
+      <c r="G2" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>186</v>
+        <v>234</v>
       </c>
       <c r="C3" t="s">
-        <v>187</v>
+        <v>235</v>
       </c>
       <c r="D3" t="s">
-        <v>188</v>
+        <v>236</v>
       </c>
       <c r="E3" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="F3" t="s">
-        <v>189</v>
+        <v>237</v>
+      </c>
+      <c r="G3" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>190</v>
+        <v>239</v>
       </c>
       <c r="B4" t="s">
-        <v>191</v>
+        <v>240</v>
       </c>
       <c r="C4" t="s">
-        <v>192</v>
+        <v>241</v>
       </c>
       <c r="D4" t="s">
-        <v>193</v>
+        <v>242</v>
       </c>
       <c r="E4" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="F4" t="s">
-        <v>194</v>
+        <v>243</v>
+      </c>
+      <c r="G4" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>195</v>
+        <v>245</v>
       </c>
       <c r="B5" t="s">
-        <v>196</v>
+        <v>246</v>
       </c>
       <c r="C5" t="s">
-        <v>197</v>
+        <v>247</v>
       </c>
       <c r="D5" t="s">
-        <v>198</v>
+        <v>248</v>
       </c>
       <c r="E5" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="F5" t="s">
-        <v>199</v>
+        <v>249</v>
+      </c>
+      <c r="G5" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>200</v>
+        <v>251</v>
       </c>
       <c r="B6" t="s">
-        <v>201</v>
+        <v>252</v>
       </c>
       <c r="C6" t="s">
-        <v>202</v>
+        <v>253</v>
       </c>
       <c r="D6" t="s">
-        <v>203</v>
+        <v>254</v>
       </c>
       <c r="E6" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="F6" t="s">
-        <v>204</v>
+        <v>255</v>
+      </c>
+      <c r="G6" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>205</v>
+        <v>257</v>
       </c>
       <c r="B7" t="s">
-        <v>206</v>
+        <v>258</v>
       </c>
       <c r="C7" t="s">
-        <v>207</v>
+        <v>259</v>
       </c>
       <c r="D7" t="s">
-        <v>208</v>
+        <v>260</v>
       </c>
       <c r="E7" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="F7" t="s">
-        <v>209</v>
+        <v>261</v>
+      </c>
+      <c r="G7" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>210</v>
+        <v>263</v>
       </c>
       <c r="B8" t="s">
-        <v>211</v>
+        <v>264</v>
       </c>
       <c r="C8" t="s">
-        <v>212</v>
+        <v>265</v>
       </c>
       <c r="D8" t="s">
-        <v>213</v>
+        <v>266</v>
       </c>
       <c r="E8" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="F8" t="s">
-        <v>214</v>
+        <v>267</v>
+      </c>
+      <c r="G8" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>215</v>
+        <v>269</v>
       </c>
       <c r="B9" t="s">
-        <v>216</v>
+        <v>270</v>
       </c>
       <c r="C9" t="s">
-        <v>217</v>
+        <v>271</v>
       </c>
       <c r="D9" t="s">
-        <v>218</v>
+        <v>272</v>
       </c>
       <c r="E9" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="F9" t="s">
-        <v>219</v>
+        <v>273</v>
+      </c>
+      <c r="G9" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>220</v>
+        <v>275</v>
       </c>
       <c r="B10" t="s">
-        <v>221</v>
+        <v>276</v>
       </c>
       <c r="C10" t="s">
-        <v>143</v>
+        <v>171</v>
       </c>
       <c r="D10" t="s">
-        <v>222</v>
+        <v>277</v>
       </c>
       <c r="E10" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="F10" t="s">
-        <v>146</v>
+        <v>174</v>
+      </c>
+      <c r="G10" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>223</v>
+        <v>279</v>
       </c>
       <c r="B11" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="C11" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="D11" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="E11" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="F11" t="s">
-        <v>227</v>
+        <v>221</v>
+      </c>
+      <c r="G11" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
+        <v>280</v>
+      </c>
+      <c r="B12" t="s">
+        <v>224</v>
+      </c>
+      <c r="C12" t="s">
+        <v>225</v>
+      </c>
+      <c r="D12" t="s">
+        <v>226</v>
+      </c>
+      <c r="E12" t="s">
+        <v>160</v>
+      </c>
+      <c r="F12" t="s">
+        <v>227</v>
+      </c>
+      <c r="G12" t="s">
         <v>228</v>
-      </c>
-      <c r="B12" t="s">
-        <v>229</v>
-      </c>
-      <c r="C12" t="s">
-        <v>230</v>
-      </c>
-      <c r="D12" t="s">
-        <v>231</v>
-      </c>
-      <c r="E12" t="s">
-        <v>134</v>
-      </c>
-      <c r="F12" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>233</v>
+        <v>281</v>
       </c>
       <c r="B13" t="s">
-        <v>234</v>
+        <v>282</v>
       </c>
       <c r="C13" t="s">
-        <v>235</v>
+        <v>283</v>
       </c>
       <c r="D13" t="s">
-        <v>236</v>
+        <v>284</v>
       </c>
       <c r="E13" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="F13" t="s">
-        <v>237</v>
+        <v>285</v>
+      </c>
+      <c r="G13" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>238</v>
+        <v>287</v>
       </c>
       <c r="B14" t="s">
-        <v>239</v>
+        <v>288</v>
       </c>
       <c r="C14" t="s">
-        <v>240</v>
+        <v>289</v>
       </c>
       <c r="D14" t="s">
-        <v>241</v>
+        <v>290</v>
       </c>
       <c r="E14" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="F14" t="s">
-        <v>242</v>
+        <v>291</v>
+      </c>
+      <c r="G14" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>243</v>
+        <v>293</v>
       </c>
       <c r="B15" t="s">
-        <v>244</v>
+        <v>294</v>
       </c>
       <c r="C15" t="s">
-        <v>245</v>
+        <v>295</v>
       </c>
       <c r="D15" t="s">
-        <v>246</v>
+        <v>296</v>
       </c>
       <c r="E15" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="F15" t="s">
-        <v>247</v>
+        <v>297</v>
+      </c>
+      <c r="G15" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>248</v>
+        <v>299</v>
       </c>
       <c r="B16" t="s">
-        <v>249</v>
+        <v>300</v>
       </c>
       <c r="C16" t="s">
-        <v>250</v>
+        <v>301</v>
       </c>
       <c r="D16" t="s">
-        <v>251</v>
+        <v>302</v>
       </c>
       <c r="E16" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="F16" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+        <v>303</v>
+      </c>
+      <c r="G16" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>253</v>
+        <v>305</v>
       </c>
       <c r="B17" t="s">
-        <v>254</v>
+        <v>306</v>
       </c>
       <c r="C17" t="s">
-        <v>255</v>
+        <v>307</v>
       </c>
       <c r="D17" t="s">
-        <v>256</v>
+        <v>308</v>
       </c>
       <c r="E17" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="F17" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+        <v>309</v>
+      </c>
+      <c r="G17" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>258</v>
+        <v>311</v>
       </c>
       <c r="B18" t="s">
-        <v>259</v>
+        <v>312</v>
       </c>
       <c r="C18" t="s">
-        <v>260</v>
+        <v>313</v>
       </c>
       <c r="D18" t="s">
-        <v>261</v>
+        <v>314</v>
       </c>
       <c r="E18" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="F18" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+        <v>315</v>
+      </c>
+      <c r="G18" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>263</v>
+        <v>317</v>
       </c>
       <c r="B19" t="s">
-        <v>264</v>
+        <v>318</v>
       </c>
       <c r="C19" t="s">
-        <v>265</v>
+        <v>319</v>
       </c>
       <c r="D19" t="s">
-        <v>266</v>
+        <v>320</v>
       </c>
       <c r="E19" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="F19" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+        <v>321</v>
+      </c>
+      <c r="G19" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>268</v>
+        <v>323</v>
       </c>
       <c r="B20" t="s">
-        <v>269</v>
+        <v>324</v>
       </c>
       <c r="C20" t="s">
-        <v>270</v>
+        <v>325</v>
       </c>
       <c r="D20" t="s">
-        <v>271</v>
+        <v>326</v>
       </c>
       <c r="E20" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="F20" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+        <v>327</v>
+      </c>
+      <c r="G20" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>273</v>
+        <v>329</v>
       </c>
       <c r="B21" t="s">
-        <v>274</v>
+        <v>330</v>
       </c>
       <c r="C21" t="s">
-        <v>275</v>
+        <v>331</v>
       </c>
       <c r="D21" t="s">
-        <v>276</v>
+        <v>332</v>
       </c>
       <c r="E21" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="F21" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+        <v>333</v>
+      </c>
+      <c r="G21" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>278</v>
+        <v>335</v>
       </c>
       <c r="B22" t="s">
-        <v>279</v>
+        <v>336</v>
       </c>
       <c r="C22" t="s">
-        <v>280</v>
+        <v>337</v>
       </c>
       <c r="D22" t="s">
-        <v>281</v>
+        <v>338</v>
       </c>
       <c r="E22" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="F22" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+        <v>339</v>
+      </c>
+      <c r="G22" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>283</v>
+        <v>341</v>
       </c>
       <c r="B23" t="s">
-        <v>284</v>
+        <v>342</v>
       </c>
       <c r="C23" t="s">
-        <v>285</v>
+        <v>343</v>
       </c>
       <c r="D23" t="s">
-        <v>286</v>
+        <v>344</v>
       </c>
       <c r="E23" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="F23" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+        <v>345</v>
+      </c>
+      <c r="G23" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>288</v>
+        <v>347</v>
       </c>
       <c r="B24" t="s">
-        <v>289</v>
+        <v>348</v>
       </c>
       <c r="C24" t="s">
-        <v>290</v>
+        <v>349</v>
       </c>
       <c r="D24" t="s">
-        <v>291</v>
+        <v>350</v>
       </c>
       <c r="E24" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="F24" t="s">
-        <v>292</v>
+        <v>351</v>
+      </c>
+      <c r="G24" t="s">
+        <v>352</v>
       </c>
     </row>
   </sheetData>
@@ -3055,162 +3444,186 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>293</v>
+        <v>353</v>
       </c>
       <c r="C2" t="s">
-        <v>294</v>
+        <v>354</v>
       </c>
       <c r="D2" t="s">
-        <v>295</v>
+        <v>355</v>
       </c>
       <c r="E2" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="F2" t="s">
-        <v>296</v>
+        <v>356</v>
+      </c>
+      <c r="G2" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>297</v>
+        <v>358</v>
       </c>
       <c r="C3" t="s">
-        <v>298</v>
+        <v>359</v>
       </c>
       <c r="D3" t="s">
-        <v>299</v>
+        <v>360</v>
       </c>
       <c r="E3" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="F3" t="s">
-        <v>300</v>
+        <v>361</v>
+      </c>
+      <c r="G3" t="s">
+        <v>362</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>190</v>
+        <v>239</v>
       </c>
       <c r="B4" t="s">
-        <v>191</v>
+        <v>240</v>
       </c>
       <c r="C4" t="s">
-        <v>192</v>
+        <v>241</v>
       </c>
       <c r="D4" t="s">
-        <v>193</v>
+        <v>242</v>
       </c>
       <c r="E4" t="s">
-        <v>301</v>
+        <v>363</v>
       </c>
       <c r="F4" t="s">
-        <v>302</v>
+        <v>364</v>
+      </c>
+      <c r="G4" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>195</v>
+        <v>245</v>
       </c>
       <c r="B5" t="s">
-        <v>196</v>
+        <v>246</v>
       </c>
       <c r="C5" t="s">
-        <v>197</v>
+        <v>247</v>
       </c>
       <c r="D5" t="s">
-        <v>198</v>
+        <v>248</v>
       </c>
       <c r="E5" t="s">
-        <v>303</v>
+        <v>365</v>
       </c>
       <c r="F5" t="s">
-        <v>199</v>
+        <v>249</v>
+      </c>
+      <c r="G5" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>200</v>
+        <v>251</v>
       </c>
       <c r="B6" t="s">
-        <v>201</v>
+        <v>252</v>
       </c>
       <c r="C6" t="s">
-        <v>202</v>
+        <v>253</v>
       </c>
       <c r="D6" t="s">
-        <v>203</v>
+        <v>254</v>
       </c>
       <c r="E6" t="s">
-        <v>304</v>
+        <v>366</v>
       </c>
       <c r="F6" t="s">
-        <v>305</v>
+        <v>367</v>
+      </c>
+      <c r="G6" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>205</v>
+        <v>257</v>
       </c>
       <c r="B7" t="s">
-        <v>206</v>
+        <v>258</v>
       </c>
       <c r="C7" t="s">
-        <v>207</v>
+        <v>259</v>
       </c>
       <c r="D7" t="s">
-        <v>208</v>
+        <v>260</v>
       </c>
       <c r="E7" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="F7" t="s">
-        <v>306</v>
+        <v>369</v>
+      </c>
+      <c r="G7" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>307</v>
+        <v>371</v>
       </c>
       <c r="B8" t="s">
-        <v>308</v>
+        <v>372</v>
       </c>
       <c r="C8" t="s">
-        <v>309</v>
+        <v>373</v>
       </c>
       <c r="D8" t="s">
-        <v>310</v>
+        <v>374</v>
       </c>
       <c r="E8" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="F8" t="s">
-        <v>311</v>
+        <v>375</v>
+      </c>
+      <c r="G8" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>312</v>
+        <v>377</v>
       </c>
       <c r="B9" t="s">
-        <v>313</v>
+        <v>378</v>
       </c>
       <c r="C9" t="s">
-        <v>314</v>
+        <v>379</v>
       </c>
       <c r="D9" t="s">
-        <v>315</v>
+        <v>380</v>
       </c>
       <c r="E9" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="F9" t="s">
-        <v>316</v>
+        <v>381</v>
+      </c>
+      <c r="G9" t="s">
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -3220,7 +3633,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3251,262 +3664,140 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>317</v>
+        <v>383</v>
       </c>
       <c r="C2" t="s">
-        <v>318</v>
+        <v>384</v>
       </c>
       <c r="D2" t="s">
-        <v>319</v>
+        <v>385</v>
       </c>
       <c r="E2" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="F2" t="s">
-        <v>320</v>
+        <v>386</v>
+      </c>
+      <c r="G2" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>321</v>
+        <v>388</v>
       </c>
       <c r="C3" t="s">
-        <v>322</v>
+        <v>389</v>
       </c>
       <c r="D3" t="s">
-        <v>323</v>
+        <v>390</v>
       </c>
       <c r="E3" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="F3" t="s">
-        <v>324</v>
+        <v>391</v>
+      </c>
+      <c r="G3" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>325</v>
+        <v>393</v>
       </c>
       <c r="B4" t="s">
-        <v>326</v>
+        <v>394</v>
       </c>
       <c r="C4" t="s">
-        <v>327</v>
+        <v>395</v>
       </c>
       <c r="D4" t="s">
-        <v>328</v>
+        <v>396</v>
       </c>
       <c r="E4" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="F4" t="s">
-        <v>329</v>
+        <v>397</v>
+      </c>
+      <c r="G4" t="s">
+        <v>398</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>330</v>
+        <v>399</v>
       </c>
       <c r="B5" t="s">
-        <v>331</v>
+        <v>400</v>
       </c>
       <c r="C5" t="s">
-        <v>332</v>
+        <v>401</v>
       </c>
       <c r="D5" t="s">
-        <v>333</v>
+        <v>402</v>
       </c>
       <c r="E5" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="F5" t="s">
-        <v>334</v>
+        <v>403</v>
+      </c>
+      <c r="G5" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>335</v>
+        <v>405</v>
       </c>
       <c r="B6" t="s">
-        <v>336</v>
+        <v>406</v>
       </c>
       <c r="C6" t="s">
-        <v>337</v>
+        <v>407</v>
       </c>
       <c r="D6" t="s">
-        <v>338</v>
+        <v>160</v>
       </c>
       <c r="E6" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="F6" t="s">
-        <v>339</v>
+        <v>408</v>
+      </c>
+      <c r="G6" t="s">
+        <v>409</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>340</v>
+        <v>410</v>
       </c>
       <c r="B7" t="s">
-        <v>341</v>
+        <v>411</v>
       </c>
       <c r="C7" t="s">
-        <v>342</v>
+        <v>412</v>
       </c>
       <c r="D7" t="s">
-        <v>343</v>
+        <v>160</v>
       </c>
       <c r="E7" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="F7" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" t="s">
-        <v>345</v>
-      </c>
-      <c r="B8" t="s">
-        <v>346</v>
-      </c>
-      <c r="C8" t="s">
-        <v>347</v>
-      </c>
-      <c r="D8" t="s">
-        <v>348</v>
-      </c>
-      <c r="E8" t="s">
-        <v>134</v>
-      </c>
-      <c r="F8" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" t="s">
-        <v>350</v>
-      </c>
-      <c r="B9" t="s">
-        <v>351</v>
-      </c>
-      <c r="C9" t="s">
-        <v>352</v>
-      </c>
-      <c r="D9" t="s">
-        <v>353</v>
-      </c>
-      <c r="E9" t="s">
-        <v>134</v>
-      </c>
-      <c r="F9" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" t="s">
-        <v>355</v>
-      </c>
-      <c r="B10" t="s">
-        <v>356</v>
-      </c>
-      <c r="C10" t="s">
-        <v>357</v>
-      </c>
-      <c r="D10" t="s">
-        <v>358</v>
-      </c>
-      <c r="E10" t="s">
-        <v>134</v>
-      </c>
-      <c r="F10" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" t="s">
-        <v>360</v>
-      </c>
-      <c r="B11" t="s">
-        <v>361</v>
-      </c>
-      <c r="C11" t="s">
-        <v>362</v>
-      </c>
-      <c r="D11" t="s">
-        <v>363</v>
-      </c>
-      <c r="E11" t="s">
-        <v>134</v>
-      </c>
-      <c r="F11" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" t="s">
-        <v>365</v>
-      </c>
-      <c r="B12" t="s">
-        <v>366</v>
-      </c>
-      <c r="C12" t="s">
-        <v>367</v>
-      </c>
-      <c r="D12" t="s">
-        <v>368</v>
-      </c>
-      <c r="E12" t="s">
-        <v>134</v>
-      </c>
-      <c r="F12" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" t="s">
-        <v>370</v>
-      </c>
-      <c r="B13" t="s">
-        <v>371</v>
-      </c>
-      <c r="C13" t="s">
-        <v>372</v>
-      </c>
-      <c r="D13" t="s">
-        <v>134</v>
-      </c>
-      <c r="E13" t="s">
-        <v>134</v>
-      </c>
-      <c r="F13" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" t="s">
-        <v>374</v>
-      </c>
-      <c r="B14" t="s">
-        <v>375</v>
-      </c>
-      <c r="C14" t="s">
-        <v>376</v>
-      </c>
-      <c r="D14" t="s">
-        <v>134</v>
-      </c>
-      <c r="E14" t="s">
-        <v>134</v>
-      </c>
-      <c r="F14" t="s">
-        <v>375</v>
+        <v>411</v>
+      </c>
+      <c r="G7" t="s">
+        <v>413</v>
       </c>
     </row>
   </sheetData>
@@ -3547,82 +3838,94 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>377</v>
+        <v>414</v>
       </c>
       <c r="C2" t="s">
-        <v>378</v>
+        <v>415</v>
       </c>
       <c r="D2" t="s">
-        <v>379</v>
+        <v>416</v>
       </c>
       <c r="E2" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="F2" t="s">
-        <v>380</v>
+        <v>417</v>
+      </c>
+      <c r="G2" t="s">
+        <v>418</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>381</v>
+        <v>419</v>
       </c>
       <c r="C3" t="s">
-        <v>382</v>
+        <v>420</v>
       </c>
       <c r="D3" t="s">
-        <v>383</v>
+        <v>421</v>
       </c>
       <c r="E3" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="F3" t="s">
-        <v>384</v>
+        <v>422</v>
+      </c>
+      <c r="G3" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>385</v>
+        <v>424</v>
       </c>
       <c r="B4" t="s">
-        <v>386</v>
+        <v>425</v>
       </c>
       <c r="C4" t="s">
-        <v>387</v>
+        <v>426</v>
       </c>
       <c r="D4" t="s">
-        <v>388</v>
+        <v>427</v>
       </c>
       <c r="E4" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="F4" t="s">
-        <v>389</v>
+        <v>428</v>
+      </c>
+      <c r="G4" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>390</v>
+        <v>430</v>
       </c>
       <c r="B5" t="s">
-        <v>391</v>
+        <v>431</v>
       </c>
       <c r="C5" t="s">
-        <v>392</v>
+        <v>432</v>
       </c>
       <c r="D5" t="s">
-        <v>393</v>
+        <v>433</v>
       </c>
       <c r="E5" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="F5" t="s">
-        <v>394</v>
+        <v>434</v>
+      </c>
+      <c r="G5" t="s">
+        <v>435</v>
       </c>
     </row>
   </sheetData>
@@ -3663,122 +3966,140 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>395</v>
+        <v>436</v>
       </c>
       <c r="C2" t="s">
-        <v>396</v>
+        <v>437</v>
       </c>
       <c r="D2" t="s">
-        <v>397</v>
+        <v>438</v>
       </c>
       <c r="E2" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="F2" t="s">
-        <v>398</v>
+        <v>439</v>
+      </c>
+      <c r="G2" t="s">
+        <v>440</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>399</v>
+        <v>441</v>
       </c>
       <c r="C3" t="s">
-        <v>400</v>
+        <v>442</v>
       </c>
       <c r="D3" t="s">
-        <v>401</v>
+        <v>443</v>
       </c>
       <c r="E3" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="F3" t="s">
-        <v>402</v>
+        <v>444</v>
+      </c>
+      <c r="G3" t="s">
+        <v>445</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>385</v>
+        <v>424</v>
       </c>
       <c r="B4" t="s">
-        <v>403</v>
+        <v>446</v>
       </c>
       <c r="C4" t="s">
-        <v>404</v>
+        <v>447</v>
       </c>
       <c r="D4" t="s">
-        <v>405</v>
+        <v>448</v>
       </c>
       <c r="E4" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="F4" t="s">
-        <v>389</v>
+        <v>428</v>
+      </c>
+      <c r="G4" t="s">
+        <v>449</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>390</v>
+        <v>430</v>
       </c>
       <c r="B5" t="s">
-        <v>406</v>
+        <v>450</v>
       </c>
       <c r="C5" t="s">
-        <v>407</v>
+        <v>451</v>
       </c>
       <c r="D5" t="s">
-        <v>408</v>
+        <v>452</v>
       </c>
       <c r="E5" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="F5" t="s">
-        <v>394</v>
+        <v>434</v>
+      </c>
+      <c r="G5" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>409</v>
+        <v>454</v>
       </c>
       <c r="B6" t="s">
-        <v>410</v>
+        <v>455</v>
       </c>
       <c r="C6" t="s">
-        <v>411</v>
+        <v>456</v>
       </c>
       <c r="D6" t="s">
-        <v>412</v>
+        <v>457</v>
       </c>
       <c r="E6" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="F6" t="s">
-        <v>413</v>
+        <v>458</v>
+      </c>
+      <c r="G6" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>414</v>
+        <v>460</v>
       </c>
       <c r="B7" t="s">
-        <v>415</v>
+        <v>461</v>
       </c>
       <c r="C7" t="s">
-        <v>416</v>
+        <v>462</v>
       </c>
       <c r="D7" t="s">
-        <v>417</v>
+        <v>463</v>
       </c>
       <c r="E7" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="F7" t="s">
-        <v>418</v>
+        <v>464</v>
+      </c>
+      <c r="G7" t="s">
+        <v>465</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Simplified Chinese language support
</commit_message>
<xml_diff>
--- a/AdofaiTweaks.Generator/translations.xlsx
+++ b/AdofaiTweaks.Generator/translations.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="583">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="588">
   <si>
     <t>KEY</t>
   </si>
@@ -1717,22 +1717,19 @@
     <t>限制判定</t>
   </si>
   <si>
-    <t>Kills the player on certain judgments.</t>
-  </si>
-  <si>
-    <t>특정 판정에서 플레이어를 죽입니다.</t>
-  </si>
-  <si>
-    <t>Mata al jugador en si hace un juicio específico.</t>
-  </si>
-  <si>
-    <t>Tue le joueur dans certain jugements.</t>
-  </si>
-  <si>
-    <t>Làm bạn thua khi phạm lỗi sai nhất định.</t>
-  </si>
-  <si>
-    <t>根据某些判定结束游戏</t>
+    <t>Punishes player upon specified judgments.</t>
+  </si>
+  <si>
+    <t>특정 판정에서 플레이어를 제한합니다.</t>
+  </si>
+  <si>
+    <t>RESTRICT_HEADER</t>
+  </si>
+  <si>
+    <t>Restrict following judgments:</t>
+  </si>
+  <si>
+    <t>제한할 판정 목록:</t>
   </si>
   <si>
     <t>RESTRICT</t>
@@ -1751,6 +1748,24 @@
   </si>
   <si>
     <t>Giới hạn lỗi: "{0}"</t>
+  </si>
+  <si>
+    <t>CUSTOM_HEADER</t>
+  </si>
+  <si>
+    <t>Restrict Action:</t>
+  </si>
+  <si>
+    <t>플레이어 제한 행동:</t>
+  </si>
+  <si>
+    <t>RESTRICT_ACTION</t>
+  </si>
+  <si>
+    <t>Restriction Method:</t>
+  </si>
+  <si>
+    <t>제한 방식:</t>
   </si>
   <si>
     <t>CUSTOM_DEATH</t>
@@ -2220,7 +2235,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2288,72 +2303,90 @@
       <c r="C3" t="s">
         <v>565</v>
       </c>
-      <c r="D3" t="s">
-        <v>566</v>
-      </c>
-      <c r="E3" t="s">
-        <v>108</v>
-      </c>
-      <c r="F3" t="s">
-        <v>567</v>
-      </c>
-      <c r="G3" t="s">
-        <v>568</v>
-      </c>
-      <c r="H3" t="s">
-        <v>569</v>
-      </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="B4" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="C4" t="s">
-        <v>572</v>
-      </c>
-      <c r="D4" t="s">
-        <v>573</v>
-      </c>
-      <c r="E4" t="s">
-        <v>108</v>
-      </c>
-      <c r="F4" t="s">
-        <v>574</v>
-      </c>
-      <c r="G4" t="s">
-        <v>575</v>
-      </c>
-      <c r="H4" t="s">
-        <v>563</v>
+        <v>568</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
+        <v>569</v>
+      </c>
+      <c r="B5" t="s">
+        <v>570</v>
+      </c>
+      <c r="C5" t="s">
+        <v>571</v>
+      </c>
+      <c r="D5" t="s">
+        <v>572</v>
+      </c>
+      <c r="E5" t="s">
+        <v>108</v>
+      </c>
+      <c r="F5" t="s">
+        <v>573</v>
+      </c>
+      <c r="G5" t="s">
+        <v>574</v>
+      </c>
+      <c r="H5" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>575</v>
+      </c>
+      <c r="B6" t="s">
         <v>576</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C6" t="s">
         <v>577</v>
       </c>
-      <c r="C5" t="s">
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
         <v>578</v>
       </c>
-      <c r="D5" t="s">
+      <c r="B7" t="s">
         <v>579</v>
       </c>
-      <c r="E5" t="s">
-        <v>108</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="C7" t="s">
         <v>580</v>
       </c>
-      <c r="G5" t="s">
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
         <v>581</v>
       </c>
-      <c r="H5" t="s">
+      <c r="B8" t="s">
         <v>582</v>
+      </c>
+      <c r="C8" t="s">
+        <v>583</v>
+      </c>
+      <c r="D8" t="s">
+        <v>584</v>
+      </c>
+      <c r="E8" t="s">
+        <v>108</v>
+      </c>
+      <c r="F8" t="s">
+        <v>585</v>
+      </c>
+      <c r="G8" t="s">
+        <v>586</v>
+      </c>
+      <c r="H8" t="s">
+        <v>587</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix multiplanet coloring, add planet toggle
</commit_message>
<xml_diff>
--- a/AdofaiTweaks.Generator/translations.xlsx
+++ b/AdofaiTweaks.Generator/translations.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="726">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="728">
   <si>
     <t>Translation Status</t>
   </si>
@@ -1913,31 +1913,37 @@
     <t>Stellt die Farbe der Planeten ein</t>
   </si>
   <si>
-    <t>Planet 1:</t>
-  </si>
-  <si>
-    <t>행성 1:</t>
-  </si>
-  <si>
-    <t>Planeta 1:</t>
-  </si>
-  <si>
-    <t>Hành tinh thứ nhất:</t>
+    <t>Planet 1</t>
+  </si>
+  <si>
+    <t>행성 1</t>
+  </si>
+  <si>
+    <t>Planeta 1</t>
+  </si>
+  <si>
+    <t>Planète 1</t>
+  </si>
+  <si>
+    <t>Hành tinh thứ nhất</t>
   </si>
   <si>
     <t>第一个球</t>
   </si>
   <si>
-    <t>Planet 2:</t>
-  </si>
-  <si>
-    <t>행성 2:</t>
-  </si>
-  <si>
-    <t>Planeta 2:</t>
-  </si>
-  <si>
-    <t>Hành tinh thứ hai:</t>
+    <t>Planet 2</t>
+  </si>
+  <si>
+    <t>행성 2</t>
+  </si>
+  <si>
+    <t>Planeta 2</t>
+  </si>
+  <si>
+    <t>Planète 2</t>
+  </si>
+  <si>
+    <t>Hành tinh thứ hai</t>
   </si>
   <si>
     <t>第二个球</t>
@@ -2951,13 +2957,13 @@
         <v>154</v>
       </c>
       <c r="F4" t="s">
-        <v>545</v>
+        <v>632</v>
       </c>
       <c r="G4" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="H4" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="I4" t="s">
         <v>629</v>
@@ -2968,86 +2974,86 @@
         <v>549</v>
       </c>
       <c r="B5" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="C5" t="s">
+        <v>636</v>
+      </c>
+      <c r="D5" t="s">
+        <v>637</v>
+      </c>
+      <c r="E5" t="s">
+        <v>154</v>
+      </c>
+      <c r="F5" t="s">
+        <v>638</v>
+      </c>
+      <c r="G5" t="s">
+        <v>639</v>
+      </c>
+      <c r="H5" t="s">
+        <v>640</v>
+      </c>
+      <c r="I5" t="s">
         <v>635</v>
-      </c>
-      <c r="D5" t="s">
-        <v>636</v>
-      </c>
-      <c r="E5" t="s">
-        <v>154</v>
-      </c>
-      <c r="F5" t="s">
-        <v>553</v>
-      </c>
-      <c r="G5" t="s">
-        <v>637</v>
-      </c>
-      <c r="H5" t="s">
-        <v>638</v>
-      </c>
-      <c r="I5" t="s">
-        <v>634</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>639</v>
+        <v>641</v>
       </c>
       <c r="B6" t="s">
-        <v>640</v>
+        <v>642</v>
       </c>
       <c r="C6" t="s">
-        <v>641</v>
+        <v>643</v>
       </c>
       <c r="D6" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="E6" t="s">
         <v>154</v>
       </c>
       <c r="F6" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="G6" t="s">
-        <v>644</v>
+        <v>646</v>
       </c>
       <c r="H6" t="s">
-        <v>645</v>
+        <v>647</v>
       </c>
       <c r="I6" t="s">
-        <v>646</v>
+        <v>648</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>647</v>
+        <v>649</v>
       </c>
       <c r="B7" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="C7" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="D7" t="s">
-        <v>650</v>
+        <v>652</v>
       </c>
       <c r="E7" t="s">
         <v>154</v>
       </c>
       <c r="F7" t="s">
-        <v>651</v>
+        <v>653</v>
       </c>
       <c r="G7" t="s">
-        <v>652</v>
+        <v>654</v>
       </c>
       <c r="H7" t="s">
-        <v>653</v>
+        <v>655</v>
       </c>
       <c r="I7" t="s">
-        <v>654</v>
+        <v>656</v>
       </c>
     </row>
   </sheetData>
@@ -3097,28 +3103,28 @@
         <v>69</v>
       </c>
       <c r="B2" t="s">
-        <v>655</v>
+        <v>657</v>
       </c>
       <c r="C2" t="s">
-        <v>656</v>
+        <v>658</v>
       </c>
       <c r="D2" t="s">
-        <v>657</v>
+        <v>659</v>
       </c>
       <c r="E2" t="s">
         <v>154</v>
       </c>
       <c r="F2" t="s">
-        <v>658</v>
+        <v>660</v>
       </c>
       <c r="G2" t="s">
-        <v>659</v>
+        <v>661</v>
       </c>
       <c r="H2" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
       <c r="I2" t="s">
-        <v>661</v>
+        <v>663</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -3126,257 +3132,257 @@
         <v>78</v>
       </c>
       <c r="B3" t="s">
-        <v>662</v>
+        <v>664</v>
       </c>
       <c r="C3" t="s">
-        <v>663</v>
+        <v>665</v>
       </c>
       <c r="D3" t="s">
-        <v>664</v>
+        <v>666</v>
       </c>
       <c r="E3" t="s">
         <v>154</v>
       </c>
       <c r="F3" t="s">
-        <v>665</v>
+        <v>667</v>
       </c>
       <c r="G3" t="s">
         <v>154</v>
       </c>
       <c r="H3" t="s">
-        <v>666</v>
+        <v>668</v>
       </c>
       <c r="I3" t="s">
-        <v>667</v>
+        <v>669</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>668</v>
+        <v>670</v>
       </c>
       <c r="B4" t="s">
-        <v>669</v>
+        <v>671</v>
       </c>
       <c r="C4" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
       <c r="D4" t="s">
-        <v>671</v>
+        <v>673</v>
       </c>
       <c r="E4" t="s">
         <v>154</v>
       </c>
       <c r="F4" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
       <c r="G4" t="s">
         <v>154</v>
       </c>
       <c r="H4" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="I4" t="s">
-        <v>674</v>
+        <v>676</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>675</v>
+        <v>677</v>
       </c>
       <c r="B5" t="s">
-        <v>676</v>
+        <v>678</v>
       </c>
       <c r="C5" t="s">
-        <v>677</v>
+        <v>679</v>
       </c>
       <c r="D5" t="s">
-        <v>678</v>
+        <v>680</v>
       </c>
       <c r="E5" t="s">
         <v>154</v>
       </c>
       <c r="F5" t="s">
-        <v>679</v>
+        <v>681</v>
       </c>
       <c r="G5" t="s">
-        <v>680</v>
+        <v>682</v>
       </c>
       <c r="H5" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="I5" t="s">
-        <v>682</v>
+        <v>684</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>683</v>
+        <v>685</v>
       </c>
       <c r="B6" t="s">
-        <v>684</v>
+        <v>686</v>
       </c>
       <c r="C6" t="s">
-        <v>685</v>
+        <v>687</v>
       </c>
       <c r="D6" t="s">
-        <v>686</v>
+        <v>688</v>
       </c>
       <c r="E6" t="s">
         <v>154</v>
       </c>
       <c r="F6" t="s">
-        <v>687</v>
+        <v>689</v>
       </c>
       <c r="G6" t="s">
         <v>154</v>
       </c>
       <c r="H6" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
       <c r="I6" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
       <c r="B7" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="C7" t="s">
-        <v>692</v>
+        <v>694</v>
       </c>
       <c r="D7" t="s">
-        <v>693</v>
+        <v>695</v>
       </c>
       <c r="E7" t="s">
         <v>154</v>
       </c>
       <c r="F7" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
       <c r="G7" t="s">
         <v>154</v>
       </c>
       <c r="H7" t="s">
-        <v>695</v>
+        <v>697</v>
       </c>
       <c r="I7" t="s">
-        <v>696</v>
+        <v>698</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>697</v>
+        <v>699</v>
       </c>
       <c r="B8" t="s">
-        <v>698</v>
+        <v>700</v>
       </c>
       <c r="C8" t="s">
-        <v>699</v>
+        <v>701</v>
       </c>
       <c r="D8" t="s">
-        <v>700</v>
+        <v>702</v>
       </c>
       <c r="E8" t="s">
         <v>154</v>
       </c>
       <c r="F8" t="s">
-        <v>701</v>
+        <v>703</v>
       </c>
       <c r="G8" t="s">
         <v>154</v>
       </c>
       <c r="H8" t="s">
-        <v>702</v>
+        <v>704</v>
       </c>
       <c r="I8" t="s">
-        <v>703</v>
+        <v>705</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>704</v>
+        <v>706</v>
       </c>
       <c r="B9" t="s">
-        <v>705</v>
+        <v>707</v>
       </c>
       <c r="C9" t="s">
-        <v>706</v>
+        <v>708</v>
       </c>
       <c r="D9" t="s">
-        <v>707</v>
+        <v>709</v>
       </c>
       <c r="E9" t="s">
         <v>154</v>
       </c>
       <c r="F9" t="s">
-        <v>708</v>
+        <v>710</v>
       </c>
       <c r="G9" t="s">
         <v>154</v>
       </c>
       <c r="H9" t="s">
-        <v>709</v>
+        <v>711</v>
       </c>
       <c r="I9" t="s">
-        <v>710</v>
+        <v>712</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>711</v>
+        <v>713</v>
       </c>
       <c r="B10" t="s">
-        <v>712</v>
+        <v>714</v>
       </c>
       <c r="C10" t="s">
-        <v>713</v>
+        <v>715</v>
       </c>
       <c r="D10" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
       <c r="E10" t="s">
-        <v>715</v>
+        <v>717</v>
       </c>
       <c r="F10" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="G10" t="s">
         <v>154</v>
       </c>
       <c r="H10" t="s">
-        <v>717</v>
+        <v>719</v>
       </c>
       <c r="I10" t="s">
-        <v>718</v>
+        <v>720</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>719</v>
+        <v>721</v>
       </c>
       <c r="B11" t="s">
-        <v>720</v>
+        <v>722</v>
       </c>
       <c r="C11" t="s">
-        <v>721</v>
+        <v>723</v>
       </c>
       <c r="D11" t="s">
-        <v>722</v>
+        <v>724</v>
       </c>
       <c r="E11" t="s">
         <v>154</v>
       </c>
       <c r="F11" t="s">
-        <v>723</v>
+        <v>725</v>
       </c>
       <c r="G11" t="s">
-        <v>724</v>
+        <v>726</v>
       </c>
       <c r="H11" t="s">
-        <v>725</v>
+        <v>727</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update translations + fix strings DLL reference
</commit_message>
<xml_diff>
--- a/AdofaiTweaks.Generator/translations.xlsx
+++ b/AdofaiTweaks.Generator/translations.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="723">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1072" uniqueCount="746">
   <si>
     <t>Translation Status</t>
   </si>
@@ -62,6 +62,9 @@
     <t>100% (0 left)</t>
   </si>
   <si>
+    <t>66.7% (2 left)</t>
+  </si>
+  <si>
     <t>DisableEffects</t>
   </si>
   <si>
@@ -71,6 +74,9 @@
     <t>HideUiElements</t>
   </si>
   <si>
+    <t>57.1% (6 left)</t>
+  </si>
+  <si>
     <t>JudgmentVisuals</t>
   </si>
   <si>
@@ -236,6 +242,24 @@
     <t>Deutsch</t>
   </si>
   <si>
+    <t>SHORTCUT_CHANGE_KEY</t>
+  </si>
+  <si>
+    <t>Change Key</t>
+  </si>
+  <si>
+    <t>키 변경하기</t>
+  </si>
+  <si>
+    <t>SHORTCUT_DONE</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>완료</t>
+  </si>
+  <si>
     <t>NAME</t>
   </si>
   <si>
@@ -734,10 +758,64 @@
     <t>Verberge den "Beta Build" Text</t>
   </si>
   <si>
+    <t>RESULT_TEXT</t>
+  </si>
+  <si>
+    <t>Hide "Congratulations!" &amp; detailed results text</t>
+  </si>
+  <si>
+    <t>"축하합니다!" 및 상세한 결과 텍스트 숨기기</t>
+  </si>
+  <si>
+    <t>HIT_ERROR_METER</t>
+  </si>
+  <si>
+    <t>Hide hit error meter</t>
+  </si>
+  <si>
+    <t>입력 계기판 숨기기</t>
+  </si>
+  <si>
+    <t>LAST_FLOOR_FLASH</t>
+  </si>
+  <si>
+    <t>Hide the white flash on landing last tile</t>
+  </si>
+  <si>
+    <t>마지막 타일을 밟을 때 흰색 플래시 숨기기</t>
+  </si>
+  <si>
+    <t>RECORDING_MODE</t>
+  </si>
+  <si>
+    <t>Recording mode</t>
+  </si>
+  <si>
+    <t>녹화 모드</t>
+  </si>
+  <si>
+    <t>USE_RECORDING_MODE_SHORTCUT</t>
+  </si>
+  <si>
+    <t>Use recording mode toggle shortcut</t>
+  </si>
+  <si>
+    <t>녹화 모드 토글 단축키 사용하기</t>
+  </si>
+  <si>
+    <t>RECORDING_MODE_SHORTCUT</t>
+  </si>
+  <si>
+    <t>Recording mode toggle shortcut:</t>
+  </si>
+  <si>
+    <t>녹화 모드 토글 단축키</t>
+  </si>
+  <si>
     <t>Judgment Visuals</t>
   </si>
   <si>
-    <t>판정선</t>
+    <t>판정 표기</t>
   </si>
   <si>
     <t>Visualización de los juicios</t>
@@ -758,7 +836,7 @@
     <t>Improves the visuals of judgments.</t>
   </si>
   <si>
-    <t>게임 UI에 판정선을 추가합니다.</t>
+    <t>판정 표기를 개선합니다.</t>
   </si>
   <si>
     <t>Mejora los visuales de los juicios.</t>
@@ -779,7 +857,7 @@
     <t>Show hit error meter</t>
   </si>
   <si>
-    <t>판정선 표시하기</t>
+    <t>입력 계기판 표시하기</t>
   </si>
   <si>
     <t>Mostrar barra de errores</t>
@@ -1091,12 +1169,6 @@
     <t>DONE</t>
   </si>
   <si>
-    <t>Done</t>
-  </si>
-  <si>
-    <t>완료</t>
-  </si>
-  <si>
     <t>Hecho</t>
   </si>
   <si>
@@ -1140,9 +1212,6 @@
   </si>
   <si>
     <t>Change Keys</t>
-  </si>
-  <si>
-    <t>키 변경하기</t>
   </si>
   <si>
     <t>Cambiar teclas</t>
@@ -2575,27 +2644,27 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -2607,13 +2676,13 @@
         <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F4" t="s">
         <v>11</v>
       </c>
       <c r="G4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H4" t="s">
         <v>11</v>
@@ -2624,7 +2693,7 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -2633,27 +2702,27 @@
         <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="G5" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="H5" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="I5" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -2665,7 +2734,7 @@
         <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F6" t="s">
         <v>11</v>
@@ -2677,12 +2746,12 @@
         <v>11</v>
       </c>
       <c r="I6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -2694,24 +2763,24 @@
         <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F7" t="s">
         <v>11</v>
       </c>
       <c r="G7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H7" t="s">
         <v>11</v>
       </c>
       <c r="I7" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
@@ -2723,24 +2792,24 @@
         <v>11</v>
       </c>
       <c r="E8" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F8" t="s">
         <v>11</v>
       </c>
       <c r="G8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -2752,13 +2821,13 @@
         <v>11</v>
       </c>
       <c r="E9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F9" t="s">
         <v>11</v>
       </c>
       <c r="G9" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H9" t="s">
         <v>11</v>
@@ -2769,7 +2838,7 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -2781,7 +2850,7 @@
         <v>11</v>
       </c>
       <c r="E10" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F10" t="s">
         <v>11</v>
@@ -2798,7 +2867,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -2810,19 +2879,19 @@
         <v>11</v>
       </c>
       <c r="E11" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F11" t="s">
         <v>11</v>
       </c>
       <c r="G11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H11" t="s">
         <v>11</v>
       </c>
       <c r="I11" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -2840,225 +2909,225 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
-        <v>633</v>
+        <v>656</v>
       </c>
       <c r="C2" t="s">
-        <v>634</v>
+        <v>657</v>
       </c>
       <c r="D2" t="s">
-        <v>635</v>
+        <v>658</v>
       </c>
       <c r="E2" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F2" t="s">
-        <v>636</v>
+        <v>659</v>
       </c>
       <c r="G2" t="s">
-        <v>637</v>
+        <v>660</v>
       </c>
       <c r="H2" t="s">
-        <v>638</v>
+        <v>661</v>
       </c>
       <c r="I2" t="s">
-        <v>639</v>
+        <v>662</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="B3" t="s">
-        <v>640</v>
+        <v>663</v>
       </c>
       <c r="C3" t="s">
-        <v>641</v>
+        <v>664</v>
       </c>
       <c r="D3" t="s">
-        <v>642</v>
+        <v>665</v>
       </c>
       <c r="E3" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F3" t="s">
-        <v>643</v>
+        <v>666</v>
       </c>
       <c r="G3" t="s">
-        <v>644</v>
+        <v>667</v>
       </c>
       <c r="H3" t="s">
-        <v>645</v>
+        <v>668</v>
       </c>
       <c r="I3" t="s">
-        <v>646</v>
+        <v>669</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>603</v>
+        <v>626</v>
       </c>
       <c r="B4" t="s">
-        <v>604</v>
+        <v>627</v>
       </c>
       <c r="C4" t="s">
-        <v>605</v>
+        <v>628</v>
       </c>
       <c r="D4" t="s">
-        <v>606</v>
+        <v>629</v>
       </c>
       <c r="E4" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F4" t="s">
-        <v>607</v>
+        <v>630</v>
       </c>
       <c r="G4" t="s">
-        <v>608</v>
+        <v>631</v>
       </c>
       <c r="H4" t="s">
-        <v>609</v>
+        <v>632</v>
       </c>
       <c r="I4" t="s">
-        <v>604</v>
+        <v>627</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>610</v>
+        <v>633</v>
       </c>
       <c r="B5" t="s">
-        <v>611</v>
+        <v>634</v>
       </c>
       <c r="C5" t="s">
-        <v>612</v>
+        <v>635</v>
       </c>
       <c r="D5" t="s">
-        <v>613</v>
+        <v>636</v>
       </c>
       <c r="E5" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F5" t="s">
-        <v>614</v>
+        <v>637</v>
       </c>
       <c r="G5" t="s">
-        <v>615</v>
+        <v>638</v>
       </c>
       <c r="H5" t="s">
-        <v>616</v>
+        <v>639</v>
       </c>
       <c r="I5" t="s">
-        <v>611</v>
+        <v>634</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>617</v>
+        <v>640</v>
       </c>
       <c r="B6" t="s">
-        <v>618</v>
+        <v>641</v>
       </c>
       <c r="C6" t="s">
-        <v>619</v>
+        <v>642</v>
       </c>
       <c r="D6" t="s">
-        <v>620</v>
+        <v>643</v>
       </c>
       <c r="E6" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F6" t="s">
-        <v>621</v>
+        <v>644</v>
       </c>
       <c r="G6" t="s">
-        <v>622</v>
+        <v>645</v>
       </c>
       <c r="H6" t="s">
-        <v>623</v>
+        <v>646</v>
       </c>
       <c r="I6" t="s">
-        <v>624</v>
+        <v>647</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>625</v>
+        <v>648</v>
       </c>
       <c r="B7" t="s">
-        <v>626</v>
+        <v>649</v>
       </c>
       <c r="C7" t="s">
-        <v>627</v>
+        <v>650</v>
       </c>
       <c r="D7" t="s">
-        <v>628</v>
+        <v>651</v>
       </c>
       <c r="E7" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F7" t="s">
-        <v>629</v>
+        <v>652</v>
       </c>
       <c r="G7" t="s">
-        <v>630</v>
+        <v>653</v>
       </c>
       <c r="H7" t="s">
-        <v>631</v>
+        <v>654</v>
       </c>
       <c r="I7" t="s">
-        <v>632</v>
+        <v>655</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>647</v>
+        <v>670</v>
       </c>
       <c r="B8" t="s">
-        <v>648</v>
+        <v>671</v>
       </c>
       <c r="C8" t="s">
-        <v>649</v>
+        <v>672</v>
       </c>
       <c r="D8" t="s">
-        <v>650</v>
+        <v>673</v>
       </c>
       <c r="E8" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F8" t="s">
-        <v>651</v>
+        <v>674</v>
       </c>
     </row>
   </sheetData>
@@ -3076,318 +3145,318 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
-        <v>652</v>
+        <v>675</v>
       </c>
       <c r="C2" t="s">
-        <v>653</v>
+        <v>676</v>
       </c>
       <c r="D2" t="s">
-        <v>654</v>
+        <v>677</v>
       </c>
       <c r="E2" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F2" t="s">
-        <v>655</v>
+        <v>678</v>
       </c>
       <c r="G2" t="s">
-        <v>656</v>
+        <v>679</v>
       </c>
       <c r="H2" t="s">
-        <v>657</v>
+        <v>680</v>
       </c>
       <c r="I2" t="s">
-        <v>658</v>
+        <v>681</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="B3" t="s">
-        <v>659</v>
+        <v>682</v>
       </c>
       <c r="C3" t="s">
-        <v>660</v>
+        <v>683</v>
       </c>
       <c r="D3" t="s">
-        <v>661</v>
+        <v>684</v>
       </c>
       <c r="E3" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F3" t="s">
-        <v>662</v>
+        <v>685</v>
       </c>
       <c r="G3" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="H3" t="s">
-        <v>663</v>
+        <v>686</v>
       </c>
       <c r="I3" t="s">
-        <v>664</v>
+        <v>687</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>665</v>
+        <v>688</v>
       </c>
       <c r="B4" t="s">
-        <v>666</v>
+        <v>689</v>
       </c>
       <c r="C4" t="s">
-        <v>667</v>
+        <v>690</v>
       </c>
       <c r="D4" t="s">
-        <v>668</v>
+        <v>691</v>
       </c>
       <c r="E4" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F4" t="s">
-        <v>669</v>
+        <v>692</v>
       </c>
       <c r="G4" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="H4" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="I4" t="s">
-        <v>671</v>
+        <v>694</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>672</v>
+        <v>695</v>
       </c>
       <c r="B5" t="s">
-        <v>673</v>
+        <v>696</v>
       </c>
       <c r="C5" t="s">
-        <v>674</v>
+        <v>697</v>
       </c>
       <c r="D5" t="s">
-        <v>675</v>
+        <v>698</v>
       </c>
       <c r="E5" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F5" t="s">
-        <v>676</v>
+        <v>699</v>
       </c>
       <c r="G5" t="s">
-        <v>677</v>
+        <v>700</v>
       </c>
       <c r="H5" t="s">
-        <v>678</v>
+        <v>701</v>
       </c>
       <c r="I5" t="s">
-        <v>679</v>
+        <v>702</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>680</v>
+        <v>703</v>
       </c>
       <c r="B6" t="s">
-        <v>681</v>
+        <v>704</v>
       </c>
       <c r="C6" t="s">
-        <v>682</v>
+        <v>705</v>
       </c>
       <c r="D6" t="s">
-        <v>683</v>
+        <v>706</v>
       </c>
       <c r="E6" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F6" t="s">
-        <v>684</v>
+        <v>707</v>
       </c>
       <c r="G6" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="H6" t="s">
-        <v>685</v>
+        <v>708</v>
       </c>
       <c r="I6" t="s">
-        <v>686</v>
+        <v>709</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>687</v>
+        <v>710</v>
       </c>
       <c r="B7" t="s">
-        <v>688</v>
+        <v>711</v>
       </c>
       <c r="C7" t="s">
-        <v>689</v>
+        <v>712</v>
       </c>
       <c r="D7" t="s">
-        <v>690</v>
+        <v>713</v>
       </c>
       <c r="E7" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F7" t="s">
-        <v>691</v>
+        <v>714</v>
       </c>
       <c r="G7" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="H7" t="s">
-        <v>692</v>
+        <v>715</v>
       </c>
       <c r="I7" t="s">
-        <v>693</v>
+        <v>716</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>694</v>
+        <v>717</v>
       </c>
       <c r="B8" t="s">
-        <v>695</v>
+        <v>718</v>
       </c>
       <c r="C8" t="s">
-        <v>696</v>
+        <v>719</v>
       </c>
       <c r="D8" t="s">
-        <v>697</v>
+        <v>720</v>
       </c>
       <c r="E8" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F8" t="s">
-        <v>698</v>
+        <v>721</v>
       </c>
       <c r="G8" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="H8" t="s">
-        <v>699</v>
+        <v>722</v>
       </c>
       <c r="I8" t="s">
-        <v>700</v>
+        <v>723</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>701</v>
+        <v>724</v>
       </c>
       <c r="B9" t="s">
-        <v>702</v>
+        <v>725</v>
       </c>
       <c r="C9" t="s">
-        <v>703</v>
+        <v>726</v>
       </c>
       <c r="D9" t="s">
-        <v>704</v>
+        <v>727</v>
       </c>
       <c r="E9" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F9" t="s">
-        <v>705</v>
+        <v>728</v>
       </c>
       <c r="G9" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="H9" t="s">
-        <v>706</v>
+        <v>729</v>
       </c>
       <c r="I9" t="s">
-        <v>707</v>
+        <v>730</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>708</v>
+        <v>731</v>
       </c>
       <c r="B10" t="s">
-        <v>709</v>
+        <v>732</v>
       </c>
       <c r="C10" t="s">
-        <v>710</v>
+        <v>733</v>
       </c>
       <c r="D10" t="s">
-        <v>711</v>
+        <v>734</v>
       </c>
       <c r="E10" t="s">
-        <v>712</v>
+        <v>735</v>
       </c>
       <c r="F10" t="s">
-        <v>713</v>
+        <v>736</v>
       </c>
       <c r="G10" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="H10" t="s">
-        <v>714</v>
+        <v>737</v>
       </c>
       <c r="I10" t="s">
-        <v>715</v>
+        <v>738</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>716</v>
+        <v>739</v>
       </c>
       <c r="B11" t="s">
-        <v>717</v>
+        <v>740</v>
       </c>
       <c r="C11" t="s">
-        <v>718</v>
+        <v>741</v>
       </c>
       <c r="D11" t="s">
-        <v>719</v>
+        <v>742</v>
       </c>
       <c r="E11" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F11" t="s">
-        <v>720</v>
+        <v>743</v>
       </c>
       <c r="G11" t="s">
-        <v>721</v>
+        <v>744</v>
       </c>
       <c r="H11" t="s">
-        <v>722</v>
+        <v>745</v>
       </c>
     </row>
   </sheetData>
@@ -3397,7 +3466,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3405,147 +3474,169 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="H2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="I2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" t="s">
         <v>52</v>
       </c>
-      <c r="B3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H3" t="s">
-        <v>50</v>
-      </c>
       <c r="I3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="I4" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D5" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E5" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F5" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G5" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="I5" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -3563,350 +3654,350 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="D2" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="E2" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F2" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="G2" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="H2" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="I2" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="C3" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="D3" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="E3" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="F3" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="G3" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="H3" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="I3" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="B4" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="C4" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="D4" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="E4" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="F4" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="G4" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="H4" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="I4" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="B5" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="C5" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="D5" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="E5" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="F5" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="G5" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="H5" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="I5" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="B6" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="C6" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="D6" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="E6" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="F6" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="G6" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="H6" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="I6" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="B7" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="C7" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="D7" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="E7" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="F7" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="G7" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="H7" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="I7" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="B8" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="C8" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="D8" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="E8" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="F8" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="G8" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="H8" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="I8" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="B9" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="C9" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="D9" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="E9" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="F9" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="G9" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="H9" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="I9" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="B10" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="C10" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="D10" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E10" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="F10" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="G10" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="H10" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="I10" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B11" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="C11" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="D11" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="E11" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F11" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="G11" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="H11" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="I11" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="B12" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="C12" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="D12" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="E12" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F12" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="G12" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="H12" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="I12" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -3916,7 +4007,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3924,263 +4015,329 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="C2" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="D2" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="E2" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="F2" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="G2" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="H2" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="I2" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="B3" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="C3" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="D3" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="E3" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="F3" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="G3" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="H3" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="I3" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="B4" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="C4" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="D4" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="E4" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="F4" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="G4" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="H4" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="I4" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="B5" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="C5" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="D5" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="E5" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="F5" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="G5" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="H5" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="I5" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="B6" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="C6" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="D6" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="E6" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="F6" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="G6" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="H6" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="I6" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="B7" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="C7" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="D7" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="E7" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
       <c r="F7" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="G7" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="H7" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="I7" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="B8" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="C8" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="D8" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="E8" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="F8" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="G8" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="H8" t="s">
-        <v>225</v>
+        <v>233</v>
       </c>
       <c r="I8" t="s">
-        <v>226</v>
+        <v>234</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="B9" t="s">
-        <v>228</v>
+        <v>236</v>
       </c>
       <c r="C9" t="s">
-        <v>229</v>
+        <v>237</v>
       </c>
       <c r="D9" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="E9" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="F9" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
       <c r="G9" t="s">
-        <v>233</v>
+        <v>241</v>
       </c>
       <c r="H9" t="s">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="I9" t="s">
-        <v>235</v>
+        <v>243</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>244</v>
+      </c>
+      <c r="B10" t="s">
+        <v>245</v>
+      </c>
+      <c r="C10" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>247</v>
+      </c>
+      <c r="B11" t="s">
+        <v>248</v>
+      </c>
+      <c r="C11" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>250</v>
+      </c>
+      <c r="B12" t="s">
+        <v>251</v>
+      </c>
+      <c r="C12" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" t="s">
+        <v>253</v>
+      </c>
+      <c r="B13" t="s">
+        <v>254</v>
+      </c>
+      <c r="C13" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" t="s">
+        <v>256</v>
+      </c>
+      <c r="B14" t="s">
+        <v>257</v>
+      </c>
+      <c r="C14" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" t="s">
+        <v>259</v>
+      </c>
+      <c r="B15" t="s">
+        <v>260</v>
+      </c>
+      <c r="C15" t="s">
+        <v>261</v>
       </c>
     </row>
   </sheetData>
@@ -4198,370 +4355,370 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
-        <v>236</v>
+        <v>262</v>
       </c>
       <c r="C2" t="s">
-        <v>237</v>
+        <v>263</v>
       </c>
       <c r="D2" t="s">
-        <v>238</v>
+        <v>264</v>
       </c>
       <c r="E2" t="s">
-        <v>239</v>
+        <v>265</v>
       </c>
       <c r="F2" t="s">
-        <v>240</v>
+        <v>266</v>
       </c>
       <c r="G2" t="s">
-        <v>241</v>
+        <v>267</v>
       </c>
       <c r="H2" t="s">
-        <v>242</v>
+        <v>268</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="B3" t="s">
-        <v>243</v>
+        <v>269</v>
       </c>
       <c r="C3" t="s">
-        <v>244</v>
+        <v>270</v>
       </c>
       <c r="D3" t="s">
-        <v>245</v>
+        <v>271</v>
       </c>
       <c r="E3" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F3" t="s">
-        <v>246</v>
+        <v>272</v>
       </c>
       <c r="G3" t="s">
-        <v>247</v>
+        <v>273</v>
       </c>
       <c r="H3" t="s">
-        <v>248</v>
+        <v>274</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>249</v>
+        <v>275</v>
       </c>
       <c r="B4" t="s">
-        <v>250</v>
+        <v>276</v>
       </c>
       <c r="C4" t="s">
-        <v>251</v>
+        <v>277</v>
       </c>
       <c r="D4" t="s">
-        <v>252</v>
+        <v>278</v>
       </c>
       <c r="E4" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F4" t="s">
-        <v>253</v>
+        <v>279</v>
       </c>
       <c r="G4" t="s">
-        <v>254</v>
+        <v>280</v>
       </c>
       <c r="H4" t="s">
-        <v>255</v>
+        <v>281</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>256</v>
+        <v>282</v>
       </c>
       <c r="B5" t="s">
-        <v>257</v>
+        <v>283</v>
       </c>
       <c r="C5" t="s">
-        <v>258</v>
+        <v>284</v>
       </c>
       <c r="D5" t="s">
-        <v>259</v>
+        <v>285</v>
       </c>
       <c r="E5" t="s">
-        <v>260</v>
+        <v>286</v>
       </c>
       <c r="F5" t="s">
-        <v>261</v>
+        <v>287</v>
       </c>
       <c r="G5" t="s">
-        <v>262</v>
+        <v>288</v>
       </c>
       <c r="H5" t="s">
-        <v>263</v>
+        <v>289</v>
       </c>
       <c r="I5" t="s">
-        <v>264</v>
+        <v>290</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>265</v>
+        <v>291</v>
       </c>
       <c r="B6" t="s">
-        <v>266</v>
+        <v>292</v>
       </c>
       <c r="C6" t="s">
-        <v>267</v>
+        <v>293</v>
       </c>
       <c r="D6" t="s">
-        <v>268</v>
+        <v>294</v>
       </c>
       <c r="E6" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F6" t="s">
-        <v>269</v>
+        <v>295</v>
       </c>
       <c r="G6" t="s">
-        <v>270</v>
+        <v>296</v>
       </c>
       <c r="H6" t="s">
-        <v>271</v>
+        <v>297</v>
       </c>
       <c r="I6" t="s">
-        <v>272</v>
+        <v>298</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>273</v>
+        <v>299</v>
       </c>
       <c r="B7" t="s">
-        <v>274</v>
+        <v>300</v>
       </c>
       <c r="C7" t="s">
-        <v>275</v>
+        <v>301</v>
       </c>
       <c r="D7" t="s">
-        <v>276</v>
+        <v>302</v>
       </c>
       <c r="E7" t="s">
-        <v>277</v>
+        <v>303</v>
       </c>
       <c r="F7" t="s">
-        <v>278</v>
+        <v>304</v>
       </c>
       <c r="G7" t="s">
-        <v>279</v>
+        <v>305</v>
       </c>
       <c r="H7" t="s">
-        <v>280</v>
+        <v>306</v>
       </c>
       <c r="I7" t="s">
-        <v>281</v>
+        <v>307</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>282</v>
+        <v>308</v>
       </c>
       <c r="B8" t="s">
-        <v>283</v>
+        <v>309</v>
       </c>
       <c r="C8" t="s">
-        <v>284</v>
+        <v>310</v>
       </c>
       <c r="D8" t="s">
-        <v>285</v>
+        <v>311</v>
       </c>
       <c r="E8" t="s">
-        <v>286</v>
+        <v>312</v>
       </c>
       <c r="F8" t="s">
-        <v>287</v>
+        <v>313</v>
       </c>
       <c r="G8" t="s">
-        <v>288</v>
+        <v>314</v>
       </c>
       <c r="H8" t="s">
-        <v>289</v>
+        <v>315</v>
       </c>
       <c r="I8" t="s">
-        <v>290</v>
+        <v>316</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>291</v>
+        <v>317</v>
       </c>
       <c r="B9" t="s">
-        <v>292</v>
+        <v>318</v>
       </c>
       <c r="C9" t="s">
-        <v>293</v>
+        <v>319</v>
       </c>
       <c r="D9" t="s">
-        <v>294</v>
+        <v>320</v>
       </c>
       <c r="E9" t="s">
-        <v>295</v>
+        <v>321</v>
       </c>
       <c r="F9" t="s">
-        <v>296</v>
+        <v>322</v>
       </c>
       <c r="G9" t="s">
-        <v>297</v>
+        <v>323</v>
       </c>
       <c r="H9" t="s">
-        <v>298</v>
+        <v>324</v>
       </c>
       <c r="I9" t="s">
-        <v>299</v>
+        <v>325</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>300</v>
+        <v>326</v>
       </c>
       <c r="B10" t="s">
-        <v>301</v>
+        <v>327</v>
       </c>
       <c r="C10" t="s">
-        <v>302</v>
+        <v>328</v>
       </c>
       <c r="D10" t="s">
-        <v>303</v>
+        <v>329</v>
       </c>
       <c r="E10" t="s">
-        <v>304</v>
+        <v>330</v>
       </c>
       <c r="F10" t="s">
-        <v>305</v>
+        <v>331</v>
       </c>
       <c r="G10" t="s">
-        <v>306</v>
+        <v>332</v>
       </c>
       <c r="H10" t="s">
-        <v>307</v>
+        <v>333</v>
       </c>
       <c r="I10" t="s">
-        <v>308</v>
+        <v>334</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>309</v>
+        <v>335</v>
       </c>
       <c r="B11" t="s">
-        <v>310</v>
+        <v>336</v>
       </c>
       <c r="C11" t="s">
-        <v>311</v>
+        <v>337</v>
       </c>
       <c r="D11" t="s">
-        <v>312</v>
+        <v>338</v>
       </c>
       <c r="E11" t="s">
-        <v>313</v>
+        <v>339</v>
       </c>
       <c r="F11" t="s">
-        <v>314</v>
+        <v>340</v>
       </c>
       <c r="G11" t="s">
-        <v>315</v>
+        <v>341</v>
       </c>
       <c r="H11" t="s">
-        <v>316</v>
+        <v>342</v>
       </c>
       <c r="I11" t="s">
-        <v>317</v>
+        <v>343</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>318</v>
+        <v>344</v>
       </c>
       <c r="B12" t="s">
-        <v>319</v>
+        <v>345</v>
       </c>
       <c r="C12" t="s">
-        <v>320</v>
+        <v>346</v>
       </c>
       <c r="D12" t="s">
-        <v>321</v>
+        <v>347</v>
       </c>
       <c r="E12" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F12" t="s">
-        <v>322</v>
+        <v>348</v>
       </c>
       <c r="G12" t="s">
-        <v>323</v>
+        <v>349</v>
       </c>
       <c r="H12" t="s">
-        <v>324</v>
+        <v>350</v>
       </c>
       <c r="I12" t="s">
-        <v>319</v>
+        <v>345</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>325</v>
+        <v>351</v>
       </c>
       <c r="B13" t="s">
-        <v>326</v>
+        <v>352</v>
       </c>
       <c r="C13" t="s">
-        <v>327</v>
+        <v>353</v>
       </c>
       <c r="D13" t="s">
-        <v>328</v>
+        <v>354</v>
       </c>
       <c r="E13" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F13" t="s">
-        <v>329</v>
+        <v>355</v>
       </c>
       <c r="G13" t="s">
-        <v>330</v>
+        <v>356</v>
       </c>
       <c r="H13" t="s">
-        <v>331</v>
+        <v>357</v>
       </c>
       <c r="I13" t="s">
-        <v>326</v>
+        <v>352</v>
       </c>
     </row>
   </sheetData>
@@ -4579,706 +4736,706 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
-        <v>332</v>
+        <v>358</v>
       </c>
       <c r="C2" t="s">
-        <v>333</v>
+        <v>359</v>
       </c>
       <c r="D2" t="s">
-        <v>334</v>
+        <v>360</v>
       </c>
       <c r="E2" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F2" t="s">
-        <v>335</v>
+        <v>361</v>
       </c>
       <c r="G2" t="s">
-        <v>336</v>
+        <v>362</v>
       </c>
       <c r="H2" t="s">
-        <v>337</v>
+        <v>363</v>
       </c>
       <c r="I2" t="s">
-        <v>338</v>
+        <v>364</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="B3" t="s">
-        <v>339</v>
+        <v>365</v>
       </c>
       <c r="C3" t="s">
-        <v>340</v>
+        <v>366</v>
       </c>
       <c r="D3" t="s">
-        <v>341</v>
+        <v>367</v>
       </c>
       <c r="E3" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F3" t="s">
-        <v>342</v>
+        <v>368</v>
       </c>
       <c r="G3" t="s">
-        <v>343</v>
+        <v>369</v>
       </c>
       <c r="H3" t="s">
-        <v>344</v>
+        <v>370</v>
       </c>
       <c r="I3" t="s">
-        <v>345</v>
+        <v>371</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>346</v>
+        <v>372</v>
       </c>
       <c r="B4" t="s">
-        <v>347</v>
+        <v>373</v>
       </c>
       <c r="C4" t="s">
-        <v>348</v>
+        <v>374</v>
       </c>
       <c r="D4" t="s">
-        <v>349</v>
+        <v>375</v>
       </c>
       <c r="E4" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F4" t="s">
-        <v>350</v>
+        <v>376</v>
       </c>
       <c r="G4" t="s">
-        <v>351</v>
+        <v>377</v>
       </c>
       <c r="H4" t="s">
-        <v>352</v>
+        <v>378</v>
       </c>
       <c r="I4" t="s">
-        <v>353</v>
+        <v>379</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>354</v>
+        <v>380</v>
       </c>
       <c r="B5" t="s">
-        <v>355</v>
+        <v>76</v>
       </c>
       <c r="C5" t="s">
-        <v>356</v>
+        <v>77</v>
       </c>
       <c r="D5" t="s">
-        <v>357</v>
+        <v>381</v>
       </c>
       <c r="E5" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F5" t="s">
-        <v>358</v>
+        <v>382</v>
       </c>
       <c r="G5" t="s">
-        <v>359</v>
+        <v>383</v>
       </c>
       <c r="H5" t="s">
-        <v>360</v>
+        <v>384</v>
       </c>
       <c r="I5" t="s">
-        <v>361</v>
+        <v>385</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>362</v>
+        <v>386</v>
       </c>
       <c r="B6" t="s">
-        <v>363</v>
+        <v>387</v>
       </c>
       <c r="C6" t="s">
-        <v>364</v>
+        <v>388</v>
       </c>
       <c r="D6" t="s">
-        <v>365</v>
+        <v>389</v>
       </c>
       <c r="E6" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F6" t="s">
-        <v>366</v>
+        <v>390</v>
       </c>
       <c r="G6" t="s">
-        <v>367</v>
+        <v>391</v>
       </c>
       <c r="H6" t="s">
-        <v>368</v>
+        <v>392</v>
       </c>
       <c r="I6" t="s">
-        <v>369</v>
+        <v>393</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>370</v>
+        <v>394</v>
       </c>
       <c r="B7" t="s">
-        <v>371</v>
+        <v>395</v>
       </c>
       <c r="C7" t="s">
-        <v>372</v>
+        <v>74</v>
       </c>
       <c r="D7" t="s">
-        <v>373</v>
+        <v>396</v>
       </c>
       <c r="E7" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F7" t="s">
-        <v>374</v>
+        <v>397</v>
       </c>
       <c r="G7" t="s">
-        <v>375</v>
+        <v>398</v>
       </c>
       <c r="H7" t="s">
-        <v>376</v>
+        <v>399</v>
       </c>
       <c r="I7" t="s">
-        <v>377</v>
+        <v>400</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>378</v>
+        <v>401</v>
       </c>
       <c r="B8" t="s">
-        <v>379</v>
+        <v>402</v>
       </c>
       <c r="C8" t="s">
-        <v>380</v>
+        <v>403</v>
       </c>
       <c r="D8" t="s">
-        <v>381</v>
+        <v>404</v>
       </c>
       <c r="E8" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F8" t="s">
-        <v>382</v>
+        <v>405</v>
       </c>
       <c r="G8" t="s">
-        <v>383</v>
+        <v>406</v>
       </c>
       <c r="H8" t="s">
-        <v>384</v>
+        <v>407</v>
       </c>
       <c r="I8" t="s">
-        <v>385</v>
+        <v>408</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>386</v>
+        <v>409</v>
       </c>
       <c r="B9" t="s">
-        <v>387</v>
+        <v>410</v>
       </c>
       <c r="C9" t="s">
-        <v>388</v>
+        <v>411</v>
       </c>
       <c r="D9" t="s">
-        <v>389</v>
+        <v>412</v>
       </c>
       <c r="E9" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F9" t="s">
-        <v>390</v>
+        <v>413</v>
       </c>
       <c r="G9" t="s">
-        <v>391</v>
+        <v>414</v>
       </c>
       <c r="H9" t="s">
-        <v>392</v>
+        <v>415</v>
       </c>
       <c r="I9" t="s">
-        <v>393</v>
+        <v>416</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>394</v>
+        <v>417</v>
       </c>
       <c r="B10" t="s">
-        <v>395</v>
+        <v>418</v>
       </c>
       <c r="C10" t="s">
-        <v>258</v>
+        <v>284</v>
       </c>
       <c r="D10" t="s">
-        <v>396</v>
+        <v>419</v>
       </c>
       <c r="E10" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F10" t="s">
-        <v>261</v>
+        <v>287</v>
       </c>
       <c r="G10" t="s">
-        <v>397</v>
+        <v>420</v>
       </c>
       <c r="H10" t="s">
-        <v>398</v>
+        <v>421</v>
       </c>
       <c r="I10" t="s">
-        <v>264</v>
+        <v>290</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>399</v>
+        <v>422</v>
       </c>
       <c r="B11" t="s">
-        <v>319</v>
+        <v>345</v>
       </c>
       <c r="C11" t="s">
-        <v>320</v>
+        <v>346</v>
       </c>
       <c r="D11" t="s">
-        <v>321</v>
+        <v>347</v>
       </c>
       <c r="E11" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F11" t="s">
-        <v>322</v>
+        <v>348</v>
       </c>
       <c r="G11" t="s">
-        <v>323</v>
+        <v>349</v>
       </c>
       <c r="H11" t="s">
-        <v>324</v>
+        <v>350</v>
       </c>
       <c r="I11" t="s">
-        <v>319</v>
+        <v>345</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>400</v>
+        <v>423</v>
       </c>
       <c r="B12" t="s">
-        <v>326</v>
+        <v>352</v>
       </c>
       <c r="C12" t="s">
-        <v>327</v>
+        <v>353</v>
       </c>
       <c r="D12" t="s">
-        <v>328</v>
+        <v>354</v>
       </c>
       <c r="E12" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F12" t="s">
-        <v>329</v>
+        <v>355</v>
       </c>
       <c r="G12" t="s">
-        <v>330</v>
+        <v>356</v>
       </c>
       <c r="H12" t="s">
-        <v>331</v>
+        <v>357</v>
       </c>
       <c r="I12" t="s">
-        <v>326</v>
+        <v>352</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>401</v>
+        <v>424</v>
       </c>
       <c r="B13" t="s">
-        <v>402</v>
+        <v>425</v>
       </c>
       <c r="C13" t="s">
-        <v>403</v>
+        <v>426</v>
       </c>
       <c r="D13" t="s">
-        <v>404</v>
+        <v>427</v>
       </c>
       <c r="E13" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F13" t="s">
-        <v>405</v>
+        <v>428</v>
       </c>
       <c r="G13" t="s">
-        <v>406</v>
+        <v>429</v>
       </c>
       <c r="H13" t="s">
-        <v>407</v>
+        <v>430</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>408</v>
+        <v>431</v>
       </c>
       <c r="B14" t="s">
-        <v>409</v>
+        <v>432</v>
       </c>
       <c r="C14" t="s">
-        <v>410</v>
+        <v>433</v>
       </c>
       <c r="D14" t="s">
-        <v>411</v>
+        <v>434</v>
       </c>
       <c r="E14" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F14" t="s">
-        <v>412</v>
+        <v>435</v>
       </c>
       <c r="G14" t="s">
-        <v>413</v>
+        <v>436</v>
       </c>
       <c r="H14" t="s">
-        <v>414</v>
+        <v>437</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>415</v>
+        <v>438</v>
       </c>
       <c r="B15" t="s">
-        <v>416</v>
+        <v>439</v>
       </c>
       <c r="C15" t="s">
-        <v>417</v>
+        <v>440</v>
       </c>
       <c r="D15" t="s">
-        <v>418</v>
+        <v>441</v>
       </c>
       <c r="E15" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F15" t="s">
-        <v>419</v>
+        <v>442</v>
       </c>
       <c r="G15" t="s">
-        <v>420</v>
+        <v>443</v>
       </c>
       <c r="H15" t="s">
-        <v>421</v>
+        <v>444</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>422</v>
+        <v>445</v>
       </c>
       <c r="B16" t="s">
-        <v>423</v>
+        <v>446</v>
       </c>
       <c r="C16" t="s">
-        <v>424</v>
+        <v>447</v>
       </c>
       <c r="D16" t="s">
-        <v>425</v>
+        <v>448</v>
       </c>
       <c r="E16" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F16" t="s">
-        <v>426</v>
+        <v>449</v>
       </c>
       <c r="G16" t="s">
-        <v>427</v>
+        <v>450</v>
       </c>
       <c r="H16" t="s">
-        <v>428</v>
+        <v>451</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>429</v>
+        <v>452</v>
       </c>
       <c r="B17" t="s">
-        <v>430</v>
+        <v>453</v>
       </c>
       <c r="C17" t="s">
-        <v>431</v>
+        <v>454</v>
       </c>
       <c r="D17" t="s">
-        <v>432</v>
+        <v>455</v>
       </c>
       <c r="E17" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F17" t="s">
-        <v>433</v>
+        <v>456</v>
       </c>
       <c r="G17" t="s">
-        <v>434</v>
+        <v>457</v>
       </c>
       <c r="H17" t="s">
-        <v>435</v>
+        <v>458</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>436</v>
+        <v>459</v>
       </c>
       <c r="B18" t="s">
-        <v>437</v>
+        <v>460</v>
       </c>
       <c r="C18" t="s">
-        <v>438</v>
+        <v>461</v>
       </c>
       <c r="D18" t="s">
-        <v>439</v>
+        <v>462</v>
       </c>
       <c r="E18" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F18" t="s">
-        <v>440</v>
+        <v>463</v>
       </c>
       <c r="G18" t="s">
-        <v>441</v>
+        <v>464</v>
       </c>
       <c r="H18" t="s">
-        <v>442</v>
+        <v>465</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>443</v>
+        <v>466</v>
       </c>
       <c r="B19" t="s">
-        <v>444</v>
+        <v>467</v>
       </c>
       <c r="C19" t="s">
-        <v>445</v>
+        <v>468</v>
       </c>
       <c r="D19" t="s">
-        <v>446</v>
+        <v>469</v>
       </c>
       <c r="E19" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F19" t="s">
-        <v>447</v>
+        <v>470</v>
       </c>
       <c r="G19" t="s">
-        <v>448</v>
+        <v>471</v>
       </c>
       <c r="H19" t="s">
-        <v>449</v>
+        <v>472</v>
       </c>
       <c r="I19" t="s">
-        <v>450</v>
+        <v>473</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>451</v>
+        <v>474</v>
       </c>
       <c r="B20" t="s">
-        <v>452</v>
+        <v>475</v>
       </c>
       <c r="C20" t="s">
-        <v>453</v>
+        <v>476</v>
       </c>
       <c r="D20" t="s">
-        <v>454</v>
+        <v>477</v>
       </c>
       <c r="E20" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F20" t="s">
-        <v>455</v>
+        <v>478</v>
       </c>
       <c r="G20" t="s">
-        <v>456</v>
+        <v>479</v>
       </c>
       <c r="H20" t="s">
-        <v>457</v>
+        <v>480</v>
       </c>
       <c r="I20" t="s">
-        <v>458</v>
+        <v>481</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>459</v>
+        <v>482</v>
       </c>
       <c r="B21" t="s">
-        <v>460</v>
+        <v>483</v>
       </c>
       <c r="C21" t="s">
-        <v>461</v>
+        <v>484</v>
       </c>
       <c r="D21" t="s">
-        <v>462</v>
+        <v>485</v>
       </c>
       <c r="E21" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F21" t="s">
-        <v>463</v>
+        <v>486</v>
       </c>
       <c r="G21" t="s">
-        <v>464</v>
+        <v>487</v>
       </c>
       <c r="H21" t="s">
-        <v>465</v>
+        <v>488</v>
       </c>
       <c r="I21" t="s">
-        <v>466</v>
+        <v>489</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>467</v>
+        <v>490</v>
       </c>
       <c r="B22" t="s">
-        <v>468</v>
+        <v>491</v>
       </c>
       <c r="C22" t="s">
-        <v>469</v>
+        <v>492</v>
       </c>
       <c r="D22" t="s">
-        <v>470</v>
+        <v>493</v>
       </c>
       <c r="E22" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F22" t="s">
-        <v>471</v>
+        <v>494</v>
       </c>
       <c r="G22" t="s">
-        <v>472</v>
+        <v>495</v>
       </c>
       <c r="H22" t="s">
-        <v>473</v>
+        <v>496</v>
       </c>
       <c r="I22" t="s">
-        <v>474</v>
+        <v>497</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>475</v>
+        <v>498</v>
       </c>
       <c r="B23" t="s">
-        <v>476</v>
+        <v>499</v>
       </c>
       <c r="C23" t="s">
-        <v>477</v>
+        <v>500</v>
       </c>
       <c r="D23" t="s">
-        <v>478</v>
+        <v>501</v>
       </c>
       <c r="E23" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F23" t="s">
-        <v>479</v>
+        <v>502</v>
       </c>
       <c r="G23" t="s">
-        <v>480</v>
+        <v>503</v>
       </c>
       <c r="H23" t="s">
-        <v>481</v>
+        <v>504</v>
       </c>
       <c r="I23" t="s">
-        <v>482</v>
+        <v>505</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>483</v>
+        <v>506</v>
       </c>
       <c r="B24" t="s">
-        <v>484</v>
+        <v>507</v>
       </c>
       <c r="C24" t="s">
-        <v>485</v>
+        <v>508</v>
       </c>
       <c r="D24" t="s">
-        <v>486</v>
+        <v>509</v>
       </c>
       <c r="E24" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F24" t="s">
-        <v>487</v>
+        <v>510</v>
       </c>
       <c r="G24" t="s">
-        <v>488</v>
+        <v>511</v>
       </c>
       <c r="H24" t="s">
-        <v>489</v>
+        <v>512</v>
       </c>
       <c r="I24" t="s">
-        <v>490</v>
+        <v>513</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>491</v>
+        <v>514</v>
       </c>
       <c r="B25" t="s">
-        <v>492</v>
+        <v>515</v>
       </c>
       <c r="C25" t="s">
-        <v>493</v>
+        <v>516</v>
       </c>
       <c r="D25" t="s">
-        <v>494</v>
+        <v>517</v>
       </c>
       <c r="E25" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F25" t="s">
-        <v>495</v>
+        <v>518</v>
       </c>
       <c r="G25" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="H25" t="s">
-        <v>496</v>
+        <v>519</v>
       </c>
     </row>
   </sheetData>
@@ -5296,260 +5453,260 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
-        <v>497</v>
+        <v>520</v>
       </c>
       <c r="C2" t="s">
-        <v>498</v>
+        <v>521</v>
       </c>
       <c r="D2" t="s">
-        <v>499</v>
+        <v>522</v>
       </c>
       <c r="E2" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F2" t="s">
-        <v>499</v>
+        <v>522</v>
       </c>
       <c r="G2" t="s">
-        <v>500</v>
+        <v>523</v>
       </c>
       <c r="H2" t="s">
-        <v>501</v>
+        <v>524</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="B3" t="s">
-        <v>502</v>
+        <v>525</v>
       </c>
       <c r="C3" t="s">
-        <v>503</v>
+        <v>526</v>
       </c>
       <c r="D3" t="s">
-        <v>504</v>
+        <v>527</v>
       </c>
       <c r="E3" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F3" t="s">
-        <v>504</v>
+        <v>527</v>
       </c>
       <c r="G3" t="s">
-        <v>505</v>
+        <v>528</v>
       </c>
       <c r="H3" t="s">
-        <v>506</v>
+        <v>529</v>
       </c>
       <c r="I3" t="s">
-        <v>507</v>
+        <v>530</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>346</v>
+        <v>372</v>
       </c>
       <c r="B4" t="s">
-        <v>347</v>
+        <v>373</v>
       </c>
       <c r="C4" t="s">
-        <v>348</v>
+        <v>374</v>
       </c>
       <c r="D4" t="s">
-        <v>508</v>
+        <v>531</v>
       </c>
       <c r="E4" t="s">
-        <v>509</v>
+        <v>532</v>
       </c>
       <c r="F4" t="s">
-        <v>508</v>
+        <v>531</v>
       </c>
       <c r="G4" t="s">
-        <v>351</v>
+        <v>377</v>
       </c>
       <c r="H4" t="s">
-        <v>352</v>
+        <v>378</v>
       </c>
       <c r="I4" t="s">
-        <v>510</v>
+        <v>533</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>354</v>
+        <v>380</v>
       </c>
       <c r="B5" t="s">
-        <v>355</v>
+        <v>76</v>
       </c>
       <c r="C5" t="s">
-        <v>356</v>
+        <v>77</v>
       </c>
       <c r="D5" t="s">
-        <v>358</v>
+        <v>382</v>
       </c>
       <c r="E5" t="s">
-        <v>511</v>
+        <v>534</v>
       </c>
       <c r="F5" t="s">
-        <v>358</v>
+        <v>382</v>
       </c>
       <c r="G5" t="s">
-        <v>359</v>
+        <v>383</v>
       </c>
       <c r="H5" t="s">
-        <v>360</v>
+        <v>384</v>
       </c>
       <c r="I5" t="s">
-        <v>361</v>
+        <v>385</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>362</v>
+        <v>386</v>
       </c>
       <c r="B6" t="s">
-        <v>363</v>
+        <v>387</v>
       </c>
       <c r="C6" t="s">
-        <v>364</v>
+        <v>388</v>
       </c>
       <c r="D6" t="s">
-        <v>512</v>
+        <v>535</v>
       </c>
       <c r="E6" t="s">
-        <v>513</v>
+        <v>536</v>
       </c>
       <c r="F6" t="s">
-        <v>512</v>
+        <v>535</v>
       </c>
       <c r="G6" t="s">
-        <v>514</v>
+        <v>537</v>
       </c>
       <c r="H6" t="s">
-        <v>368</v>
+        <v>392</v>
       </c>
       <c r="I6" t="s">
-        <v>515</v>
+        <v>538</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>370</v>
+        <v>394</v>
       </c>
       <c r="B7" t="s">
-        <v>371</v>
+        <v>395</v>
       </c>
       <c r="C7" t="s">
-        <v>372</v>
+        <v>74</v>
       </c>
       <c r="D7" t="s">
-        <v>374</v>
+        <v>397</v>
       </c>
       <c r="E7" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F7" t="s">
-        <v>374</v>
+        <v>397</v>
       </c>
       <c r="G7" t="s">
-        <v>516</v>
+        <v>539</v>
       </c>
       <c r="H7" t="s">
-        <v>376</v>
+        <v>399</v>
       </c>
       <c r="I7" t="s">
-        <v>377</v>
+        <v>400</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>517</v>
+        <v>540</v>
       </c>
       <c r="B8" t="s">
-        <v>518</v>
+        <v>541</v>
       </c>
       <c r="C8" t="s">
-        <v>519</v>
+        <v>542</v>
       </c>
       <c r="D8" t="s">
-        <v>520</v>
+        <v>543</v>
       </c>
       <c r="E8" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F8" t="s">
-        <v>520</v>
+        <v>543</v>
       </c>
       <c r="G8" t="s">
-        <v>521</v>
+        <v>544</v>
       </c>
       <c r="H8" t="s">
-        <v>522</v>
+        <v>545</v>
       </c>
       <c r="I8" t="s">
-        <v>523</v>
+        <v>546</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>524</v>
+        <v>547</v>
       </c>
       <c r="B9" t="s">
-        <v>525</v>
+        <v>548</v>
       </c>
       <c r="C9" t="s">
-        <v>526</v>
+        <v>549</v>
       </c>
       <c r="D9" t="s">
-        <v>527</v>
+        <v>550</v>
       </c>
       <c r="E9" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F9" t="s">
-        <v>527</v>
+        <v>550</v>
       </c>
       <c r="G9" t="s">
-        <v>528</v>
+        <v>551</v>
       </c>
       <c r="H9" t="s">
-        <v>529</v>
+        <v>552</v>
       </c>
       <c r="I9" t="s">
-        <v>530</v>
+        <v>553</v>
       </c>
     </row>
   </sheetData>
@@ -5567,263 +5724,263 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>531</v>
+        <v>554</v>
       </c>
       <c r="D2" t="s">
-        <v>532</v>
+        <v>555</v>
       </c>
       <c r="E2" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F2" t="s">
-        <v>533</v>
+        <v>556</v>
       </c>
       <c r="G2" t="s">
-        <v>534</v>
+        <v>557</v>
       </c>
       <c r="H2" t="s">
-        <v>535</v>
+        <v>558</v>
       </c>
       <c r="I2" t="s">
-        <v>536</v>
+        <v>559</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="B3" t="s">
-        <v>537</v>
+        <v>560</v>
       </c>
       <c r="C3" t="s">
-        <v>538</v>
+        <v>561</v>
       </c>
       <c r="D3" t="s">
-        <v>539</v>
+        <v>562</v>
       </c>
       <c r="E3" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F3" t="s">
-        <v>540</v>
+        <v>563</v>
       </c>
       <c r="G3" t="s">
-        <v>541</v>
+        <v>564</v>
       </c>
       <c r="H3" t="s">
-        <v>542</v>
+        <v>565</v>
       </c>
       <c r="I3" t="s">
-        <v>543</v>
+        <v>566</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>544</v>
+        <v>567</v>
       </c>
       <c r="B4" t="s">
-        <v>545</v>
+        <v>568</v>
       </c>
       <c r="C4" t="s">
-        <v>546</v>
+        <v>569</v>
       </c>
       <c r="D4" t="s">
-        <v>547</v>
+        <v>570</v>
       </c>
       <c r="E4" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F4" t="s">
-        <v>548</v>
+        <v>571</v>
       </c>
       <c r="G4" t="s">
-        <v>549</v>
+        <v>572</v>
       </c>
       <c r="H4" t="s">
-        <v>550</v>
+        <v>573</v>
       </c>
       <c r="I4" t="s">
-        <v>551</v>
+        <v>574</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>552</v>
+        <v>575</v>
       </c>
       <c r="B5" t="s">
-        <v>553</v>
+        <v>576</v>
       </c>
       <c r="C5" t="s">
-        <v>554</v>
+        <v>577</v>
       </c>
       <c r="D5" t="s">
-        <v>555</v>
+        <v>578</v>
       </c>
       <c r="E5" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F5" t="s">
-        <v>556</v>
+        <v>579</v>
       </c>
       <c r="G5" t="s">
-        <v>557</v>
+        <v>580</v>
       </c>
       <c r="H5" t="s">
-        <v>558</v>
+        <v>581</v>
       </c>
       <c r="I5" t="s">
-        <v>559</v>
+        <v>582</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>560</v>
+        <v>583</v>
       </c>
       <c r="B6" t="s">
-        <v>561</v>
+        <v>584</v>
       </c>
       <c r="C6" t="s">
-        <v>562</v>
+        <v>585</v>
       </c>
       <c r="D6" t="s">
-        <v>563</v>
+        <v>586</v>
       </c>
       <c r="E6" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F6" t="s">
-        <v>564</v>
+        <v>587</v>
       </c>
       <c r="G6" t="s">
-        <v>565</v>
+        <v>588</v>
       </c>
       <c r="H6" t="s">
-        <v>566</v>
+        <v>589</v>
       </c>
       <c r="I6" t="s">
-        <v>567</v>
+        <v>590</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>568</v>
+        <v>591</v>
       </c>
       <c r="B7" t="s">
-        <v>569</v>
+        <v>592</v>
       </c>
       <c r="C7" t="s">
-        <v>570</v>
+        <v>593</v>
       </c>
       <c r="D7" t="s">
-        <v>571</v>
+        <v>594</v>
       </c>
       <c r="E7" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F7" t="s">
-        <v>569</v>
+        <v>592</v>
       </c>
       <c r="G7" t="s">
-        <v>572</v>
+        <v>595</v>
       </c>
       <c r="H7" t="s">
-        <v>573</v>
+        <v>596</v>
       </c>
       <c r="I7" t="s">
-        <v>574</v>
+        <v>597</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>575</v>
+        <v>598</v>
       </c>
       <c r="B8" t="s">
-        <v>576</v>
+        <v>599</v>
       </c>
       <c r="C8" t="s">
-        <v>577</v>
+        <v>600</v>
       </c>
       <c r="D8" t="s">
-        <v>578</v>
+        <v>601</v>
       </c>
       <c r="E8" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F8" t="s">
-        <v>579</v>
+        <v>602</v>
       </c>
       <c r="G8" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="H8" t="s">
-        <v>580</v>
+        <v>603</v>
       </c>
       <c r="I8" t="s">
-        <v>581</v>
+        <v>604</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>582</v>
+        <v>605</v>
       </c>
       <c r="B9" t="s">
-        <v>583</v>
+        <v>606</v>
       </c>
       <c r="C9" t="s">
-        <v>584</v>
+        <v>607</v>
       </c>
       <c r="D9" t="s">
-        <v>585</v>
+        <v>608</v>
       </c>
       <c r="E9" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F9" t="s">
-        <v>586</v>
+        <v>609</v>
       </c>
       <c r="G9" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="H9" t="s">
-        <v>587</v>
+        <v>610</v>
       </c>
       <c r="I9" t="s">
-        <v>588</v>
+        <v>611</v>
       </c>
     </row>
   </sheetData>
@@ -5841,205 +5998,205 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
-        <v>589</v>
+        <v>612</v>
       </c>
       <c r="C2" t="s">
-        <v>590</v>
+        <v>613</v>
       </c>
       <c r="D2" t="s">
-        <v>591</v>
+        <v>614</v>
       </c>
       <c r="E2" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F2" t="s">
-        <v>592</v>
+        <v>615</v>
       </c>
       <c r="G2" t="s">
-        <v>593</v>
+        <v>616</v>
       </c>
       <c r="H2" t="s">
-        <v>594</v>
+        <v>617</v>
       </c>
       <c r="I2" t="s">
-        <v>595</v>
+        <v>618</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="B3" t="s">
-        <v>596</v>
+        <v>619</v>
       </c>
       <c r="C3" t="s">
-        <v>597</v>
+        <v>620</v>
       </c>
       <c r="D3" t="s">
-        <v>598</v>
+        <v>621</v>
       </c>
       <c r="E3" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F3" t="s">
-        <v>599</v>
+        <v>622</v>
       </c>
       <c r="G3" t="s">
-        <v>600</v>
+        <v>623</v>
       </c>
       <c r="H3" t="s">
-        <v>601</v>
+        <v>624</v>
       </c>
       <c r="I3" t="s">
-        <v>602</v>
+        <v>625</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>603</v>
+        <v>626</v>
       </c>
       <c r="B4" t="s">
-        <v>604</v>
+        <v>627</v>
       </c>
       <c r="C4" t="s">
-        <v>605</v>
+        <v>628</v>
       </c>
       <c r="D4" t="s">
-        <v>606</v>
+        <v>629</v>
       </c>
       <c r="E4" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F4" t="s">
-        <v>607</v>
+        <v>630</v>
       </c>
       <c r="G4" t="s">
-        <v>608</v>
+        <v>631</v>
       </c>
       <c r="H4" t="s">
-        <v>609</v>
+        <v>632</v>
       </c>
       <c r="I4" t="s">
-        <v>604</v>
+        <v>627</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>610</v>
+        <v>633</v>
       </c>
       <c r="B5" t="s">
-        <v>611</v>
+        <v>634</v>
       </c>
       <c r="C5" t="s">
-        <v>612</v>
+        <v>635</v>
       </c>
       <c r="D5" t="s">
-        <v>613</v>
+        <v>636</v>
       </c>
       <c r="E5" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F5" t="s">
-        <v>614</v>
+        <v>637</v>
       </c>
       <c r="G5" t="s">
-        <v>615</v>
+        <v>638</v>
       </c>
       <c r="H5" t="s">
-        <v>616</v>
+        <v>639</v>
       </c>
       <c r="I5" t="s">
-        <v>611</v>
+        <v>634</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>617</v>
+        <v>640</v>
       </c>
       <c r="B6" t="s">
-        <v>618</v>
+        <v>641</v>
       </c>
       <c r="C6" t="s">
-        <v>619</v>
+        <v>642</v>
       </c>
       <c r="D6" t="s">
-        <v>620</v>
+        <v>643</v>
       </c>
       <c r="E6" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F6" t="s">
-        <v>621</v>
+        <v>644</v>
       </c>
       <c r="G6" t="s">
-        <v>622</v>
+        <v>645</v>
       </c>
       <c r="H6" t="s">
-        <v>623</v>
+        <v>646</v>
       </c>
       <c r="I6" t="s">
-        <v>624</v>
+        <v>647</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>625</v>
+        <v>648</v>
       </c>
       <c r="B7" t="s">
-        <v>626</v>
+        <v>649</v>
       </c>
       <c r="C7" t="s">
-        <v>627</v>
+        <v>650</v>
       </c>
       <c r="D7" t="s">
-        <v>628</v>
+        <v>651</v>
       </c>
       <c r="E7" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F7" t="s">
-        <v>629</v>
+        <v>652</v>
       </c>
       <c r="G7" t="s">
-        <v>630</v>
+        <v>653</v>
       </c>
       <c r="H7" t="s">
-        <v>631</v>
+        <v>654</v>
       </c>
       <c r="I7" t="s">
-        <v>632</v>
+        <v>655</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor async key limiter improvements
- SkyHook key caching is done every frame rather than only when changing the key limiter
- Players can clear all keys (useful due to differences in key codes between SharpHook and SkyHook)
- Formatting fixes
</commit_message>
<xml_diff>
--- a/AdofaiTweaks.Generator/translations.xlsx
+++ b/AdofaiTweaks.Generator/translations.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1453" uniqueCount="1005">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1455" uniqueCount="1007">
   <si>
     <t>Translation Status</t>
   </si>
@@ -2154,6 +2154,12 @@
   </si>
   <si>
     <t>Thay đổi phím</t>
+  </si>
+  <si>
+    <t>CLEAR_ALL_KEYS</t>
+  </si>
+  <si>
+    <t>Clear All Keys</t>
   </si>
   <si>
     <t>LIMIT_CLS</t>
@@ -3789,34 +3795,34 @@
         <v>102</v>
       </c>
       <c r="B2" t="s">
-        <v>884</v>
+        <v>886</v>
       </c>
       <c r="C2" t="s">
-        <v>885</v>
+        <v>887</v>
       </c>
       <c r="D2" t="s">
-        <v>886</v>
+        <v>888</v>
       </c>
       <c r="E2" t="s">
         <v>87</v>
       </c>
       <c r="F2" t="s">
-        <v>887</v>
+        <v>889</v>
       </c>
       <c r="G2" t="s">
-        <v>888</v>
+        <v>890</v>
       </c>
       <c r="H2" t="s">
-        <v>889</v>
+        <v>891</v>
       </c>
       <c r="I2" t="s">
-        <v>890</v>
+        <v>892</v>
       </c>
       <c r="J2" t="s">
-        <v>891</v>
+        <v>893</v>
       </c>
       <c r="K2" t="s">
-        <v>892</v>
+        <v>894</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -3824,209 +3830,209 @@
         <v>113</v>
       </c>
       <c r="B3" t="s">
-        <v>893</v>
+        <v>895</v>
       </c>
       <c r="C3" t="s">
-        <v>894</v>
+        <v>896</v>
       </c>
       <c r="D3" t="s">
-        <v>895</v>
+        <v>897</v>
       </c>
       <c r="E3" t="s">
         <v>87</v>
       </c>
       <c r="F3" t="s">
-        <v>896</v>
+        <v>898</v>
       </c>
       <c r="G3" t="s">
-        <v>897</v>
+        <v>899</v>
       </c>
       <c r="H3" t="s">
-        <v>898</v>
+        <v>900</v>
       </c>
       <c r="I3" t="s">
-        <v>899</v>
+        <v>901</v>
       </c>
       <c r="J3" t="s">
-        <v>900</v>
+        <v>902</v>
       </c>
       <c r="K3" t="s">
-        <v>901</v>
+        <v>903</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>846</v>
+        <v>848</v>
       </c>
       <c r="B4" t="s">
-        <v>847</v>
+        <v>849</v>
       </c>
       <c r="C4" t="s">
-        <v>848</v>
+        <v>850</v>
       </c>
       <c r="D4" t="s">
+        <v>851</v>
+      </c>
+      <c r="E4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F4" t="s">
+        <v>852</v>
+      </c>
+      <c r="G4" t="s">
+        <v>853</v>
+      </c>
+      <c r="H4" t="s">
+        <v>854</v>
+      </c>
+      <c r="I4" t="s">
         <v>849</v>
       </c>
-      <c r="E4" t="s">
-        <v>87</v>
-      </c>
-      <c r="F4" t="s">
-        <v>850</v>
-      </c>
-      <c r="G4" t="s">
-        <v>851</v>
-      </c>
-      <c r="H4" t="s">
-        <v>852</v>
-      </c>
-      <c r="I4" t="s">
-        <v>847</v>
-      </c>
       <c r="J4" t="s">
-        <v>853</v>
+        <v>855</v>
       </c>
       <c r="K4" t="s">
-        <v>902</v>
+        <v>904</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>855</v>
+        <v>857</v>
       </c>
       <c r="B5" t="s">
-        <v>856</v>
+        <v>858</v>
       </c>
       <c r="C5" t="s">
-        <v>857</v>
+        <v>859</v>
       </c>
       <c r="D5" t="s">
+        <v>860</v>
+      </c>
+      <c r="E5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F5" t="s">
+        <v>861</v>
+      </c>
+      <c r="G5" t="s">
+        <v>862</v>
+      </c>
+      <c r="H5" t="s">
+        <v>863</v>
+      </c>
+      <c r="I5" t="s">
         <v>858</v>
       </c>
-      <c r="E5" t="s">
-        <v>87</v>
-      </c>
-      <c r="F5" t="s">
-        <v>859</v>
-      </c>
-      <c r="G5" t="s">
-        <v>860</v>
-      </c>
-      <c r="H5" t="s">
-        <v>861</v>
-      </c>
-      <c r="I5" t="s">
-        <v>856</v>
-      </c>
       <c r="J5" t="s">
-        <v>862</v>
+        <v>864</v>
       </c>
       <c r="K5" t="s">
-        <v>903</v>
+        <v>905</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>864</v>
+        <v>866</v>
       </c>
       <c r="B6" t="s">
-        <v>865</v>
+        <v>867</v>
       </c>
       <c r="C6" t="s">
-        <v>866</v>
+        <v>868</v>
       </c>
       <c r="D6" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="E6" t="s">
         <v>87</v>
       </c>
       <c r="F6" t="s">
-        <v>868</v>
+        <v>870</v>
       </c>
       <c r="G6" t="s">
-        <v>869</v>
+        <v>871</v>
       </c>
       <c r="H6" t="s">
-        <v>904</v>
+        <v>906</v>
       </c>
       <c r="I6" t="s">
-        <v>871</v>
+        <v>873</v>
       </c>
       <c r="J6" t="s">
-        <v>872</v>
+        <v>874</v>
       </c>
       <c r="K6" t="s">
-        <v>873</v>
+        <v>875</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>874</v>
+        <v>876</v>
       </c>
       <c r="B7" t="s">
-        <v>875</v>
+        <v>877</v>
       </c>
       <c r="C7" t="s">
-        <v>876</v>
+        <v>878</v>
       </c>
       <c r="D7" t="s">
-        <v>877</v>
+        <v>879</v>
       </c>
       <c r="E7" t="s">
         <v>87</v>
       </c>
       <c r="F7" t="s">
-        <v>878</v>
+        <v>880</v>
       </c>
       <c r="G7" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
       <c r="H7" t="s">
-        <v>905</v>
+        <v>907</v>
       </c>
       <c r="I7" t="s">
-        <v>881</v>
+        <v>883</v>
       </c>
       <c r="J7" t="s">
-        <v>882</v>
+        <v>884</v>
       </c>
       <c r="K7" t="s">
-        <v>883</v>
+        <v>885</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" t="s">
-        <v>906</v>
+        <v>908</v>
       </c>
       <c r="B8" t="s">
-        <v>907</v>
+        <v>909</v>
       </c>
       <c r="C8" t="s">
-        <v>908</v>
+        <v>910</v>
       </c>
       <c r="D8" t="s">
-        <v>909</v>
+        <v>911</v>
       </c>
       <c r="E8" t="s">
         <v>87</v>
       </c>
       <c r="F8" t="s">
-        <v>910</v>
+        <v>912</v>
       </c>
       <c r="G8" t="s">
         <v>87</v>
       </c>
       <c r="H8" t="s">
-        <v>911</v>
+        <v>913</v>
       </c>
       <c r="I8" t="s">
         <v>87</v>
       </c>
       <c r="J8" t="s">
-        <v>912</v>
+        <v>914</v>
       </c>
       <c r="K8" t="s">
-        <v>913</v>
+        <v>915</v>
       </c>
     </row>
   </sheetData>
@@ -4082,34 +4088,34 @@
         <v>102</v>
       </c>
       <c r="B2" t="s">
-        <v>914</v>
+        <v>916</v>
       </c>
       <c r="C2" t="s">
-        <v>915</v>
+        <v>917</v>
       </c>
       <c r="D2" t="s">
-        <v>916</v>
+        <v>918</v>
       </c>
       <c r="E2" t="s">
         <v>87</v>
       </c>
       <c r="F2" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
       <c r="G2" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="H2" t="s">
-        <v>919</v>
+        <v>921</v>
       </c>
       <c r="I2" t="s">
-        <v>920</v>
+        <v>922</v>
       </c>
       <c r="J2" t="s">
-        <v>921</v>
+        <v>923</v>
       </c>
       <c r="K2" t="s">
-        <v>922</v>
+        <v>924</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -4117,314 +4123,314 @@
         <v>113</v>
       </c>
       <c r="B3" t="s">
-        <v>923</v>
+        <v>925</v>
       </c>
       <c r="C3" t="s">
-        <v>924</v>
+        <v>926</v>
       </c>
       <c r="D3" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="E3" t="s">
         <v>87</v>
       </c>
       <c r="F3" t="s">
-        <v>926</v>
+        <v>928</v>
       </c>
       <c r="G3" t="s">
         <v>87</v>
       </c>
       <c r="H3" t="s">
-        <v>927</v>
+        <v>929</v>
       </c>
       <c r="I3" t="s">
-        <v>928</v>
+        <v>930</v>
       </c>
       <c r="J3" t="s">
-        <v>929</v>
+        <v>931</v>
       </c>
       <c r="K3" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>931</v>
+        <v>933</v>
       </c>
       <c r="B4" t="s">
-        <v>932</v>
+        <v>934</v>
       </c>
       <c r="C4" t="s">
-        <v>933</v>
+        <v>935</v>
       </c>
       <c r="D4" t="s">
-        <v>934</v>
+        <v>936</v>
       </c>
       <c r="E4" t="s">
         <v>87</v>
       </c>
       <c r="F4" t="s">
-        <v>935</v>
+        <v>937</v>
       </c>
       <c r="G4" t="s">
         <v>87</v>
       </c>
       <c r="H4" t="s">
-        <v>936</v>
+        <v>938</v>
       </c>
       <c r="I4" t="s">
-        <v>937</v>
+        <v>939</v>
       </c>
       <c r="J4" t="s">
-        <v>938</v>
+        <v>940</v>
       </c>
       <c r="K4" t="s">
-        <v>939</v>
+        <v>941</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>940</v>
+        <v>942</v>
       </c>
       <c r="B5" t="s">
-        <v>941</v>
+        <v>943</v>
       </c>
       <c r="C5" t="s">
-        <v>942</v>
+        <v>944</v>
       </c>
       <c r="D5" t="s">
-        <v>943</v>
+        <v>945</v>
       </c>
       <c r="E5" t="s">
         <v>87</v>
       </c>
       <c r="F5" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
       <c r="G5" t="s">
-        <v>945</v>
+        <v>947</v>
       </c>
       <c r="H5" t="s">
-        <v>946</v>
+        <v>948</v>
       </c>
       <c r="I5" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="J5" t="s">
-        <v>948</v>
+        <v>950</v>
       </c>
       <c r="K5" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
       <c r="B6" t="s">
-        <v>951</v>
+        <v>953</v>
       </c>
       <c r="C6" t="s">
-        <v>952</v>
+        <v>954</v>
       </c>
       <c r="D6" t="s">
-        <v>953</v>
+        <v>955</v>
       </c>
       <c r="E6" t="s">
         <v>87</v>
       </c>
       <c r="F6" t="s">
-        <v>954</v>
+        <v>956</v>
       </c>
       <c r="G6" t="s">
         <v>87</v>
       </c>
       <c r="H6" t="s">
-        <v>955</v>
+        <v>957</v>
       </c>
       <c r="I6" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="J6" t="s">
-        <v>957</v>
+        <v>959</v>
       </c>
       <c r="K6" t="s">
-        <v>958</v>
+        <v>960</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>959</v>
+        <v>961</v>
       </c>
       <c r="B7" t="s">
-        <v>960</v>
+        <v>962</v>
       </c>
       <c r="C7" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="D7" t="s">
-        <v>962</v>
+        <v>964</v>
       </c>
       <c r="E7" t="s">
         <v>87</v>
       </c>
       <c r="F7" t="s">
-        <v>963</v>
+        <v>965</v>
       </c>
       <c r="G7" t="s">
         <v>87</v>
       </c>
       <c r="H7" t="s">
-        <v>964</v>
+        <v>966</v>
       </c>
       <c r="I7" t="s">
-        <v>965</v>
+        <v>967</v>
       </c>
       <c r="J7" t="s">
-        <v>966</v>
+        <v>968</v>
       </c>
       <c r="K7" t="s">
-        <v>967</v>
+        <v>969</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" t="s">
-        <v>968</v>
+        <v>970</v>
       </c>
       <c r="B8" t="s">
-        <v>969</v>
+        <v>971</v>
       </c>
       <c r="C8" t="s">
-        <v>970</v>
+        <v>972</v>
       </c>
       <c r="D8" t="s">
-        <v>971</v>
+        <v>973</v>
       </c>
       <c r="E8" t="s">
         <v>87</v>
       </c>
       <c r="F8" t="s">
-        <v>972</v>
+        <v>974</v>
       </c>
       <c r="G8" t="s">
         <v>87</v>
       </c>
       <c r="H8" t="s">
-        <v>973</v>
+        <v>975</v>
       </c>
       <c r="I8" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="J8" t="s">
-        <v>975</v>
+        <v>977</v>
       </c>
       <c r="K8" t="s">
-        <v>976</v>
+        <v>978</v>
       </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" t="s">
-        <v>977</v>
+        <v>979</v>
       </c>
       <c r="B9" t="s">
-        <v>978</v>
+        <v>980</v>
       </c>
       <c r="C9" t="s">
-        <v>979</v>
+        <v>981</v>
       </c>
       <c r="D9" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="E9" t="s">
         <v>87</v>
       </c>
       <c r="F9" t="s">
-        <v>981</v>
+        <v>983</v>
       </c>
       <c r="G9" t="s">
         <v>87</v>
       </c>
       <c r="H9" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
       <c r="I9" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="J9" t="s">
-        <v>984</v>
+        <v>986</v>
       </c>
       <c r="K9" t="s">
-        <v>985</v>
+        <v>987</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="B10" t="s">
-        <v>987</v>
+        <v>989</v>
       </c>
       <c r="C10" t="s">
-        <v>988</v>
+        <v>990</v>
       </c>
       <c r="D10" t="s">
-        <v>989</v>
+        <v>991</v>
       </c>
       <c r="E10" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="F10" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
       <c r="G10" t="s">
         <v>87</v>
       </c>
       <c r="H10" t="s">
-        <v>992</v>
+        <v>994</v>
       </c>
       <c r="I10" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="J10" t="s">
-        <v>994</v>
+        <v>996</v>
       </c>
       <c r="K10" t="s">
-        <v>995</v>
+        <v>997</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" t="s">
-        <v>996</v>
+        <v>998</v>
       </c>
       <c r="B11" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="C11" t="s">
-        <v>998</v>
+        <v>1000</v>
       </c>
       <c r="D11" t="s">
-        <v>999</v>
+        <v>1001</v>
       </c>
       <c r="E11" t="s">
         <v>87</v>
       </c>
       <c r="F11" t="s">
-        <v>1000</v>
+        <v>1002</v>
       </c>
       <c r="G11" t="s">
-        <v>1001</v>
+        <v>1003</v>
       </c>
       <c r="H11" t="s">
-        <v>1002</v>
+        <v>1004</v>
       </c>
       <c r="I11" t="s">
         <v>87</v>
       </c>
       <c r="J11" t="s">
-        <v>1003</v>
+        <v>1005</v>
       </c>
       <c r="K11" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
     </row>
   </sheetData>
@@ -7089,7 +7095,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -7347,172 +7353,180 @@
       <c r="B8" t="s">
         <v>711</v>
       </c>
-      <c r="C8" t="s">
-        <v>712</v>
-      </c>
-      <c r="D8" t="s">
-        <v>713</v>
-      </c>
-      <c r="E8" t="s">
-        <v>87</v>
-      </c>
-      <c r="F8" t="s">
-        <v>713</v>
-      </c>
-      <c r="G8" t="s">
-        <v>714</v>
-      </c>
-      <c r="H8" t="s">
-        <v>715</v>
-      </c>
-      <c r="I8" t="s">
-        <v>716</v>
-      </c>
-      <c r="J8" t="s">
-        <v>717</v>
-      </c>
-      <c r="K8" t="s">
-        <v>718</v>
-      </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" t="s">
+        <v>712</v>
+      </c>
+      <c r="B9" t="s">
+        <v>713</v>
+      </c>
+      <c r="C9" t="s">
+        <v>714</v>
+      </c>
+      <c r="D9" t="s">
+        <v>715</v>
+      </c>
+      <c r="E9" t="s">
+        <v>87</v>
+      </c>
+      <c r="F9" t="s">
+        <v>715</v>
+      </c>
+      <c r="G9" t="s">
+        <v>716</v>
+      </c>
+      <c r="H9" t="s">
+        <v>717</v>
+      </c>
+      <c r="I9" t="s">
+        <v>718</v>
+      </c>
+      <c r="J9" t="s">
         <v>719</v>
       </c>
-      <c r="B9" t="s">
+      <c r="K9" t="s">
         <v>720</v>
-      </c>
-      <c r="C9" t="s">
-        <v>721</v>
-      </c>
-      <c r="D9" t="s">
-        <v>722</v>
-      </c>
-      <c r="E9" t="s">
-        <v>87</v>
-      </c>
-      <c r="F9" t="s">
-        <v>722</v>
-      </c>
-      <c r="G9" t="s">
-        <v>723</v>
-      </c>
-      <c r="H9" t="s">
-        <v>724</v>
-      </c>
-      <c r="I9" t="s">
-        <v>725</v>
-      </c>
-      <c r="J9" t="s">
-        <v>726</v>
-      </c>
-      <c r="K9" t="s">
-        <v>727</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" t="s">
+        <v>721</v>
+      </c>
+      <c r="B10" t="s">
+        <v>722</v>
+      </c>
+      <c r="C10" t="s">
+        <v>723</v>
+      </c>
+      <c r="D10" t="s">
+        <v>724</v>
+      </c>
+      <c r="E10" t="s">
+        <v>87</v>
+      </c>
+      <c r="F10" t="s">
+        <v>724</v>
+      </c>
+      <c r="G10" t="s">
+        <v>725</v>
+      </c>
+      <c r="H10" t="s">
+        <v>726</v>
+      </c>
+      <c r="I10" t="s">
+        <v>727</v>
+      </c>
+      <c r="J10" t="s">
         <v>728</v>
       </c>
-      <c r="B10" t="s">
+      <c r="K10" t="s">
         <v>729</v>
-      </c>
-      <c r="C10" t="s">
-        <v>730</v>
-      </c>
-      <c r="D10" t="s">
-        <v>87</v>
-      </c>
-      <c r="E10" t="s">
-        <v>87</v>
-      </c>
-      <c r="F10" t="s">
-        <v>731</v>
-      </c>
-      <c r="G10" t="s">
-        <v>87</v>
-      </c>
-      <c r="H10" t="s">
-        <v>87</v>
-      </c>
-      <c r="I10" t="s">
-        <v>87</v>
-      </c>
-      <c r="J10" t="s">
-        <v>732</v>
-      </c>
-      <c r="K10" t="s">
-        <v>733</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" t="s">
+        <v>730</v>
+      </c>
+      <c r="B11" t="s">
+        <v>731</v>
+      </c>
+      <c r="C11" t="s">
+        <v>732</v>
+      </c>
+      <c r="D11" t="s">
+        <v>87</v>
+      </c>
+      <c r="E11" t="s">
+        <v>87</v>
+      </c>
+      <c r="F11" t="s">
+        <v>733</v>
+      </c>
+      <c r="G11" t="s">
+        <v>87</v>
+      </c>
+      <c r="H11" t="s">
+        <v>87</v>
+      </c>
+      <c r="I11" t="s">
+        <v>87</v>
+      </c>
+      <c r="J11" t="s">
         <v>734</v>
       </c>
-      <c r="B11" t="s">
+      <c r="K11" t="s">
         <v>735</v>
-      </c>
-      <c r="C11" t="s">
-        <v>736</v>
-      </c>
-      <c r="D11" t="s">
-        <v>87</v>
-      </c>
-      <c r="E11" t="s">
-        <v>87</v>
-      </c>
-      <c r="F11" t="s">
-        <v>737</v>
-      </c>
-      <c r="G11" t="s">
-        <v>87</v>
-      </c>
-      <c r="H11" t="s">
-        <v>87</v>
-      </c>
-      <c r="I11" t="s">
-        <v>87</v>
-      </c>
-      <c r="J11" t="s">
-        <v>738</v>
-      </c>
-      <c r="K11" t="s">
-        <v>739</v>
       </c>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" t="s">
+        <v>736</v>
+      </c>
+      <c r="B12" t="s">
+        <v>737</v>
+      </c>
+      <c r="C12" t="s">
+        <v>738</v>
+      </c>
+      <c r="D12" t="s">
+        <v>87</v>
+      </c>
+      <c r="E12" t="s">
+        <v>87</v>
+      </c>
+      <c r="F12" t="s">
+        <v>739</v>
+      </c>
+      <c r="G12" t="s">
+        <v>87</v>
+      </c>
+      <c r="H12" t="s">
+        <v>87</v>
+      </c>
+      <c r="I12" t="s">
+        <v>87</v>
+      </c>
+      <c r="J12" t="s">
         <v>740</v>
       </c>
-      <c r="B12" t="s">
+      <c r="K12" t="s">
         <v>741</v>
       </c>
-      <c r="C12" t="s">
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" t="s">
         <v>742</v>
       </c>
-      <c r="D12" t="s">
-        <v>87</v>
-      </c>
-      <c r="E12" t="s">
-        <v>87</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="B13" t="s">
         <v>743</v>
       </c>
-      <c r="G12" t="s">
-        <v>87</v>
-      </c>
-      <c r="H12" t="s">
-        <v>87</v>
-      </c>
-      <c r="I12" t="s">
-        <v>87</v>
-      </c>
-      <c r="J12" t="s">
+      <c r="C13" t="s">
         <v>744</v>
       </c>
-      <c r="K12" t="s">
+      <c r="D13" t="s">
+        <v>87</v>
+      </c>
+      <c r="E13" t="s">
+        <v>87</v>
+      </c>
+      <c r="F13" t="s">
         <v>745</v>
+      </c>
+      <c r="G13" t="s">
+        <v>87</v>
+      </c>
+      <c r="H13" t="s">
+        <v>87</v>
+      </c>
+      <c r="I13" t="s">
+        <v>87</v>
+      </c>
+      <c r="J13" t="s">
+        <v>746</v>
+      </c>
+      <c r="K13" t="s">
+        <v>747</v>
       </c>
     </row>
   </sheetData>
@@ -7571,31 +7585,31 @@
         <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>746</v>
+        <v>748</v>
       </c>
       <c r="D2" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
       <c r="E2" t="s">
         <v>87</v>
       </c>
       <c r="F2" t="s">
-        <v>748</v>
+        <v>750</v>
       </c>
       <c r="G2" t="s">
-        <v>749</v>
+        <v>751</v>
       </c>
       <c r="H2" t="s">
-        <v>750</v>
+        <v>752</v>
       </c>
       <c r="I2" t="s">
-        <v>751</v>
+        <v>753</v>
       </c>
       <c r="J2" t="s">
-        <v>752</v>
+        <v>754</v>
       </c>
       <c r="K2" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -7603,279 +7617,279 @@
         <v>113</v>
       </c>
       <c r="B3" t="s">
-        <v>754</v>
+        <v>756</v>
       </c>
       <c r="C3" t="s">
-        <v>755</v>
+        <v>757</v>
       </c>
       <c r="D3" t="s">
-        <v>756</v>
+        <v>758</v>
       </c>
       <c r="E3" t="s">
         <v>87</v>
       </c>
       <c r="F3" t="s">
-        <v>757</v>
+        <v>759</v>
       </c>
       <c r="G3" t="s">
-        <v>758</v>
+        <v>760</v>
       </c>
       <c r="H3" t="s">
-        <v>759</v>
+        <v>761</v>
       </c>
       <c r="I3" t="s">
-        <v>760</v>
+        <v>762</v>
       </c>
       <c r="J3" t="s">
-        <v>761</v>
+        <v>763</v>
       </c>
       <c r="K3" t="s">
-        <v>762</v>
+        <v>764</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>763</v>
+        <v>765</v>
       </c>
       <c r="B4" t="s">
-        <v>764</v>
+        <v>766</v>
       </c>
       <c r="C4" t="s">
-        <v>765</v>
+        <v>767</v>
       </c>
       <c r="D4" t="s">
-        <v>766</v>
+        <v>768</v>
       </c>
       <c r="E4" t="s">
         <v>87</v>
       </c>
       <c r="F4" t="s">
-        <v>767</v>
+        <v>769</v>
       </c>
       <c r="G4" t="s">
-        <v>768</v>
+        <v>770</v>
       </c>
       <c r="H4" t="s">
-        <v>769</v>
+        <v>771</v>
       </c>
       <c r="I4" t="s">
-        <v>770</v>
+        <v>772</v>
       </c>
       <c r="J4" t="s">
-        <v>771</v>
+        <v>773</v>
       </c>
       <c r="K4" t="s">
-        <v>772</v>
+        <v>774</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>773</v>
+        <v>775</v>
       </c>
       <c r="B5" t="s">
-        <v>774</v>
+        <v>776</v>
       </c>
       <c r="C5" t="s">
-        <v>775</v>
+        <v>777</v>
       </c>
       <c r="D5" t="s">
-        <v>776</v>
+        <v>778</v>
       </c>
       <c r="E5" t="s">
         <v>87</v>
       </c>
       <c r="F5" t="s">
-        <v>777</v>
+        <v>779</v>
       </c>
       <c r="G5" t="s">
-        <v>778</v>
+        <v>780</v>
       </c>
       <c r="H5" t="s">
-        <v>779</v>
+        <v>781</v>
       </c>
       <c r="I5" t="s">
-        <v>780</v>
+        <v>782</v>
       </c>
       <c r="J5" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
       <c r="K5" t="s">
-        <v>782</v>
+        <v>784</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="B6" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="C6" t="s">
-        <v>785</v>
+        <v>787</v>
       </c>
       <c r="D6" t="s">
-        <v>786</v>
+        <v>788</v>
       </c>
       <c r="E6" t="s">
         <v>87</v>
       </c>
       <c r="F6" t="s">
-        <v>787</v>
+        <v>789</v>
       </c>
       <c r="G6" t="s">
-        <v>788</v>
+        <v>790</v>
       </c>
       <c r="H6" t="s">
-        <v>789</v>
+        <v>791</v>
       </c>
       <c r="I6" t="s">
-        <v>790</v>
+        <v>792</v>
       </c>
       <c r="J6" t="s">
-        <v>791</v>
+        <v>793</v>
       </c>
       <c r="K6" t="s">
-        <v>792</v>
+        <v>794</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>793</v>
+        <v>795</v>
       </c>
       <c r="B7" t="s">
-        <v>794</v>
+        <v>796</v>
       </c>
       <c r="C7" t="s">
-        <v>795</v>
+        <v>797</v>
       </c>
       <c r="D7" t="s">
+        <v>798</v>
+      </c>
+      <c r="E7" t="s">
+        <v>87</v>
+      </c>
+      <c r="F7" t="s">
         <v>796</v>
       </c>
-      <c r="E7" t="s">
-        <v>87</v>
-      </c>
-      <c r="F7" t="s">
-        <v>794</v>
-      </c>
       <c r="G7" t="s">
-        <v>797</v>
+        <v>799</v>
       </c>
       <c r="H7" t="s">
-        <v>798</v>
+        <v>800</v>
       </c>
       <c r="I7" t="s">
-        <v>799</v>
+        <v>801</v>
       </c>
       <c r="J7" t="s">
-        <v>800</v>
+        <v>802</v>
       </c>
       <c r="K7" t="s">
-        <v>801</v>
+        <v>803</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" t="s">
-        <v>802</v>
+        <v>804</v>
       </c>
       <c r="B8" t="s">
-        <v>803</v>
+        <v>805</v>
       </c>
       <c r="C8" t="s">
-        <v>804</v>
+        <v>806</v>
       </c>
       <c r="D8" t="s">
-        <v>805</v>
+        <v>807</v>
       </c>
       <c r="E8" t="s">
         <v>87</v>
       </c>
       <c r="F8" t="s">
-        <v>806</v>
+        <v>808</v>
       </c>
       <c r="G8" t="s">
         <v>87</v>
       </c>
       <c r="H8" t="s">
-        <v>807</v>
+        <v>809</v>
       </c>
       <c r="I8" t="s">
-        <v>808</v>
+        <v>810</v>
       </c>
       <c r="J8" t="s">
-        <v>809</v>
+        <v>811</v>
       </c>
       <c r="K8" t="s">
-        <v>810</v>
+        <v>812</v>
       </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" t="s">
-        <v>811</v>
+        <v>813</v>
       </c>
       <c r="B9" t="s">
-        <v>812</v>
+        <v>814</v>
       </c>
       <c r="C9" t="s">
-        <v>813</v>
+        <v>815</v>
       </c>
       <c r="D9" t="s">
-        <v>814</v>
+        <v>816</v>
       </c>
       <c r="E9" t="s">
         <v>87</v>
       </c>
       <c r="F9" t="s">
-        <v>815</v>
+        <v>817</v>
       </c>
       <c r="G9" t="s">
         <v>87</v>
       </c>
       <c r="H9" t="s">
-        <v>816</v>
+        <v>818</v>
       </c>
       <c r="I9" t="s">
-        <v>817</v>
+        <v>819</v>
       </c>
       <c r="J9" t="s">
-        <v>818</v>
+        <v>820</v>
       </c>
       <c r="K9" t="s">
-        <v>819</v>
+        <v>821</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" t="s">
-        <v>820</v>
+        <v>822</v>
       </c>
       <c r="B10" t="s">
-        <v>821</v>
+        <v>823</v>
       </c>
       <c r="C10" t="s">
-        <v>822</v>
+        <v>824</v>
       </c>
       <c r="D10" t="s">
-        <v>823</v>
+        <v>825</v>
       </c>
       <c r="E10" t="s">
         <v>87</v>
       </c>
       <c r="F10" t="s">
-        <v>824</v>
+        <v>826</v>
       </c>
       <c r="G10" t="s">
         <v>87</v>
       </c>
       <c r="H10" t="s">
-        <v>825</v>
+        <v>827</v>
       </c>
       <c r="I10" t="s">
         <v>87</v>
       </c>
       <c r="J10" t="s">
-        <v>826</v>
+        <v>828</v>
       </c>
       <c r="K10" t="s">
-        <v>827</v>
+        <v>829</v>
       </c>
     </row>
   </sheetData>
@@ -7931,34 +7945,34 @@
         <v>102</v>
       </c>
       <c r="B2" t="s">
-        <v>828</v>
+        <v>830</v>
       </c>
       <c r="C2" t="s">
-        <v>829</v>
+        <v>831</v>
       </c>
       <c r="D2" t="s">
-        <v>830</v>
+        <v>832</v>
       </c>
       <c r="E2" t="s">
         <v>87</v>
       </c>
       <c r="F2" t="s">
-        <v>831</v>
+        <v>833</v>
       </c>
       <c r="G2" t="s">
-        <v>832</v>
+        <v>834</v>
       </c>
       <c r="H2" t="s">
-        <v>833</v>
+        <v>835</v>
       </c>
       <c r="I2" t="s">
-        <v>834</v>
+        <v>836</v>
       </c>
       <c r="J2" t="s">
-        <v>835</v>
+        <v>837</v>
       </c>
       <c r="K2" t="s">
-        <v>836</v>
+        <v>838</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -7966,174 +7980,174 @@
         <v>113</v>
       </c>
       <c r="B3" t="s">
-        <v>837</v>
+        <v>839</v>
       </c>
       <c r="C3" t="s">
-        <v>838</v>
+        <v>840</v>
       </c>
       <c r="D3" t="s">
-        <v>839</v>
+        <v>841</v>
       </c>
       <c r="E3" t="s">
         <v>87</v>
       </c>
       <c r="F3" t="s">
-        <v>840</v>
+        <v>842</v>
       </c>
       <c r="G3" t="s">
-        <v>841</v>
+        <v>843</v>
       </c>
       <c r="H3" t="s">
-        <v>842</v>
+        <v>844</v>
       </c>
       <c r="I3" t="s">
-        <v>843</v>
+        <v>845</v>
       </c>
       <c r="J3" t="s">
-        <v>844</v>
+        <v>846</v>
       </c>
       <c r="K3" t="s">
-        <v>845</v>
+        <v>847</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>846</v>
+        <v>848</v>
       </c>
       <c r="B4" t="s">
-        <v>847</v>
+        <v>849</v>
       </c>
       <c r="C4" t="s">
-        <v>848</v>
+        <v>850</v>
       </c>
       <c r="D4" t="s">
+        <v>851</v>
+      </c>
+      <c r="E4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F4" t="s">
+        <v>852</v>
+      </c>
+      <c r="G4" t="s">
+        <v>853</v>
+      </c>
+      <c r="H4" t="s">
+        <v>854</v>
+      </c>
+      <c r="I4" t="s">
         <v>849</v>
       </c>
-      <c r="E4" t="s">
-        <v>87</v>
-      </c>
-      <c r="F4" t="s">
-        <v>850</v>
-      </c>
-      <c r="G4" t="s">
-        <v>851</v>
-      </c>
-      <c r="H4" t="s">
-        <v>852</v>
-      </c>
-      <c r="I4" t="s">
-        <v>847</v>
-      </c>
       <c r="J4" t="s">
-        <v>853</v>
+        <v>855</v>
       </c>
       <c r="K4" t="s">
-        <v>854</v>
+        <v>856</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>855</v>
+        <v>857</v>
       </c>
       <c r="B5" t="s">
-        <v>856</v>
+        <v>858</v>
       </c>
       <c r="C5" t="s">
-        <v>857</v>
+        <v>859</v>
       </c>
       <c r="D5" t="s">
+        <v>860</v>
+      </c>
+      <c r="E5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F5" t="s">
+        <v>861</v>
+      </c>
+      <c r="G5" t="s">
+        <v>862</v>
+      </c>
+      <c r="H5" t="s">
+        <v>863</v>
+      </c>
+      <c r="I5" t="s">
         <v>858</v>
       </c>
-      <c r="E5" t="s">
-        <v>87</v>
-      </c>
-      <c r="F5" t="s">
-        <v>859</v>
-      </c>
-      <c r="G5" t="s">
-        <v>860</v>
-      </c>
-      <c r="H5" t="s">
-        <v>861</v>
-      </c>
-      <c r="I5" t="s">
-        <v>856</v>
-      </c>
       <c r="J5" t="s">
-        <v>862</v>
+        <v>864</v>
       </c>
       <c r="K5" t="s">
-        <v>863</v>
+        <v>865</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>864</v>
+        <v>866</v>
       </c>
       <c r="B6" t="s">
-        <v>865</v>
+        <v>867</v>
       </c>
       <c r="C6" t="s">
-        <v>866</v>
+        <v>868</v>
       </c>
       <c r="D6" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="E6" t="s">
         <v>87</v>
       </c>
       <c r="F6" t="s">
-        <v>868</v>
+        <v>870</v>
       </c>
       <c r="G6" t="s">
-        <v>869</v>
+        <v>871</v>
       </c>
       <c r="H6" t="s">
-        <v>870</v>
+        <v>872</v>
       </c>
       <c r="I6" t="s">
-        <v>871</v>
+        <v>873</v>
       </c>
       <c r="J6" t="s">
-        <v>872</v>
+        <v>874</v>
       </c>
       <c r="K6" t="s">
-        <v>873</v>
+        <v>875</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>874</v>
+        <v>876</v>
       </c>
       <c r="B7" t="s">
-        <v>875</v>
+        <v>877</v>
       </c>
       <c r="C7" t="s">
-        <v>876</v>
+        <v>878</v>
       </c>
       <c r="D7" t="s">
-        <v>877</v>
+        <v>879</v>
       </c>
       <c r="E7" t="s">
         <v>87</v>
       </c>
       <c r="F7" t="s">
-        <v>878</v>
+        <v>880</v>
       </c>
       <c r="G7" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
       <c r="H7" t="s">
-        <v>880</v>
+        <v>882</v>
       </c>
       <c r="I7" t="s">
-        <v>881</v>
+        <v>883</v>
       </c>
       <c r="J7" t="s">
-        <v>882</v>
+        <v>884</v>
       </c>
       <c r="K7" t="s">
-        <v>883</v>
+        <v>885</v>
       </c>
     </row>
   </sheetData>

</xml_diff>